<commit_message>
Actualización en carpetas del repositorio
</commit_message>
<xml_diff>
--- a/Organización/Procesos/Soporte Organizacional/2. Administración de Configuración/IWM_Administración de la Configuración.xlsx
+++ b/Organización/Procesos/Soporte Organizacional/2. Administración de Configuración/IWM_Administración de la Configuración.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gus\Dropbox\Repositorio\Organización\Procesos\Soporte Organizacional\2. Administración de Configuración\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gus\Desktop\GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="30" yWindow="15" windowWidth="6720" windowHeight="8655" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="30" yWindow="15" windowWidth="6720" windowHeight="7740" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Plan CMbkps" sheetId="1" state="hidden" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="349">
   <si>
     <t>Adapiaciones al Estándar de Administración de Datos</t>
   </si>
@@ -1472,9 +1472,6 @@
     </r>
   </si>
   <si>
-    <t>IWM_Plan_Mejora_año</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">    </t>
     </r>
@@ -1609,9 +1606,6 @@
     <t>IWM_&lt;C/R&gt;_aammdd</t>
   </si>
   <si>
-    <t>&lt;proyecto&gt;_Matriaz_Riesgos.xlsx</t>
-  </si>
-  <si>
     <t>&lt;proyecto&gt;_Toma_Decision</t>
   </si>
   <si>
@@ -1621,10 +1615,84 @@
     <t>IWM_LeccionesAprendidas</t>
   </si>
   <si>
-    <t>Guías de Adaptación</t>
-  </si>
-  <si>
-    <t>IWM_GuiaAdaptacion</t>
+    <t>&lt;proyecto&gt;_Evaluacion_Proveedores</t>
+  </si>
+  <si>
+    <t>Guías de Revición por pares</t>
+  </si>
+  <si>
+    <t>IWM_Guia_Revición_por_pares</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="9"/>
+        <rFont val="Wingdings"/>
+        <charset val="2"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Solicitudes</t>
+    </r>
+  </si>
+  <si>
+    <t>Solicitud Mejora</t>
+  </si>
+  <si>
+    <t>Solicitud_Mejora_mm_aaaa</t>
+  </si>
+  <si>
+    <t>IWM_Plan_Mejora_aaaa</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="9"/>
+        <rFont val="Wingdings"/>
+        <charset val="2"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Reporte de Actividades</t>
+    </r>
+  </si>
+  <si>
+    <t>Reporte de Actividades</t>
+  </si>
+  <si>
+    <t>Reporte_Actividades_aaaa</t>
+  </si>
+  <si>
+    <t>Concentrado de Mejoras</t>
+  </si>
+  <si>
+    <t>Concentrado_Mejoras</t>
+  </si>
+  <si>
+    <t>Solicitud de mejora</t>
+  </si>
+  <si>
+    <t>PTLL_Solicitud_Mejora</t>
   </si>
 </sst>
 </file>
@@ -4591,10 +4659,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:E63"/>
+  <dimension ref="A3:E62"/>
   <sheetViews>
     <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -4739,95 +4807,94 @@
       <c r="D14" s="76"/>
     </row>
     <row r="15" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="103" t="s">
+      <c r="A15" s="77" t="s">
+        <v>136</v>
+      </c>
+      <c r="B15" s="70" t="s">
+        <v>335</v>
+      </c>
+      <c r="C15" s="70"/>
+    </row>
+    <row r="16" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="103" t="s">
         <v>218</v>
       </c>
-      <c r="B15" s="104" t="s">
+      <c r="B16" s="104" t="s">
         <v>226</v>
-      </c>
-      <c r="C15" s="70"/>
-      <c r="D15" s="70"/>
-    </row>
-    <row r="16" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="77" t="s">
-        <v>78</v>
-      </c>
-      <c r="B16" s="70" t="s">
-        <v>125</v>
       </c>
       <c r="C16" s="70"/>
       <c r="D16" s="70"/>
     </row>
     <row r="17" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A17" s="77" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="B17" s="70" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C17" s="70"/>
-      <c r="D17" s="70" t="s">
-        <v>159</v>
-      </c>
+      <c r="D17" s="70"/>
     </row>
     <row r="18" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A18" s="77" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18" s="70" t="s">
+        <v>126</v>
+      </c>
+      <c r="C18" s="70"/>
+      <c r="D18" s="70" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="77" t="s">
         <v>106</v>
       </c>
-      <c r="B18" s="70" t="s">
+      <c r="B19" s="70" t="s">
         <v>127</v>
       </c>
-      <c r="C18" s="70" t="s">
+      <c r="C19" s="70" t="s">
         <v>159</v>
       </c>
-      <c r="D18" s="70"/>
-    </row>
-    <row r="19" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="75" t="s">
+      <c r="D19" s="70"/>
+    </row>
+    <row r="20" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="75" t="s">
         <v>149</v>
       </c>
-      <c r="B19" s="76"/>
-      <c r="C19" s="76"/>
-      <c r="D19" s="76"/>
-    </row>
-    <row r="20" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="77" t="s">
-        <v>104</v>
-      </c>
-      <c r="B20" s="78" t="s">
-        <v>228</v>
-      </c>
-      <c r="C20" s="70"/>
-      <c r="D20" s="70"/>
+      <c r="B20" s="76"/>
+      <c r="C20" s="76"/>
+      <c r="D20" s="76"/>
     </row>
     <row r="21" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A21" s="77" t="s">
-        <v>164</v>
+        <v>104</v>
       </c>
       <c r="B21" s="78" t="s">
-        <v>229</v>
-      </c>
-      <c r="C21" s="70" t="s">
-        <v>159</v>
-      </c>
+        <v>228</v>
+      </c>
+      <c r="C21" s="70"/>
       <c r="D21" s="70"/>
     </row>
     <row r="22" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A22" s="77" t="s">
-        <v>142</v>
-      </c>
-      <c r="B22" s="70" t="s">
-        <v>165</v>
-      </c>
-      <c r="C22" s="70"/>
+        <v>164</v>
+      </c>
+      <c r="B22" s="78" t="s">
+        <v>229</v>
+      </c>
+      <c r="C22" s="70" t="s">
+        <v>159</v>
+      </c>
       <c r="D22" s="70"/>
     </row>
     <row r="23" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A23" s="77" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B23" s="70" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C23" s="70"/>
       <c r="D23" s="70"/>
@@ -4837,73 +4904,73 @@
         <v>143</v>
       </c>
       <c r="B24" s="70" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C24" s="70"/>
       <c r="D24" s="70"/>
     </row>
     <row r="25" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A25" s="77" t="s">
-        <v>224</v>
+        <v>143</v>
       </c>
       <c r="B25" s="70" t="s">
-        <v>225</v>
+        <v>167</v>
       </c>
       <c r="C25" s="70"/>
       <c r="D25" s="70"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="95" t="s">
+      <c r="A26" s="77" t="s">
+        <v>224</v>
+      </c>
+      <c r="B26" s="70" t="s">
+        <v>225</v>
+      </c>
+      <c r="C26" s="70"/>
+      <c r="D26" s="70"/>
+    </row>
+    <row r="27" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="95" t="s">
         <v>145</v>
       </c>
-      <c r="B26" s="96"/>
-      <c r="C26" s="96"/>
-      <c r="D26" s="96"/>
-    </row>
-    <row r="27" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="81" t="s">
+      <c r="B27" s="96"/>
+      <c r="C27" s="96"/>
+      <c r="D27" s="96"/>
+    </row>
+    <row r="28" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="81" t="s">
         <v>146</v>
       </c>
-      <c r="B27" s="81"/>
-      <c r="C27" s="81"/>
-      <c r="D27" s="81"/>
-    </row>
-    <row r="28" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="77" t="s">
+      <c r="B28" s="81"/>
+      <c r="C28" s="81"/>
+      <c r="D28" s="81"/>
+    </row>
+    <row r="29" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="77" t="s">
         <v>103</v>
       </c>
-      <c r="B28" s="83" t="s">
+      <c r="B29" s="83" t="s">
         <v>169</v>
       </c>
-      <c r="C28" s="70" t="s">
+      <c r="C29" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="D28" s="70"/>
-    </row>
-    <row r="29" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="81" t="s">
+      <c r="D29" s="70"/>
+    </row>
+    <row r="30" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="81" t="s">
         <v>147</v>
       </c>
-      <c r="B29" s="81"/>
-      <c r="C29" s="81"/>
-      <c r="D29" s="81"/>
-    </row>
-    <row r="30" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="77" t="s">
-        <v>178</v>
-      </c>
-      <c r="B30" s="105" t="s">
-        <v>179</v>
-      </c>
-      <c r="C30" s="105"/>
-      <c r="D30" s="105"/>
+      <c r="B30" s="81"/>
+      <c r="C30" s="81"/>
+      <c r="D30" s="81"/>
     </row>
     <row r="31" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A31" s="77" t="s">
         <v>178</v>
       </c>
       <c r="B31" s="105" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C31" s="105"/>
       <c r="D31" s="105"/>
@@ -4913,119 +4980,115 @@
         <v>178</v>
       </c>
       <c r="B32" s="105" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C32" s="105"/>
       <c r="D32" s="105"/>
     </row>
     <row r="33" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A33" s="77" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B33" s="105" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C33" s="105"/>
       <c r="D33" s="105"/>
     </row>
     <row r="34" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A34" s="77" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B34" s="105" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C34" s="105"/>
       <c r="D34" s="105"/>
     </row>
     <row r="35" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A35" s="77" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B35" s="105" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C35" s="105"/>
       <c r="D35" s="105"/>
     </row>
     <row r="36" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="84" t="s">
+      <c r="A36" s="77" t="s">
+        <v>186</v>
+      </c>
+      <c r="B36" s="105" t="s">
+        <v>187</v>
+      </c>
+      <c r="C36" s="105"/>
+      <c r="D36" s="105"/>
+    </row>
+    <row r="37" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="84" t="s">
         <v>188</v>
       </c>
-      <c r="B36" s="85" t="s">
+      <c r="B37" s="85" t="s">
         <v>189</v>
       </c>
-      <c r="C36" s="70"/>
-      <c r="D36" s="70"/>
-    </row>
-    <row r="37" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="81" t="s">
+      <c r="C37" s="70"/>
+      <c r="D37" s="70"/>
+    </row>
+    <row r="38" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="81" t="s">
         <v>162</v>
       </c>
-      <c r="B37" s="81"/>
-      <c r="C37" s="81"/>
-      <c r="D37" s="81"/>
-    </row>
-    <row r="38" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="84" t="s">
-        <v>214</v>
-      </c>
-      <c r="B38" s="86" t="s">
-        <v>212</v>
-      </c>
-      <c r="C38" s="70"/>
-      <c r="D38" s="70"/>
+      <c r="B38" s="81"/>
+      <c r="C38" s="81"/>
+      <c r="D38" s="81"/>
     </row>
     <row r="39" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A39" s="84" t="s">
-        <v>170</v>
-      </c>
-      <c r="B39" s="85" t="s">
-        <v>213</v>
-      </c>
-      <c r="C39" s="70" t="s">
-        <v>77</v>
-      </c>
+        <v>214</v>
+      </c>
+      <c r="B39" s="86" t="s">
+        <v>212</v>
+      </c>
+      <c r="C39" s="70"/>
       <c r="D39" s="70"/>
     </row>
     <row r="40" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A40" s="84" t="s">
+        <v>170</v>
+      </c>
+      <c r="B40" s="85" t="s">
+        <v>213</v>
+      </c>
+      <c r="C40" s="70" t="s">
+        <v>77</v>
+      </c>
+      <c r="D40" s="70"/>
+    </row>
+    <row r="41" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="84" t="s">
         <v>45</v>
       </c>
-      <c r="B40" s="85" t="s">
+      <c r="B41" s="85" t="s">
         <v>215</v>
       </c>
-      <c r="C40" s="70"/>
-      <c r="D40" s="70"/>
-    </row>
-    <row r="41" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="81" t="s">
+      <c r="C41" s="70"/>
+      <c r="D41" s="70"/>
+    </row>
+    <row r="42" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="81" t="s">
         <v>168</v>
       </c>
-      <c r="B41" s="81"/>
-      <c r="C41" s="81"/>
-      <c r="D41" s="81"/>
-    </row>
-    <row r="42" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="84" t="s">
-        <v>85</v>
-      </c>
-      <c r="B42" s="86" t="s">
-        <v>128</v>
-      </c>
-      <c r="C42" s="70" t="s">
-        <v>77</v>
-      </c>
-      <c r="D42" s="70" t="s">
-        <v>159</v>
-      </c>
+      <c r="B42" s="81"/>
+      <c r="C42" s="81"/>
+      <c r="D42" s="81"/>
     </row>
     <row r="43" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A43" s="84" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B43" s="86" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C43" s="70" t="s">
         <v>77</v>
@@ -5035,215 +5098,210 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="95" t="s">
+      <c r="A44" s="84" t="s">
+        <v>84</v>
+      </c>
+      <c r="B44" s="86" t="s">
+        <v>129</v>
+      </c>
+      <c r="C44" s="70" t="s">
+        <v>77</v>
+      </c>
+      <c r="D44" s="70" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="95" t="s">
         <v>150</v>
       </c>
-      <c r="B44" s="96"/>
-      <c r="C44" s="96"/>
-      <c r="D44" s="96"/>
-    </row>
-    <row r="45" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="88" t="s">
-        <v>86</v>
-      </c>
-      <c r="B45" s="99" t="s">
-        <v>171</v>
-      </c>
-      <c r="C45" s="99" t="s">
-        <v>159</v>
-      </c>
-      <c r="D45" s="70" t="s">
-        <v>159</v>
-      </c>
+      <c r="B45" s="96"/>
+      <c r="C45" s="96"/>
+      <c r="D45" s="96"/>
     </row>
     <row r="46" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A46" s="88" t="s">
         <v>86</v>
       </c>
       <c r="B46" s="99" t="s">
+        <v>171</v>
+      </c>
+      <c r="C46" s="99" t="s">
+        <v>159</v>
+      </c>
+      <c r="D46" s="70" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="88" t="s">
+        <v>86</v>
+      </c>
+      <c r="B47" s="99" t="s">
         <v>227</v>
       </c>
-      <c r="C46" s="99"/>
-      <c r="D46" s="70"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="95" t="s">
+      <c r="C47" s="99"/>
+      <c r="D47" s="70"/>
+    </row>
+    <row r="48" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="95" t="s">
         <v>151</v>
       </c>
-      <c r="B47" s="96"/>
-      <c r="C47" s="96"/>
-      <c r="D47" s="96"/>
-    </row>
-    <row r="48" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="88" t="s">
-        <v>153</v>
-      </c>
-      <c r="B48" s="99" t="s">
-        <v>173</v>
-      </c>
-      <c r="C48" s="56"/>
-      <c r="D48" s="56"/>
+      <c r="B48" s="96"/>
+      <c r="C48" s="96"/>
+      <c r="D48" s="96"/>
     </row>
     <row r="49" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A49" s="88" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B49" s="99" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C49" s="56"/>
       <c r="D49" s="56"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" s="95" t="s">
+      <c r="A50" s="88" t="s">
+        <v>154</v>
+      </c>
+      <c r="B50" s="99" t="s">
+        <v>172</v>
+      </c>
+      <c r="C50" s="56"/>
+      <c r="D50" s="56"/>
+    </row>
+    <row r="51" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="95" t="s">
         <v>156</v>
       </c>
-      <c r="B50" s="96"/>
-      <c r="C50" s="96"/>
-      <c r="D50" s="96"/>
-    </row>
-    <row r="51" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="107" t="s">
+      <c r="B51" s="96"/>
+      <c r="C51" s="96"/>
+      <c r="D51" s="96"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" s="107" t="s">
         <v>190</v>
       </c>
-      <c r="B51" s="56" t="s">
+      <c r="B52" s="56" t="s">
         <v>163</v>
       </c>
-      <c r="C51" s="56"/>
-      <c r="D51" s="56"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52" s="88" t="s">
+      <c r="C52" s="56"/>
+      <c r="D52" s="56"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" s="88" t="s">
         <v>191</v>
       </c>
-      <c r="B52" s="72" t="s">
+      <c r="B53" s="72" t="s">
         <v>157</v>
       </c>
-      <c r="C52" s="88"/>
-      <c r="D52" s="88"/>
-      <c r="E52" s="64"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" s="122" t="s">
-        <v>326</v>
-      </c>
-      <c r="B53" s="67"/>
-      <c r="C53" s="67"/>
-      <c r="D53" s="113"/>
+      <c r="C53" s="88"/>
+      <c r="D53" s="88"/>
       <c r="E53" s="64"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54" s="71" t="s">
-        <v>327</v>
-      </c>
-      <c r="B54" s="72" t="s">
-        <v>333</v>
-      </c>
-      <c r="C54" s="70"/>
-      <c r="E54" s="64"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55" s="122" t="s">
+      <c r="A54" s="122" t="s">
         <v>281</v>
       </c>
-      <c r="B55" s="130"/>
-      <c r="C55" s="130"/>
-      <c r="D55" s="130"/>
+      <c r="B54" s="130"/>
+      <c r="C54" s="130"/>
+      <c r="D54" s="130"/>
+      <c r="E54" s="131"/>
+    </row>
+    <row r="55" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="132" t="s">
+        <v>313</v>
+      </c>
+      <c r="B55" s="131" t="s">
+        <v>332</v>
+      </c>
+      <c r="C55" s="131"/>
+      <c r="D55" s="131"/>
       <c r="E55" s="131"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56" s="132" t="s">
-        <v>314</v>
-      </c>
-      <c r="B56" s="131" t="s">
-        <v>334</v>
-      </c>
-      <c r="C56" s="131"/>
-      <c r="D56" s="131"/>
-      <c r="E56" s="131"/>
+      <c r="A56" s="71"/>
+      <c r="B56" s="72"/>
+      <c r="C56" s="70"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57" s="71"/>
-      <c r="B57" s="72"/>
-      <c r="C57" s="70"/>
+      <c r="A57" s="100" t="s">
+        <v>92</v>
+      </c>
+      <c r="B57" s="100"/>
+      <c r="C57" s="149"/>
+      <c r="D57" s="149"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58" s="100" t="s">
-        <v>92</v>
-      </c>
-      <c r="B58" s="100"/>
-      <c r="C58" s="149"/>
-      <c r="D58" s="149"/>
+      <c r="A58" s="101" t="s">
+        <v>95</v>
+      </c>
+      <c r="B58" s="101" t="s">
+        <v>93</v>
+      </c>
+      <c r="C58" s="148" t="s">
+        <v>94</v>
+      </c>
+      <c r="D58" s="148"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59" s="101" t="s">
-        <v>95</v>
-      </c>
-      <c r="B59" s="101" t="s">
-        <v>93</v>
-      </c>
-      <c r="C59" s="148" t="s">
-        <v>94</v>
-      </c>
-      <c r="D59" s="148"/>
-    </row>
-    <row r="60" spans="1:5" ht="92.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="102" t="s">
+        <v>96</v>
+      </c>
+      <c r="B59" s="102" t="s">
+        <v>98</v>
+      </c>
+      <c r="C59" s="147" t="s">
+        <v>230</v>
+      </c>
+      <c r="D59" s="147"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="102" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="B60" s="102" t="s">
-        <v>98</v>
+        <v>174</v>
       </c>
       <c r="C60" s="147" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D60" s="147"/>
     </row>
-    <row r="61" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="102" t="s">
-        <v>79</v>
+        <v>97</v>
       </c>
       <c r="B61" s="102" t="s">
-        <v>174</v>
-      </c>
-      <c r="C61" s="147" t="s">
-        <v>231</v>
-      </c>
-      <c r="D61" s="147"/>
+        <v>176</v>
+      </c>
+      <c r="C61" s="145" t="s">
+        <v>175</v>
+      </c>
+      <c r="D61" s="145"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="102" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="B62" s="102" t="s">
-        <v>176</v>
-      </c>
-      <c r="C62" s="145" t="s">
-        <v>175</v>
-      </c>
-      <c r="D62" s="145"/>
-    </row>
-    <row r="63" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="102" t="s">
-        <v>71</v>
-      </c>
-      <c r="B63" s="102" t="s">
         <v>177</v>
       </c>
-      <c r="C63" s="144" t="s">
+      <c r="C62" s="144" t="s">
         <v>232</v>
       </c>
-      <c r="D63" s="144"/>
+      <c r="D62" s="144"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="C63:D63"/>
     <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C61:D61"/>
     <mergeCell ref="A3:C3"/>
+    <mergeCell ref="C59:D59"/>
     <mergeCell ref="C60:D60"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="C59:D59"/>
     <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C57:D57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5252,10 +5310,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I98"/>
+  <dimension ref="A1:I104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="B52" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -5305,19 +5363,19 @@
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="49"/>
       <c r="B4" s="48" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C4" s="48" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="49"/>
       <c r="B5" s="48" t="s">
+        <v>336</v>
+      </c>
+      <c r="C5" s="48" t="s">
         <v>337</v>
-      </c>
-      <c r="C5" s="48" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -5336,405 +5394,402 @@
         <v>268</v>
       </c>
       <c r="C7" s="48" t="s">
-        <v>313</v>
+        <v>341</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="62"/>
-      <c r="B8" s="127" t="s">
+      <c r="A8" s="49"/>
+      <c r="B8" s="48" t="s">
+        <v>345</v>
+      </c>
+      <c r="C8" s="48" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="49"/>
+      <c r="B9" s="127" t="s">
+        <v>342</v>
+      </c>
+      <c r="C9" s="128"/>
+      <c r="D9" s="128"/>
+      <c r="E9" s="126"/>
+      <c r="F9" s="126"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="49"/>
+      <c r="B10" s="88" t="s">
+        <v>343</v>
+      </c>
+      <c r="C10" s="89" t="s">
+        <v>344</v>
+      </c>
+      <c r="D10" s="88"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="49"/>
+      <c r="B11" s="127" t="s">
+        <v>338</v>
+      </c>
+      <c r="C11" s="128"/>
+      <c r="D11" s="128"/>
+      <c r="E11" s="126"/>
+      <c r="F11" s="126"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="49"/>
+      <c r="B12" s="88" t="s">
+        <v>339</v>
+      </c>
+      <c r="C12" s="89" t="s">
+        <v>340</v>
+      </c>
+      <c r="D12" s="88"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="62"/>
+      <c r="B13" s="127" t="s">
+        <v>329</v>
+      </c>
+      <c r="C13" s="128"/>
+      <c r="D13" s="128"/>
+      <c r="E13" s="126"/>
+      <c r="F13" s="126"/>
+      <c r="I13" s="48" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="63"/>
+      <c r="B14" s="88" t="s">
         <v>330</v>
       </c>
-      <c r="C8" s="128"/>
-      <c r="D8" s="128"/>
-      <c r="E8" s="126"/>
-      <c r="F8" s="126"/>
-      <c r="I8" s="48" t="s">
+      <c r="C14" s="89" t="s">
+        <v>331</v>
+      </c>
+      <c r="D14" s="88"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="51"/>
+      <c r="B15" s="51"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="51"/>
+      <c r="I15" s="125" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="52"/>
+      <c r="B16" s="59" t="s">
+        <v>235</v>
+      </c>
+      <c r="C16" s="53"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="53"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B17" s="48" t="s">
+        <v>112</v>
+      </c>
+      <c r="C17" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="H17" s="124"/>
+      <c r="I17" s="48" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H18" s="126"/>
+      <c r="I18" s="48" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="51"/>
+      <c r="B19" s="51"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="51"/>
+      <c r="H19" s="113"/>
+      <c r="I19" s="48" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="52"/>
+      <c r="B20" s="60" t="s">
+        <v>236</v>
+      </c>
+      <c r="C20" s="61"/>
+      <c r="D20" s="61"/>
+      <c r="E20" s="52"/>
+      <c r="F20" s="52"/>
+      <c r="H20" s="114"/>
+      <c r="I20" s="48" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="62"/>
+      <c r="B21" s="127" t="s">
+        <v>256</v>
+      </c>
+      <c r="C21" s="128"/>
+      <c r="D21" s="128"/>
+      <c r="E21" s="126"/>
+      <c r="F21" s="126"/>
+      <c r="I21" s="48" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="63"/>
-      <c r="B9" s="88" t="s">
-        <v>331</v>
-      </c>
-      <c r="C9" s="89" t="s">
-        <v>332</v>
-      </c>
-      <c r="D9" s="88"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="51"/>
-      <c r="B10" s="51"/>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="51"/>
-      <c r="I10" s="125" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="52"/>
-      <c r="B11" s="59" t="s">
-        <v>235</v>
-      </c>
-      <c r="C11" s="53"/>
-      <c r="D11" s="53"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="53"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="48" t="s">
-        <v>112</v>
-      </c>
-      <c r="C12" s="48" t="s">
-        <v>87</v>
-      </c>
-      <c r="H12" s="124"/>
-      <c r="I12" s="48" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H13" s="126"/>
-      <c r="I13" s="48" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="51"/>
-      <c r="B14" s="51"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="51"/>
-      <c r="H14" s="113"/>
-      <c r="I14" s="48" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="52"/>
-      <c r="B15" s="60" t="s">
-        <v>236</v>
-      </c>
-      <c r="C15" s="61"/>
-      <c r="D15" s="61"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52"/>
-      <c r="H15" s="114"/>
-      <c r="I15" s="48" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="62"/>
-      <c r="B16" s="127" t="s">
-        <v>256</v>
-      </c>
-      <c r="C16" s="128"/>
-      <c r="D16" s="128"/>
-      <c r="E16" s="126"/>
-      <c r="F16" s="126"/>
-      <c r="I16" s="48" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="63"/>
-      <c r="B17" s="121" t="s">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="63"/>
+      <c r="B22" s="121" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="121" t="s">
+      <c r="C22" s="121" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="121" t="s">
+      <c r="D22" s="121" t="s">
         <v>58</v>
       </c>
-      <c r="E17" s="120"/>
-      <c r="F17" s="120"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="63"/>
-      <c r="B18" s="88" t="s">
+      <c r="E22" s="120"/>
+      <c r="F22" s="120"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="63"/>
+      <c r="B23" s="88" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="89" t="s">
+      <c r="C23" s="89" t="s">
         <v>144</v>
       </c>
-      <c r="D18" s="88"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="63"/>
-      <c r="B19" s="66" t="s">
+      <c r="D23" s="88"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="63"/>
+      <c r="B24" s="66" t="s">
         <v>237</v>
       </c>
-      <c r="C19" s="67"/>
-      <c r="D19" s="67"/>
-      <c r="E19" s="113"/>
-      <c r="F19" s="113"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="63"/>
-      <c r="B20" s="69" t="s">
+      <c r="C24" s="67"/>
+      <c r="D24" s="67"/>
+      <c r="E24" s="113"/>
+      <c r="F24" s="113"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="63"/>
+      <c r="B25" s="69" t="s">
         <v>76</v>
       </c>
-      <c r="C20" s="64" t="s">
+      <c r="C25" s="64" t="s">
         <v>131</v>
       </c>
-      <c r="D20" s="64" t="s">
+      <c r="D25" s="64" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="65" t="s">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="65" t="s">
         <v>80</v>
       </c>
-      <c r="B21" s="69" t="s">
+      <c r="B26" s="69" t="s">
         <v>102</v>
       </c>
-      <c r="C21" s="64" t="s">
+      <c r="C26" s="64" t="s">
         <v>130</v>
       </c>
-      <c r="D21" s="70" t="s">
+      <c r="D26" s="70" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="22" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="68"/>
-      <c r="B22" s="69" t="s">
+    <row r="27" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="68"/>
+      <c r="B27" s="69" t="s">
         <v>99</v>
       </c>
-      <c r="C22" s="64" t="s">
+      <c r="C27" s="64" t="s">
         <v>113</v>
       </c>
-      <c r="D22" s="70" t="s">
+      <c r="D27" s="70" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="23" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="68"/>
-      <c r="B23" s="69" t="s">
+    <row r="28" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="68"/>
+      <c r="B28" s="69" t="s">
         <v>100</v>
       </c>
-      <c r="C23" s="64" t="s">
+      <c r="C28" s="64" t="s">
         <v>132</v>
       </c>
-      <c r="D23" s="64" t="s">
+      <c r="D28" s="64" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="68"/>
-      <c r="B24" s="69" t="s">
+    <row r="29" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="68"/>
+      <c r="B29" s="69" t="s">
         <v>310</v>
       </c>
-      <c r="C24" s="64" t="s">
+      <c r="C29" s="64" t="s">
         <v>311</v>
       </c>
-      <c r="D24" s="64"/>
-    </row>
-    <row r="25" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="68"/>
-      <c r="B25" s="71" t="s">
+      <c r="D29" s="64"/>
+    </row>
+    <row r="30" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="68"/>
+      <c r="B30" s="71" t="s">
         <v>91</v>
       </c>
-      <c r="C25" s="72" t="s">
+      <c r="C30" s="72" t="s">
         <v>118</v>
-      </c>
-      <c r="D25" s="70" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="68"/>
-      <c r="B26" s="66" t="s">
-        <v>238</v>
-      </c>
-      <c r="C26" s="67" t="s">
-        <v>14</v>
-      </c>
-      <c r="D26" s="67"/>
-      <c r="E26" s="113"/>
-      <c r="F26" s="113"/>
-    </row>
-    <row r="27" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="68"/>
-      <c r="B27" s="75" t="s">
-        <v>240</v>
-      </c>
-      <c r="C27" s="76"/>
-      <c r="D27" s="76"/>
-      <c r="E27" s="114"/>
-      <c r="F27" s="114"/>
-    </row>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="73" t="s">
-        <v>81</v>
-      </c>
-      <c r="B28" s="77" t="s">
-        <v>136</v>
-      </c>
-      <c r="C28" s="70" t="s">
-        <v>252</v>
-      </c>
-      <c r="D28" s="70"/>
-    </row>
-    <row r="29" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="74"/>
-      <c r="B29" s="77" t="s">
-        <v>78</v>
-      </c>
-      <c r="C29" s="70" t="s">
-        <v>253</v>
-      </c>
-      <c r="D29" s="70"/>
-    </row>
-    <row r="30" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="74"/>
-      <c r="B30" s="77" t="s">
-        <v>101</v>
-      </c>
-      <c r="C30" s="70" t="s">
-        <v>114</v>
       </c>
       <c r="D30" s="70" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="31" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="74"/>
-      <c r="B31" s="75" t="s">
-        <v>239</v>
-      </c>
-      <c r="C31" s="76"/>
-      <c r="D31" s="76"/>
-      <c r="E31" s="114"/>
-      <c r="F31" s="114"/>
-    </row>
-    <row r="32" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="74"/>
-      <c r="B32" s="77" t="s">
-        <v>104</v>
-      </c>
-      <c r="C32" s="78" t="s">
-        <v>133</v>
-      </c>
-      <c r="D32" s="70" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="74"/>
+    <row r="31" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="68"/>
+      <c r="B31" s="66" t="s">
+        <v>238</v>
+      </c>
+      <c r="C31" s="67" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="67"/>
+      <c r="E31" s="113"/>
+      <c r="F31" s="113"/>
+    </row>
+    <row r="32" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="68"/>
+      <c r="B32" s="75" t="s">
+        <v>240</v>
+      </c>
+      <c r="C32" s="76"/>
+      <c r="D32" s="76"/>
+      <c r="E32" s="114"/>
+      <c r="F32" s="114"/>
+    </row>
+    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="73" t="s">
+        <v>81</v>
+      </c>
       <c r="B33" s="77" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C33" s="70" t="s">
-        <v>254</v>
-      </c>
-      <c r="D33" s="72"/>
-      <c r="E33" s="64"/>
+        <v>252</v>
+      </c>
+      <c r="D33" s="70"/>
     </row>
     <row r="34" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A34" s="74"/>
       <c r="B34" s="77" t="s">
-        <v>143</v>
+        <v>78</v>
       </c>
       <c r="C34" s="70" t="s">
-        <v>144</v>
-      </c>
-      <c r="D34" s="72"/>
+        <v>253</v>
+      </c>
+      <c r="D34" s="70"/>
     </row>
     <row r="35" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A35" s="74"/>
-      <c r="B35" s="66" t="s">
-        <v>241</v>
-      </c>
-      <c r="C35" s="67"/>
-      <c r="D35" s="67"/>
-      <c r="E35" s="113"/>
-      <c r="F35" s="113"/>
+      <c r="B35" s="77" t="s">
+        <v>101</v>
+      </c>
+      <c r="C35" s="70" t="s">
+        <v>114</v>
+      </c>
+      <c r="D35" s="70" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="36" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A36" s="74"/>
-      <c r="B36" s="80" t="s">
-        <v>242</v>
-      </c>
-      <c r="C36" s="81"/>
-      <c r="D36" s="81"/>
+      <c r="B36" s="75" t="s">
+        <v>239</v>
+      </c>
+      <c r="C36" s="76"/>
+      <c r="D36" s="76"/>
       <c r="E36" s="114"/>
       <c r="F36" s="114"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A37" s="74"/>
       <c r="B37" s="77" t="s">
+        <v>104</v>
+      </c>
+      <c r="C37" s="78" t="s">
+        <v>133</v>
+      </c>
+      <c r="D37" s="70" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="74"/>
+      <c r="B38" s="77" t="s">
+        <v>142</v>
+      </c>
+      <c r="C38" s="70" t="s">
+        <v>254</v>
+      </c>
+      <c r="D38" s="72"/>
+      <c r="E38" s="64"/>
+    </row>
+    <row r="39" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="74"/>
+      <c r="B39" s="77" t="s">
+        <v>143</v>
+      </c>
+      <c r="C39" s="70" t="s">
+        <v>144</v>
+      </c>
+      <c r="D39" s="72"/>
+    </row>
+    <row r="40" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="74"/>
+      <c r="B40" s="66" t="s">
+        <v>241</v>
+      </c>
+      <c r="C40" s="67"/>
+      <c r="D40" s="67"/>
+      <c r="E40" s="113"/>
+      <c r="F40" s="113"/>
+    </row>
+    <row r="41" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="74"/>
+      <c r="B41" s="80" t="s">
+        <v>242</v>
+      </c>
+      <c r="C41" s="81"/>
+      <c r="D41" s="81"/>
+      <c r="E41" s="114"/>
+      <c r="F41" s="114"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="74"/>
+      <c r="B42" s="77" t="s">
         <v>103</v>
       </c>
-      <c r="C37" s="83" t="s">
+      <c r="C42" s="83" t="s">
         <v>251</v>
       </c>
-      <c r="D37" s="72" t="s">
+      <c r="D42" s="72" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="38" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="79" t="s">
+    <row r="43" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="79" t="s">
         <v>82</v>
       </c>
-      <c r="B38" s="80" t="s">
+      <c r="B43" s="80" t="s">
         <v>243</v>
-      </c>
-      <c r="C38" s="81"/>
-      <c r="D38" s="81"/>
-      <c r="E38" s="114"/>
-      <c r="F38" s="114"/>
-    </row>
-    <row r="39" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="82"/>
-      <c r="B39" s="80" t="s">
-        <v>244</v>
-      </c>
-      <c r="C39" s="81"/>
-      <c r="D39" s="81"/>
-      <c r="E39" s="114"/>
-      <c r="F39" s="114"/>
-    </row>
-    <row r="40" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="82"/>
-      <c r="B40" s="84" t="s">
-        <v>207</v>
-      </c>
-      <c r="C40" s="86" t="s">
-        <v>217</v>
-      </c>
-      <c r="D40" s="72"/>
-    </row>
-    <row r="41" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="82"/>
-      <c r="B41" s="84" t="s">
-        <v>208</v>
-      </c>
-      <c r="C41" s="48" t="s">
-        <v>209</v>
-      </c>
-      <c r="D41" s="72" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="82"/>
-      <c r="B42" s="84" t="s">
-        <v>170</v>
-      </c>
-      <c r="C42" s="85" t="s">
-        <v>216</v>
-      </c>
-      <c r="D42" s="72"/>
-    </row>
-    <row r="43" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="82"/>
-      <c r="B43" s="80" t="s">
-        <v>245</v>
       </c>
       <c r="C43" s="81"/>
       <c r="D43" s="81"/>
@@ -5743,392 +5798,394 @@
     </row>
     <row r="44" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A44" s="82"/>
-      <c r="B44" s="84" t="s">
-        <v>85</v>
-      </c>
-      <c r="C44" s="86" t="s">
-        <v>255</v>
-      </c>
-      <c r="D44" s="72" t="s">
-        <v>77</v>
-      </c>
+      <c r="B44" s="80" t="s">
+        <v>244</v>
+      </c>
+      <c r="C44" s="81"/>
+      <c r="D44" s="81"/>
+      <c r="E44" s="114"/>
+      <c r="F44" s="114"/>
     </row>
     <row r="45" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A45" s="82"/>
       <c r="B45" s="84" t="s">
-        <v>84</v>
+        <v>207</v>
       </c>
       <c r="C45" s="86" t="s">
-        <v>134</v>
-      </c>
-      <c r="D45" s="72" t="s">
-        <v>77</v>
-      </c>
+        <v>217</v>
+      </c>
+      <c r="D45" s="72"/>
     </row>
     <row r="46" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A46" s="82"/>
-      <c r="B46" s="66" t="s">
-        <v>246</v>
-      </c>
-      <c r="C46" s="67"/>
-      <c r="D46" s="67"/>
-      <c r="E46" s="113"/>
-      <c r="F46" s="113"/>
+      <c r="B46" s="84" t="s">
+        <v>208</v>
+      </c>
+      <c r="C46" s="48" t="s">
+        <v>209</v>
+      </c>
+      <c r="D46" s="72" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="47" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A47" s="82"/>
-      <c r="B47" s="71" t="s">
-        <v>86</v>
-      </c>
-      <c r="C47" s="72" t="s">
-        <v>135</v>
-      </c>
-      <c r="D47" s="72" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="65" t="s">
-        <v>83</v>
-      </c>
-      <c r="B48" s="66" t="s">
-        <v>247</v>
-      </c>
-      <c r="C48" s="67"/>
-      <c r="D48" s="67"/>
-      <c r="E48" s="113"/>
-      <c r="F48" s="113"/>
+      <c r="B47" s="84" t="s">
+        <v>170</v>
+      </c>
+      <c r="C47" s="85" t="s">
+        <v>216</v>
+      </c>
+      <c r="D47" s="72"/>
+    </row>
+    <row r="48" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="82"/>
+      <c r="B48" s="80" t="s">
+        <v>245</v>
+      </c>
+      <c r="C48" s="81"/>
+      <c r="D48" s="81"/>
+      <c r="E48" s="114"/>
+      <c r="F48" s="114"/>
     </row>
     <row r="49" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="65"/>
-      <c r="B49" s="71" t="s">
-        <v>153</v>
-      </c>
-      <c r="C49" s="72" t="s">
-        <v>152</v>
-      </c>
-      <c r="D49" s="70"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B50" s="71" t="s">
-        <v>154</v>
-      </c>
-      <c r="C50" s="72" t="s">
-        <v>155</v>
-      </c>
-      <c r="D50" s="70"/>
+      <c r="A49" s="82"/>
+      <c r="B49" s="84" t="s">
+        <v>85</v>
+      </c>
+      <c r="C49" s="86" t="s">
+        <v>255</v>
+      </c>
+      <c r="D49" s="72" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="82"/>
+      <c r="B50" s="84" t="s">
+        <v>84</v>
+      </c>
+      <c r="C50" s="86" t="s">
+        <v>134</v>
+      </c>
+      <c r="D50" s="72" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="51" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="82"/>
       <c r="B51" s="66" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C51" s="67"/>
       <c r="D51" s="67"/>
-      <c r="E51" s="67"/>
-      <c r="F51" s="67"/>
+      <c r="E51" s="113"/>
+      <c r="F51" s="113"/>
     </row>
     <row r="52" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B52" s="54"/>
-      <c r="C52" s="55"/>
-      <c r="D52" s="55"/>
-      <c r="E52" s="55"/>
-      <c r="F52" s="55"/>
+      <c r="A52" s="82"/>
+      <c r="B52" s="71" t="s">
+        <v>86</v>
+      </c>
+      <c r="C52" s="72" t="s">
+        <v>135</v>
+      </c>
+      <c r="D52" s="72" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="51"/>
-      <c r="B53" s="122" t="s">
-        <v>326</v>
+      <c r="A53" s="65" t="s">
+        <v>83</v>
+      </c>
+      <c r="B53" s="66" t="s">
+        <v>247</v>
       </c>
       <c r="C53" s="67"/>
       <c r="D53" s="67"/>
       <c r="E53" s="113"/>
       <c r="F53" s="113"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="65"/>
       <c r="B54" s="71" t="s">
-        <v>327</v>
+        <v>153</v>
       </c>
       <c r="C54" s="72" t="s">
-        <v>328</v>
+        <v>152</v>
       </c>
       <c r="D54" s="70"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" s="51"/>
-      <c r="B55" s="122" t="s">
-        <v>266</v>
-      </c>
-      <c r="C55" s="67"/>
-      <c r="D55" s="67"/>
-      <c r="E55" s="113"/>
-      <c r="F55" s="113"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" s="51"/>
-      <c r="B56" s="123" t="s">
-        <v>262</v>
-      </c>
-      <c r="C56" s="105" t="s">
-        <v>269</v>
-      </c>
-      <c r="D56" s="55"/>
-      <c r="E56" s="64"/>
-      <c r="F56" s="64"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" s="51"/>
-      <c r="B57" s="123" t="s">
-        <v>265</v>
-      </c>
-      <c r="C57" s="105" t="s">
-        <v>270</v>
-      </c>
+      <c r="B55" s="71" t="s">
+        <v>154</v>
+      </c>
+      <c r="C55" s="72" t="s">
+        <v>155</v>
+      </c>
+      <c r="D55" s="70"/>
+    </row>
+    <row r="56" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B56" s="66" t="s">
+        <v>248</v>
+      </c>
+      <c r="C56" s="67"/>
+      <c r="D56" s="67"/>
+      <c r="E56" s="67"/>
+      <c r="F56" s="67"/>
+    </row>
+    <row r="57" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B57" s="54"/>
+      <c r="C57" s="55"/>
       <c r="D57" s="55"/>
-      <c r="E57" s="64"/>
-      <c r="F57" s="64"/>
+      <c r="E57" s="55"/>
+      <c r="F57" s="55"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="51"/>
-      <c r="B58" s="123" t="s">
-        <v>261</v>
-      </c>
-      <c r="C58" s="105" t="s">
-        <v>271</v>
-      </c>
-      <c r="D58" s="55"/>
-      <c r="E58" s="64"/>
-      <c r="F58" s="64"/>
+      <c r="B58" s="122" t="s">
+        <v>325</v>
+      </c>
+      <c r="C58" s="67"/>
+      <c r="D58" s="67"/>
+      <c r="E58" s="113"/>
+      <c r="F58" s="113"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" s="51"/>
-      <c r="B59" s="123" t="s">
-        <v>263</v>
-      </c>
-      <c r="C59" s="105" t="s">
-        <v>272</v>
-      </c>
-      <c r="D59" s="55"/>
-      <c r="E59" s="64"/>
-      <c r="F59" s="64"/>
+      <c r="B59" s="71" t="s">
+        <v>326</v>
+      </c>
+      <c r="C59" s="72" t="s">
+        <v>327</v>
+      </c>
+      <c r="D59" s="70"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="51"/>
-      <c r="B60" s="123" t="s">
-        <v>264</v>
-      </c>
-      <c r="C60" s="105" t="s">
-        <v>273</v>
-      </c>
-      <c r="D60" s="55"/>
-      <c r="E60" s="64"/>
-      <c r="F60" s="64"/>
+      <c r="B60" s="122" t="s">
+        <v>266</v>
+      </c>
+      <c r="C60" s="67"/>
+      <c r="D60" s="67"/>
+      <c r="E60" s="113"/>
+      <c r="F60" s="113"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="51"/>
-      <c r="B61" s="122" t="s">
-        <v>267</v>
-      </c>
-      <c r="C61" s="67"/>
-      <c r="D61" s="67"/>
-      <c r="E61" s="113"/>
-      <c r="F61" s="113"/>
-    </row>
-    <row r="62" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B61" s="123" t="s">
+        <v>262</v>
+      </c>
+      <c r="C61" s="105" t="s">
+        <v>269</v>
+      </c>
+      <c r="D61" s="55"/>
+      <c r="E61" s="64"/>
+      <c r="F61" s="64"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="51"/>
       <c r="B62" s="123" t="s">
-        <v>268</v>
-      </c>
-      <c r="C62" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B63" s="122" t="s">
-        <v>281</v>
-      </c>
-      <c r="C63" s="130"/>
-      <c r="D63" s="130"/>
-      <c r="E63" s="130"/>
-      <c r="F63" s="130"/>
-    </row>
-    <row r="64" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B64" s="132" t="s">
-        <v>314</v>
-      </c>
-      <c r="C64" s="131" t="s">
-        <v>282</v>
-      </c>
-      <c r="D64" s="131"/>
-      <c r="E64" s="131"/>
-      <c r="F64" s="131"/>
+        <v>265</v>
+      </c>
+      <c r="C62" s="105" t="s">
+        <v>270</v>
+      </c>
+      <c r="D62" s="55"/>
+      <c r="E62" s="64"/>
+      <c r="F62" s="64"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="51"/>
+      <c r="B63" s="123" t="s">
+        <v>261</v>
+      </c>
+      <c r="C63" s="105" t="s">
+        <v>271</v>
+      </c>
+      <c r="D63" s="55"/>
+      <c r="E63" s="64"/>
+      <c r="F63" s="64"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" s="51"/>
+      <c r="B64" s="123" t="s">
+        <v>263</v>
+      </c>
+      <c r="C64" s="105" t="s">
+        <v>272</v>
+      </c>
+      <c r="D64" s="55"/>
+      <c r="E64" s="64"/>
+      <c r="F64" s="64"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="51"/>
-      <c r="B65" s="127" t="s">
-        <v>249</v>
-      </c>
-      <c r="C65" s="129"/>
-      <c r="D65" s="129"/>
-      <c r="E65" s="129"/>
-      <c r="F65" s="129"/>
+      <c r="B65" s="123" t="s">
+        <v>264</v>
+      </c>
+      <c r="C65" s="105" t="s">
+        <v>273</v>
+      </c>
+      <c r="D65" s="55"/>
+      <c r="E65" s="64"/>
+      <c r="F65" s="64"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="51"/>
-      <c r="B66" s="88" t="s">
-        <v>117</v>
-      </c>
-      <c r="C66" s="89" t="s">
-        <v>116</v>
-      </c>
-      <c r="D66" s="88"/>
+      <c r="B66" s="122" t="s">
+        <v>267</v>
+      </c>
+      <c r="C66" s="67"/>
+      <c r="D66" s="67"/>
+      <c r="E66" s="113"/>
+      <c r="F66" s="113"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="51"/>
-      <c r="B67" s="88" t="s">
+      <c r="B67" s="123" t="s">
+        <v>347</v>
+      </c>
+      <c r="C67" t="s">
+        <v>348</v>
+      </c>
+      <c r="D67"/>
+      <c r="E67"/>
+      <c r="F67"/>
+    </row>
+    <row r="68" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B68" s="123" t="s">
+        <v>268</v>
+      </c>
+      <c r="C68" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B69" s="122" t="s">
+        <v>281</v>
+      </c>
+      <c r="C69" s="130"/>
+      <c r="D69" s="130"/>
+      <c r="E69" s="130"/>
+      <c r="F69" s="130"/>
+    </row>
+    <row r="70" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B70" s="132" t="s">
+        <v>313</v>
+      </c>
+      <c r="C70" s="131" t="s">
+        <v>282</v>
+      </c>
+      <c r="D70" s="131"/>
+      <c r="E70" s="131"/>
+      <c r="F70" s="131"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" s="51"/>
+      <c r="B71" s="127" t="s">
+        <v>249</v>
+      </c>
+      <c r="C71" s="129"/>
+      <c r="D71" s="129"/>
+      <c r="E71" s="129"/>
+      <c r="F71" s="129"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" s="51"/>
+      <c r="B72" s="88" t="s">
+        <v>117</v>
+      </c>
+      <c r="C72" s="89" t="s">
+        <v>116</v>
+      </c>
+      <c r="D72" s="88"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" s="51"/>
+      <c r="B73" s="88" t="s">
+        <v>314</v>
+      </c>
+      <c r="C73" s="89" t="s">
         <v>315</v>
       </c>
-      <c r="C67" s="89" t="s">
+      <c r="D73" s="88"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" s="52"/>
+      <c r="B74" s="88" t="s">
+        <v>140</v>
+      </c>
+      <c r="C74" s="89" t="s">
+        <v>141</v>
+      </c>
+      <c r="D74" s="88"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" s="52"/>
+      <c r="B75" s="88" t="s">
+        <v>326</v>
+      </c>
+      <c r="C75" s="89" t="s">
+        <v>328</v>
+      </c>
+      <c r="D75" s="88"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" s="87"/>
+      <c r="B76" s="69" t="s">
+        <v>111</v>
+      </c>
+      <c r="C76" s="64" t="s">
+        <v>115</v>
+      </c>
+      <c r="D76" s="64"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" s="87"/>
+      <c r="B77" s="142" t="s">
         <v>316</v>
       </c>
-      <c r="D67" s="88"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68" s="52"/>
-      <c r="B68" s="88" t="s">
-        <v>140</v>
-      </c>
-      <c r="C68" s="89" t="s">
-        <v>141</v>
-      </c>
-      <c r="D68" s="88"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69" s="52"/>
-      <c r="B69" s="88" t="s">
-        <v>327</v>
-      </c>
-      <c r="C69" s="89" t="s">
-        <v>329</v>
-      </c>
-      <c r="D69" s="88"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70" s="87"/>
-      <c r="B70" s="69" t="s">
-        <v>111</v>
-      </c>
-      <c r="C70" s="64" t="s">
-        <v>115</v>
-      </c>
-      <c r="D70" s="64"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A71" s="87"/>
-      <c r="B71" s="142" t="s">
+      <c r="C77" s="119"/>
+      <c r="D77" s="119"/>
+      <c r="E77" s="119"/>
+      <c r="F77" s="119"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" s="87"/>
+      <c r="B78" s="71" t="s">
+        <v>119</v>
+      </c>
+      <c r="C78" s="72" t="s">
+        <v>158</v>
+      </c>
+      <c r="D78" s="72"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79" s="87"/>
+      <c r="B79" s="71" t="s">
+        <v>318</v>
+      </c>
+      <c r="C79" s="72" t="s">
         <v>317</v>
       </c>
-      <c r="C71" s="119"/>
-      <c r="D71" s="119"/>
-      <c r="E71" s="119"/>
-      <c r="F71" s="119"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72" s="87"/>
-      <c r="B72" s="71" t="s">
-        <v>119</v>
-      </c>
-      <c r="C72" s="72" t="s">
-        <v>158</v>
-      </c>
-      <c r="D72" s="72"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73" s="87"/>
-      <c r="B73" s="71" t="s">
+      <c r="D79" s="72"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A80" s="87"/>
+      <c r="B80" s="71" t="s">
         <v>319</v>
       </c>
-      <c r="C73" s="72" t="s">
-        <v>318</v>
-      </c>
-      <c r="D73" s="72"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74" s="87"/>
-      <c r="B74" s="71" t="s">
+      <c r="C80" s="72" t="s">
         <v>320</v>
       </c>
-      <c r="C74" s="72" t="s">
+      <c r="D80" s="72"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" s="119" t="s">
+        <v>250</v>
+      </c>
+      <c r="B81" s="142" t="s">
         <v>321</v>
-      </c>
-      <c r="D74" s="72"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A75" s="119" t="s">
-        <v>250</v>
-      </c>
-      <c r="B75" s="142" t="s">
-        <v>322</v>
-      </c>
-      <c r="C75" s="119"/>
-      <c r="D75" s="119"/>
-      <c r="E75" s="119"/>
-      <c r="F75" s="119"/>
-    </row>
-    <row r="76" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="90"/>
-      <c r="B76" s="71" t="s">
-        <v>38</v>
-      </c>
-      <c r="C76" s="72" t="s">
-        <v>163</v>
-      </c>
-      <c r="D76" s="72"/>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A77" s="119" t="s">
-        <v>257</v>
-      </c>
-      <c r="B77" s="71" t="s">
-        <v>32</v>
-      </c>
-      <c r="C77" s="72" t="s">
-        <v>157</v>
-      </c>
-      <c r="D77" s="72"/>
-    </row>
-    <row r="78" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="90"/>
-      <c r="B78" s="71" t="s">
-        <v>200</v>
-      </c>
-      <c r="C78" s="110" t="s">
-        <v>201</v>
-      </c>
-      <c r="D78" s="72"/>
-    </row>
-    <row r="79" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="91"/>
-      <c r="B79" s="71" t="s">
-        <v>203</v>
-      </c>
-      <c r="C79" s="110" t="s">
-        <v>204</v>
-      </c>
-      <c r="D79" s="72"/>
-    </row>
-    <row r="80" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="91"/>
-      <c r="B80" s="71" t="s">
-        <v>324</v>
-      </c>
-      <c r="C80" s="110" t="s">
-        <v>323</v>
-      </c>
-      <c r="D80" s="72"/>
-    </row>
-    <row r="81" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="91"/>
-      <c r="B81" s="142" t="s">
-        <v>325</v>
       </c>
       <c r="C81" s="119"/>
       <c r="D81" s="119"/>
@@ -6136,168 +6193,230 @@
       <c r="F81" s="119"/>
     </row>
     <row r="82" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="91"/>
-      <c r="B82" s="75" t="s">
+      <c r="A82" s="90"/>
+      <c r="B82" s="71" t="s">
+        <v>38</v>
+      </c>
+      <c r="C82" s="72" t="s">
+        <v>163</v>
+      </c>
+      <c r="D82" s="72"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83" s="119" t="s">
+        <v>257</v>
+      </c>
+      <c r="B83" s="71" t="s">
+        <v>32</v>
+      </c>
+      <c r="C83" s="72" t="s">
+        <v>157</v>
+      </c>
+      <c r="D83" s="72"/>
+    </row>
+    <row r="84" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="90"/>
+      <c r="B84" s="71" t="s">
+        <v>200</v>
+      </c>
+      <c r="C84" s="110" t="s">
+        <v>201</v>
+      </c>
+      <c r="D84" s="72"/>
+    </row>
+    <row r="85" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="91"/>
+      <c r="B85" s="71" t="s">
+        <v>203</v>
+      </c>
+      <c r="C85" s="110" t="s">
+        <v>204</v>
+      </c>
+      <c r="D85" s="72"/>
+    </row>
+    <row r="86" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="91"/>
+      <c r="B86" s="71" t="s">
+        <v>323</v>
+      </c>
+      <c r="C86" s="110" t="s">
+        <v>322</v>
+      </c>
+      <c r="D86" s="72"/>
+    </row>
+    <row r="87" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="91"/>
+      <c r="B87" s="142" t="s">
+        <v>324</v>
+      </c>
+      <c r="C87" s="119"/>
+      <c r="D87" s="119"/>
+      <c r="E87" s="119"/>
+      <c r="F87" s="119"/>
+    </row>
+    <row r="88" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="91"/>
+      <c r="B88" s="75" t="s">
         <v>259</v>
       </c>
-      <c r="C82" s="93"/>
-      <c r="D82" s="93"/>
-      <c r="E82" s="93"/>
-      <c r="F82" s="93"/>
-    </row>
-    <row r="83" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="119" t="s">
+      <c r="C88" s="93"/>
+      <c r="D88" s="93"/>
+      <c r="E88" s="93"/>
+      <c r="F88" s="93"/>
+    </row>
+    <row r="89" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="119" t="s">
         <v>258</v>
       </c>
-      <c r="B83" s="84" t="s">
+      <c r="B89" s="84" t="s">
         <v>90</v>
       </c>
-      <c r="C83" s="72" t="s">
+      <c r="C89" s="72" t="s">
         <v>160</v>
       </c>
-      <c r="D83" s="72"/>
-    </row>
-    <row r="84" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="92"/>
-      <c r="B84" s="84" t="s">
+      <c r="D89" s="72"/>
+    </row>
+    <row r="90" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="92"/>
+      <c r="B90" s="84" t="s">
         <v>89</v>
       </c>
-      <c r="C84" s="72" t="s">
+      <c r="C90" s="72" t="s">
         <v>161</v>
       </c>
-      <c r="D84" s="72"/>
-    </row>
-    <row r="85" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="94"/>
-      <c r="B85" s="75" t="s">
+      <c r="D90" s="72"/>
+    </row>
+    <row r="91" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="94"/>
+      <c r="B91" s="75" t="s">
         <v>260</v>
       </c>
-      <c r="C85" s="93"/>
-      <c r="D85" s="93"/>
-      <c r="E85" s="93"/>
-      <c r="F85" s="93"/>
-    </row>
-    <row r="86" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="94"/>
-      <c r="B86" s="118" t="s">
+      <c r="C91" s="93"/>
+      <c r="D91" s="93"/>
+      <c r="E91" s="93"/>
+      <c r="F91" s="93"/>
+    </row>
+    <row r="92" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="94"/>
+      <c r="B92" s="118" t="s">
         <v>137</v>
       </c>
-      <c r="C86" s="72" t="s">
+      <c r="C92" s="72" t="s">
         <v>138</v>
       </c>
-      <c r="D86" s="72"/>
-    </row>
-    <row r="87" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="92"/>
-      <c r="B87" s="118" t="s">
+      <c r="D92" s="72"/>
+    </row>
+    <row r="93" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="92"/>
+      <c r="B93" s="118" t="s">
         <v>137</v>
       </c>
-      <c r="C87" s="72" t="s">
+      <c r="C93" s="72" t="s">
         <v>234</v>
       </c>
-      <c r="D87" s="72"/>
-    </row>
-    <row r="88" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="94"/>
-      <c r="B88" s="118" t="s">
+      <c r="D93" s="72"/>
+    </row>
+    <row r="94" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="94"/>
+      <c r="B94" s="118" t="s">
         <v>192</v>
       </c>
-      <c r="C88" s="72" t="s">
+      <c r="C94" s="72" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="89" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B91" s="106" t="s">
+    <row r="95" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2"/>
+    <row r="97" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B97" s="106" t="s">
         <v>193</v>
       </c>
-      <c r="C91" s="106" t="s">
+      <c r="C97" s="106" t="s">
         <v>197</v>
       </c>
-      <c r="D91" s="149" t="s">
+      <c r="D97" s="149" t="s">
         <v>198</v>
       </c>
-      <c r="E91" s="149"/>
-      <c r="F91" s="149"/>
-    </row>
-    <row r="92" spans="1:6" ht="127.5" x14ac:dyDescent="0.2">
-      <c r="B92" s="109" t="s">
+      <c r="E97" s="149"/>
+      <c r="F97" s="149"/>
+    </row>
+    <row r="98" spans="2:6" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="B98" s="109" t="s">
         <v>194</v>
       </c>
-      <c r="C92" s="108" t="s">
+      <c r="C98" s="108" t="s">
         <v>206</v>
       </c>
-      <c r="D92" s="150" t="s">
+      <c r="D98" s="150" t="s">
         <v>199</v>
       </c>
-      <c r="E92" s="150"/>
-      <c r="F92" s="150"/>
-    </row>
-    <row r="93" spans="1:6" ht="102" x14ac:dyDescent="0.2">
-      <c r="B93" s="109" t="s">
+      <c r="E98" s="150"/>
+      <c r="F98" s="150"/>
+    </row>
+    <row r="99" spans="2:6" ht="102" x14ac:dyDescent="0.2">
+      <c r="B99" s="109" t="s">
         <v>195</v>
       </c>
-      <c r="C93" s="115" t="s">
+      <c r="C99" s="115" t="s">
         <v>205</v>
       </c>
-      <c r="D93" s="150" t="s">
+      <c r="D99" s="150" t="s">
         <v>202</v>
       </c>
-      <c r="E93" s="150"/>
-      <c r="F93" s="150"/>
-    </row>
-    <row r="94" spans="1:6" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="B94" s="109" t="s">
+      <c r="E99" s="150"/>
+      <c r="F99" s="150"/>
+    </row>
+    <row r="100" spans="2:6" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="B100" s="109" t="s">
         <v>196</v>
       </c>
-      <c r="C94" s="108" t="s">
+      <c r="C100" s="108" t="s">
         <v>210</v>
       </c>
-      <c r="D94" s="150" t="s">
+      <c r="D100" s="150" t="s">
         <v>211</v>
       </c>
-      <c r="E94" s="150"/>
-      <c r="F94" s="150"/>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B95" s="117"/>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B96" s="116" t="s">
+      <c r="E100" s="150"/>
+      <c r="F100" s="150"/>
+    </row>
+    <row r="101" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B101" s="117"/>
+    </row>
+    <row r="102" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B102" s="116" t="s">
         <v>219</v>
       </c>
-      <c r="C96" s="116" t="s">
+      <c r="C102" s="116" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="97" spans="2:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="B97" s="117" t="s">
+    <row r="103" spans="2:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="B103" s="117" t="s">
         <v>220</v>
       </c>
-      <c r="C97" s="108" t="s">
+      <c r="C103" s="108" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="98" spans="2:3" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="B98" s="117" t="s">
+    <row r="104" spans="2:6" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="B104" s="117" t="s">
         <v>221</v>
       </c>
-      <c r="C98" s="108" t="s">
+      <c r="C104" s="108" t="s">
         <v>223</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="D94:F94"/>
-    <mergeCell ref="D93:F93"/>
-    <mergeCell ref="D92:F92"/>
-    <mergeCell ref="D91:F91"/>
+    <mergeCell ref="D100:F100"/>
+    <mergeCell ref="D99:F99"/>
+    <mergeCell ref="D98:F98"/>
+    <mergeCell ref="D97:F97"/>
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D92" r:id="rId1"/>
-    <hyperlink ref="D93" r:id="rId2"/>
-    <hyperlink ref="D94" r:id="rId3"/>
+    <hyperlink ref="D98" r:id="rId1"/>
+    <hyperlink ref="D99" r:id="rId2"/>
+    <hyperlink ref="D100" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>

</xml_diff>

<commit_message>
Se agregó las plantillas de Validacion y Verificación
</commit_message>
<xml_diff>
--- a/Organización/Procesos/Soporte Organizacional/2. Administración de Configuración/IWM_Administración de la Configuración.xlsx
+++ b/Organización/Procesos/Soporte Organizacional/2. Administración de Configuración/IWM_Administración de la Configuración.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gus\Desktop\GitHub\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gus\Documents\IWM\CMMI\GitHUB\Organización\Procesos\Soporte Organizacional\2. Administración de Configuración\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="355">
   <si>
     <t>Adapiaciones al Estándar de Administración de Datos</t>
   </si>
@@ -1693,6 +1693,24 @@
   </si>
   <si>
     <t>PTLL_Solicitud_Mejora</t>
+  </si>
+  <si>
+    <t>PTLL_Verificacion_CU</t>
+  </si>
+  <si>
+    <t>Validación de Manual de Requerimientos</t>
+  </si>
+  <si>
+    <t>Verificación de Casos de Uso</t>
+  </si>
+  <si>
+    <t>PTLL_Validacion_Manual_Requerimientos</t>
+  </si>
+  <si>
+    <t>Verificación Análisis y Diseño</t>
+  </si>
+  <si>
+    <t>PTLL_Verificacion_Analisis_y_Diseño</t>
   </si>
 </sst>
 </file>
@@ -4661,8 +4679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:E62"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -5310,10 +5328,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I104"/>
+  <dimension ref="A1:I107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B52" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView tabSelected="1" topLeftCell="B11" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -5584,148 +5602,148 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="63"/>
       <c r="B25" s="69" t="s">
-        <v>76</v>
+        <v>351</v>
       </c>
       <c r="C25" s="64" t="s">
-        <v>131</v>
+        <v>349</v>
       </c>
       <c r="D25" s="64" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="65" t="s">
+      <c r="A26" s="63"/>
+      <c r="B26" s="69" t="s">
+        <v>350</v>
+      </c>
+      <c r="C26" s="64" t="s">
+        <v>352</v>
+      </c>
+      <c r="D26" s="64"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="63"/>
+      <c r="B27" s="69" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" s="64" t="s">
+        <v>131</v>
+      </c>
+      <c r="D27" s="64" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="65" t="s">
         <v>80</v>
       </c>
-      <c r="B26" s="69" t="s">
+      <c r="B28" s="69" t="s">
         <v>102</v>
       </c>
-      <c r="C26" s="64" t="s">
+      <c r="C28" s="64" t="s">
         <v>130</v>
       </c>
-      <c r="D26" s="70" t="s">
+      <c r="D28" s="70" t="s">
         <v>159</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="68"/>
-      <c r="B27" s="69" t="s">
-        <v>99</v>
-      </c>
-      <c r="C27" s="64" t="s">
-        <v>113</v>
-      </c>
-      <c r="D27" s="70" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="68"/>
-      <c r="B28" s="69" t="s">
-        <v>100</v>
-      </c>
-      <c r="C28" s="64" t="s">
-        <v>132</v>
-      </c>
-      <c r="D28" s="64" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="29" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A29" s="68"/>
       <c r="B29" s="69" t="s">
-        <v>310</v>
+        <v>99</v>
       </c>
       <c r="C29" s="64" t="s">
-        <v>311</v>
-      </c>
-      <c r="D29" s="64"/>
+        <v>113</v>
+      </c>
+      <c r="D29" s="70" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="30" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A30" s="68"/>
-      <c r="B30" s="71" t="s">
-        <v>91</v>
-      </c>
-      <c r="C30" s="72" t="s">
-        <v>118</v>
-      </c>
-      <c r="D30" s="70" t="s">
-        <v>159</v>
+      <c r="B30" s="69" t="s">
+        <v>100</v>
+      </c>
+      <c r="C30" s="64" t="s">
+        <v>132</v>
+      </c>
+      <c r="D30" s="64" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A31" s="68"/>
-      <c r="B31" s="66" t="s">
-        <v>238</v>
-      </c>
-      <c r="C31" s="67" t="s">
-        <v>14</v>
-      </c>
-      <c r="D31" s="67"/>
-      <c r="E31" s="113"/>
-      <c r="F31" s="113"/>
+      <c r="B31" s="69" t="s">
+        <v>310</v>
+      </c>
+      <c r="C31" s="64" t="s">
+        <v>311</v>
+      </c>
+      <c r="D31" s="64"/>
     </row>
     <row r="32" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A32" s="68"/>
-      <c r="B32" s="75" t="s">
+      <c r="B32" s="71" t="s">
+        <v>91</v>
+      </c>
+      <c r="C32" s="72" t="s">
+        <v>118</v>
+      </c>
+      <c r="D32" s="70" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="68"/>
+      <c r="B33" s="66" t="s">
+        <v>238</v>
+      </c>
+      <c r="C33" s="67" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="67"/>
+      <c r="E33" s="113"/>
+      <c r="F33" s="113"/>
+    </row>
+    <row r="34" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="68"/>
+      <c r="B34" s="75" t="s">
         <v>240</v>
       </c>
-      <c r="C32" s="76"/>
-      <c r="D32" s="76"/>
-      <c r="E32" s="114"/>
-      <c r="F32" s="114"/>
-    </row>
-    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="73" t="s">
+      <c r="C34" s="76"/>
+      <c r="D34" s="76"/>
+      <c r="E34" s="114"/>
+      <c r="F34" s="114"/>
+    </row>
+    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="73" t="s">
         <v>81</v>
       </c>
-      <c r="B33" s="77" t="s">
+      <c r="B35" s="77" t="s">
         <v>136</v>
       </c>
-      <c r="C33" s="70" t="s">
+      <c r="C35" s="70" t="s">
         <v>252</v>
       </c>
-      <c r="D33" s="70"/>
-    </row>
-    <row r="34" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="74"/>
-      <c r="B34" s="77" t="s">
-        <v>78</v>
-      </c>
-      <c r="C34" s="70" t="s">
-        <v>253</v>
-      </c>
-      <c r="D34" s="70"/>
-    </row>
-    <row r="35" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="74"/>
-      <c r="B35" s="77" t="s">
-        <v>101</v>
-      </c>
-      <c r="C35" s="70" t="s">
-        <v>114</v>
-      </c>
-      <c r="D35" s="70" t="s">
-        <v>159</v>
-      </c>
+      <c r="D35" s="70"/>
     </row>
     <row r="36" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A36" s="74"/>
-      <c r="B36" s="75" t="s">
-        <v>239</v>
-      </c>
-      <c r="C36" s="76"/>
-      <c r="D36" s="76"/>
-      <c r="E36" s="114"/>
-      <c r="F36" s="114"/>
+      <c r="B36" s="77" t="s">
+        <v>78</v>
+      </c>
+      <c r="C36" s="70" t="s">
+        <v>253</v>
+      </c>
+      <c r="D36" s="70"/>
     </row>
     <row r="37" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A37" s="74"/>
       <c r="B37" s="77" t="s">
-        <v>104</v>
-      </c>
-      <c r="C37" s="78" t="s">
-        <v>133</v>
+        <v>101</v>
+      </c>
+      <c r="C37" s="70" t="s">
+        <v>114</v>
       </c>
       <c r="D37" s="70" t="s">
         <v>159</v>
@@ -5733,128 +5751,128 @@
     </row>
     <row r="38" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A38" s="74"/>
-      <c r="B38" s="77" t="s">
-        <v>142</v>
-      </c>
-      <c r="C38" s="70" t="s">
-        <v>254</v>
-      </c>
-      <c r="D38" s="72"/>
-      <c r="E38" s="64"/>
+      <c r="B38" s="75" t="s">
+        <v>239</v>
+      </c>
+      <c r="C38" s="76"/>
+      <c r="D38" s="76"/>
+      <c r="E38" s="114"/>
+      <c r="F38" s="114"/>
     </row>
     <row r="39" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A39" s="74"/>
       <c r="B39" s="77" t="s">
-        <v>143</v>
-      </c>
-      <c r="C39" s="70" t="s">
-        <v>144</v>
-      </c>
-      <c r="D39" s="72"/>
+        <v>104</v>
+      </c>
+      <c r="C39" s="78" t="s">
+        <v>133</v>
+      </c>
+      <c r="D39" s="70" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="40" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A40" s="74"/>
-      <c r="B40" s="66" t="s">
-        <v>241</v>
-      </c>
-      <c r="C40" s="67"/>
-      <c r="D40" s="67"/>
-      <c r="E40" s="113"/>
-      <c r="F40" s="113"/>
+      <c r="B40" s="77" t="s">
+        <v>142</v>
+      </c>
+      <c r="C40" s="70" t="s">
+        <v>254</v>
+      </c>
+      <c r="D40" s="72"/>
+      <c r="E40" s="64"/>
     </row>
     <row r="41" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A41" s="74"/>
-      <c r="B41" s="80" t="s">
+      <c r="B41" s="77" t="s">
+        <v>143</v>
+      </c>
+      <c r="C41" s="70" t="s">
+        <v>144</v>
+      </c>
+      <c r="D41" s="72"/>
+    </row>
+    <row r="42" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="74"/>
+      <c r="B42" s="66" t="s">
+        <v>241</v>
+      </c>
+      <c r="C42" s="67"/>
+      <c r="D42" s="67"/>
+      <c r="E42" s="113"/>
+      <c r="F42" s="113"/>
+    </row>
+    <row r="43" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="74"/>
+      <c r="B43" s="80" t="s">
         <v>242</v>
-      </c>
-      <c r="C41" s="81"/>
-      <c r="D41" s="81"/>
-      <c r="E41" s="114"/>
-      <c r="F41" s="114"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="74"/>
-      <c r="B42" s="77" t="s">
-        <v>103</v>
-      </c>
-      <c r="C42" s="83" t="s">
-        <v>251</v>
-      </c>
-      <c r="D42" s="72" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="79" t="s">
-        <v>82</v>
-      </c>
-      <c r="B43" s="80" t="s">
-        <v>243</v>
       </c>
       <c r="C43" s="81"/>
       <c r="D43" s="81"/>
       <c r="E43" s="114"/>
       <c r="F43" s="114"/>
     </row>
-    <row r="44" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="82"/>
-      <c r="B44" s="80" t="s">
-        <v>244</v>
-      </c>
-      <c r="C44" s="81"/>
-      <c r="D44" s="81"/>
-      <c r="E44" s="114"/>
-      <c r="F44" s="114"/>
-    </row>
-    <row r="45" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="82"/>
-      <c r="B45" s="84" t="s">
-        <v>207</v>
-      </c>
-      <c r="C45" s="86" t="s">
-        <v>217</v>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="74"/>
+      <c r="B44" s="77" t="s">
+        <v>103</v>
+      </c>
+      <c r="C44" s="83" t="s">
+        <v>251</v>
+      </c>
+      <c r="D44" s="72" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="74"/>
+      <c r="B45" s="77" t="s">
+        <v>353</v>
+      </c>
+      <c r="C45" s="83" t="s">
+        <v>354</v>
       </c>
       <c r="D45" s="72"/>
     </row>
     <row r="46" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="82"/>
-      <c r="B46" s="84" t="s">
-        <v>208</v>
-      </c>
-      <c r="C46" s="48" t="s">
-        <v>209</v>
-      </c>
-      <c r="D46" s="72" t="s">
-        <v>77</v>
-      </c>
+      <c r="A46" s="79" t="s">
+        <v>82</v>
+      </c>
+      <c r="B46" s="80" t="s">
+        <v>243</v>
+      </c>
+      <c r="C46" s="81"/>
+      <c r="D46" s="81"/>
+      <c r="E46" s="114"/>
+      <c r="F46" s="114"/>
     </row>
     <row r="47" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A47" s="82"/>
-      <c r="B47" s="84" t="s">
-        <v>170</v>
-      </c>
-      <c r="C47" s="85" t="s">
-        <v>216</v>
-      </c>
-      <c r="D47" s="72"/>
+      <c r="B47" s="80" t="s">
+        <v>244</v>
+      </c>
+      <c r="C47" s="81"/>
+      <c r="D47" s="81"/>
+      <c r="E47" s="114"/>
+      <c r="F47" s="114"/>
     </row>
     <row r="48" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A48" s="82"/>
-      <c r="B48" s="80" t="s">
-        <v>245</v>
-      </c>
-      <c r="C48" s="81"/>
-      <c r="D48" s="81"/>
-      <c r="E48" s="114"/>
-      <c r="F48" s="114"/>
+      <c r="B48" s="84" t="s">
+        <v>207</v>
+      </c>
+      <c r="C48" s="86" t="s">
+        <v>217</v>
+      </c>
+      <c r="D48" s="72"/>
     </row>
     <row r="49" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A49" s="82"/>
       <c r="B49" s="84" t="s">
-        <v>85</v>
-      </c>
-      <c r="C49" s="86" t="s">
-        <v>255</v>
+        <v>208</v>
+      </c>
+      <c r="C49" s="48" t="s">
+        <v>209</v>
       </c>
       <c r="D49" s="72" t="s">
         <v>77</v>
@@ -5863,156 +5881,152 @@
     <row r="50" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A50" s="82"/>
       <c r="B50" s="84" t="s">
-        <v>84</v>
-      </c>
-      <c r="C50" s="86" t="s">
-        <v>134</v>
-      </c>
-      <c r="D50" s="72" t="s">
-        <v>77</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="C50" s="85" t="s">
+        <v>216</v>
+      </c>
+      <c r="D50" s="72"/>
     </row>
     <row r="51" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A51" s="82"/>
-      <c r="B51" s="66" t="s">
-        <v>246</v>
-      </c>
-      <c r="C51" s="67"/>
-      <c r="D51" s="67"/>
-      <c r="E51" s="113"/>
-      <c r="F51" s="113"/>
+      <c r="B51" s="80" t="s">
+        <v>245</v>
+      </c>
+      <c r="C51" s="81"/>
+      <c r="D51" s="81"/>
+      <c r="E51" s="114"/>
+      <c r="F51" s="114"/>
     </row>
     <row r="52" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A52" s="82"/>
-      <c r="B52" s="71" t="s">
+      <c r="B52" s="84" t="s">
+        <v>85</v>
+      </c>
+      <c r="C52" s="86" t="s">
+        <v>255</v>
+      </c>
+      <c r="D52" s="72" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="82"/>
+      <c r="B53" s="84" t="s">
+        <v>84</v>
+      </c>
+      <c r="C53" s="86" t="s">
+        <v>134</v>
+      </c>
+      <c r="D53" s="72" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="82"/>
+      <c r="B54" s="66" t="s">
+        <v>246</v>
+      </c>
+      <c r="C54" s="67"/>
+      <c r="D54" s="67"/>
+      <c r="E54" s="113"/>
+      <c r="F54" s="113"/>
+    </row>
+    <row r="55" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="82"/>
+      <c r="B55" s="71" t="s">
         <v>86</v>
       </c>
-      <c r="C52" s="72" t="s">
+      <c r="C55" s="72" t="s">
         <v>135</v>
       </c>
-      <c r="D52" s="72" t="s">
+      <c r="D55" s="72" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="65" t="s">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="65" t="s">
         <v>83</v>
       </c>
-      <c r="B53" s="66" t="s">
+      <c r="B56" s="66" t="s">
         <v>247</v>
-      </c>
-      <c r="C53" s="67"/>
-      <c r="D53" s="67"/>
-      <c r="E53" s="113"/>
-      <c r="F53" s="113"/>
-    </row>
-    <row r="54" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="65"/>
-      <c r="B54" s="71" t="s">
-        <v>153</v>
-      </c>
-      <c r="C54" s="72" t="s">
-        <v>152</v>
-      </c>
-      <c r="D54" s="70"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B55" s="71" t="s">
-        <v>154</v>
-      </c>
-      <c r="C55" s="72" t="s">
-        <v>155</v>
-      </c>
-      <c r="D55" s="70"/>
-    </row>
-    <row r="56" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B56" s="66" t="s">
-        <v>248</v>
       </c>
       <c r="C56" s="67"/>
       <c r="D56" s="67"/>
-      <c r="E56" s="67"/>
-      <c r="F56" s="67"/>
+      <c r="E56" s="113"/>
+      <c r="F56" s="113"/>
     </row>
     <row r="57" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B57" s="54"/>
-      <c r="C57" s="55"/>
-      <c r="D57" s="55"/>
-      <c r="E57" s="55"/>
-      <c r="F57" s="55"/>
+      <c r="A57" s="65"/>
+      <c r="B57" s="71" t="s">
+        <v>153</v>
+      </c>
+      <c r="C57" s="72" t="s">
+        <v>152</v>
+      </c>
+      <c r="D57" s="70"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" s="51"/>
-      <c r="B58" s="122" t="s">
-        <v>325</v>
-      </c>
-      <c r="C58" s="67"/>
-      <c r="D58" s="67"/>
-      <c r="E58" s="113"/>
-      <c r="F58" s="113"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B59" s="71" t="s">
-        <v>326</v>
-      </c>
-      <c r="C59" s="72" t="s">
-        <v>327</v>
-      </c>
-      <c r="D59" s="70"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" s="51"/>
-      <c r="B60" s="122" t="s">
-        <v>266</v>
-      </c>
-      <c r="C60" s="67"/>
-      <c r="D60" s="67"/>
-      <c r="E60" s="113"/>
-      <c r="F60" s="113"/>
+      <c r="B58" s="71" t="s">
+        <v>154</v>
+      </c>
+      <c r="C58" s="72" t="s">
+        <v>155</v>
+      </c>
+      <c r="D58" s="70"/>
+    </row>
+    <row r="59" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B59" s="66" t="s">
+        <v>248</v>
+      </c>
+      <c r="C59" s="67"/>
+      <c r="D59" s="67"/>
+      <c r="E59" s="67"/>
+      <c r="F59" s="67"/>
+    </row>
+    <row r="60" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B60" s="54"/>
+      <c r="C60" s="55"/>
+      <c r="D60" s="55"/>
+      <c r="E60" s="55"/>
+      <c r="F60" s="55"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="51"/>
-      <c r="B61" s="123" t="s">
-        <v>262</v>
-      </c>
-      <c r="C61" s="105" t="s">
-        <v>269</v>
-      </c>
-      <c r="D61" s="55"/>
-      <c r="E61" s="64"/>
-      <c r="F61" s="64"/>
+      <c r="B61" s="122" t="s">
+        <v>325</v>
+      </c>
+      <c r="C61" s="67"/>
+      <c r="D61" s="67"/>
+      <c r="E61" s="113"/>
+      <c r="F61" s="113"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A62" s="51"/>
-      <c r="B62" s="123" t="s">
-        <v>265</v>
-      </c>
-      <c r="C62" s="105" t="s">
-        <v>270</v>
-      </c>
-      <c r="D62" s="55"/>
-      <c r="E62" s="64"/>
-      <c r="F62" s="64"/>
+      <c r="B62" s="71" t="s">
+        <v>326</v>
+      </c>
+      <c r="C62" s="72" t="s">
+        <v>327</v>
+      </c>
+      <c r="D62" s="70"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="51"/>
-      <c r="B63" s="123" t="s">
-        <v>261</v>
-      </c>
-      <c r="C63" s="105" t="s">
-        <v>271</v>
-      </c>
-      <c r="D63" s="55"/>
-      <c r="E63" s="64"/>
-      <c r="F63" s="64"/>
+      <c r="B63" s="122" t="s">
+        <v>266</v>
+      </c>
+      <c r="C63" s="67"/>
+      <c r="D63" s="67"/>
+      <c r="E63" s="113"/>
+      <c r="F63" s="113"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="51"/>
       <c r="B64" s="123" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C64" s="105" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D64" s="55"/>
       <c r="E64" s="64"/>
@@ -6021,10 +6035,10 @@
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="51"/>
       <c r="B65" s="123" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C65" s="105" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D65" s="55"/>
       <c r="E65" s="64"/>
@@ -6032,391 +6046,427 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="51"/>
-      <c r="B66" s="122" t="s">
-        <v>267</v>
-      </c>
-      <c r="C66" s="67"/>
-      <c r="D66" s="67"/>
-      <c r="E66" s="113"/>
-      <c r="F66" s="113"/>
+      <c r="B66" s="123" t="s">
+        <v>261</v>
+      </c>
+      <c r="C66" s="105" t="s">
+        <v>271</v>
+      </c>
+      <c r="D66" s="55"/>
+      <c r="E66" s="64"/>
+      <c r="F66" s="64"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="51"/>
       <c r="B67" s="123" t="s">
+        <v>263</v>
+      </c>
+      <c r="C67" s="105" t="s">
+        <v>272</v>
+      </c>
+      <c r="D67" s="55"/>
+      <c r="E67" s="64"/>
+      <c r="F67" s="64"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" s="51"/>
+      <c r="B68" s="123" t="s">
+        <v>264</v>
+      </c>
+      <c r="C68" s="105" t="s">
+        <v>273</v>
+      </c>
+      <c r="D68" s="55"/>
+      <c r="E68" s="64"/>
+      <c r="F68" s="64"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" s="51"/>
+      <c r="B69" s="122" t="s">
+        <v>267</v>
+      </c>
+      <c r="C69" s="67"/>
+      <c r="D69" s="67"/>
+      <c r="E69" s="113"/>
+      <c r="F69" s="113"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" s="51"/>
+      <c r="B70" s="123" t="s">
         <v>347</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C70" t="s">
         <v>348</v>
       </c>
-      <c r="D67"/>
-      <c r="E67"/>
-      <c r="F67"/>
-    </row>
-    <row r="68" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B68" s="123" t="s">
+      <c r="D70"/>
+      <c r="E70"/>
+      <c r="F70"/>
+    </row>
+    <row r="71" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B71" s="123" t="s">
         <v>268</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C71" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="69" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B69" s="122" t="s">
+    <row r="72" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B72" s="122" t="s">
         <v>281</v>
       </c>
-      <c r="C69" s="130"/>
-      <c r="D69" s="130"/>
-      <c r="E69" s="130"/>
-      <c r="F69" s="130"/>
-    </row>
-    <row r="70" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B70" s="132" t="s">
+      <c r="C72" s="130"/>
+      <c r="D72" s="130"/>
+      <c r="E72" s="130"/>
+      <c r="F72" s="130"/>
+    </row>
+    <row r="73" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B73" s="132" t="s">
         <v>313</v>
       </c>
-      <c r="C70" s="131" t="s">
+      <c r="C73" s="131" t="s">
         <v>282</v>
       </c>
-      <c r="D70" s="131"/>
-      <c r="E70" s="131"/>
-      <c r="F70" s="131"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A71" s="51"/>
-      <c r="B71" s="127" t="s">
+      <c r="D73" s="131"/>
+      <c r="E73" s="131"/>
+      <c r="F73" s="131"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" s="51"/>
+      <c r="B74" s="127" t="s">
         <v>249</v>
       </c>
-      <c r="C71" s="129"/>
-      <c r="D71" s="129"/>
-      <c r="E71" s="129"/>
-      <c r="F71" s="129"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72" s="51"/>
-      <c r="B72" s="88" t="s">
+      <c r="C74" s="129"/>
+      <c r="D74" s="129"/>
+      <c r="E74" s="129"/>
+      <c r="F74" s="129"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" s="51"/>
+      <c r="B75" s="88" t="s">
         <v>117</v>
       </c>
-      <c r="C72" s="89" t="s">
+      <c r="C75" s="89" t="s">
         <v>116</v>
       </c>
-      <c r="D72" s="88"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73" s="51"/>
-      <c r="B73" s="88" t="s">
+      <c r="D75" s="88"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" s="51"/>
+      <c r="B76" s="88" t="s">
         <v>314</v>
       </c>
-      <c r="C73" s="89" t="s">
+      <c r="C76" s="89" t="s">
         <v>315</v>
       </c>
-      <c r="D73" s="88"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74" s="52"/>
-      <c r="B74" s="88" t="s">
+      <c r="D76" s="88"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" s="52"/>
+      <c r="B77" s="88" t="s">
         <v>140</v>
       </c>
-      <c r="C74" s="89" t="s">
+      <c r="C77" s="89" t="s">
         <v>141</v>
       </c>
-      <c r="D74" s="88"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A75" s="52"/>
-      <c r="B75" s="88" t="s">
+      <c r="D77" s="88"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" s="52"/>
+      <c r="B78" s="88" t="s">
         <v>326</v>
       </c>
-      <c r="C75" s="89" t="s">
+      <c r="C78" s="89" t="s">
         <v>328</v>
       </c>
-      <c r="D75" s="88"/>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A76" s="87"/>
-      <c r="B76" s="69" t="s">
-        <v>111</v>
-      </c>
-      <c r="C76" s="64" t="s">
-        <v>115</v>
-      </c>
-      <c r="D76" s="64"/>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A77" s="87"/>
-      <c r="B77" s="142" t="s">
-        <v>316</v>
-      </c>
-      <c r="C77" s="119"/>
-      <c r="D77" s="119"/>
-      <c r="E77" s="119"/>
-      <c r="F77" s="119"/>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A78" s="87"/>
-      <c r="B78" s="71" t="s">
-        <v>119</v>
-      </c>
-      <c r="C78" s="72" t="s">
-        <v>158</v>
-      </c>
-      <c r="D78" s="72"/>
+      <c r="D78" s="88"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="87"/>
-      <c r="B79" s="71" t="s">
-        <v>318</v>
-      </c>
-      <c r="C79" s="72" t="s">
-        <v>317</v>
-      </c>
-      <c r="D79" s="72"/>
+      <c r="B79" s="69" t="s">
+        <v>111</v>
+      </c>
+      <c r="C79" s="64" t="s">
+        <v>115</v>
+      </c>
+      <c r="D79" s="64"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="87"/>
-      <c r="B80" s="71" t="s">
+      <c r="B80" s="142" t="s">
+        <v>316</v>
+      </c>
+      <c r="C80" s="119"/>
+      <c r="D80" s="119"/>
+      <c r="E80" s="119"/>
+      <c r="F80" s="119"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" s="87"/>
+      <c r="B81" s="71" t="s">
+        <v>119</v>
+      </c>
+      <c r="C81" s="72" t="s">
+        <v>158</v>
+      </c>
+      <c r="D81" s="72"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82" s="87"/>
+      <c r="B82" s="71" t="s">
+        <v>318</v>
+      </c>
+      <c r="C82" s="72" t="s">
+        <v>317</v>
+      </c>
+      <c r="D82" s="72"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83" s="87"/>
+      <c r="B83" s="71" t="s">
         <v>319</v>
       </c>
-      <c r="C80" s="72" t="s">
+      <c r="C83" s="72" t="s">
         <v>320</v>
       </c>
-      <c r="D80" s="72"/>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A81" s="119" t="s">
+      <c r="D83" s="72"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84" s="119" t="s">
         <v>250</v>
       </c>
-      <c r="B81" s="142" t="s">
+      <c r="B84" s="142" t="s">
         <v>321</v>
       </c>
-      <c r="C81" s="119"/>
-      <c r="D81" s="119"/>
-      <c r="E81" s="119"/>
-      <c r="F81" s="119"/>
-    </row>
-    <row r="82" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="90"/>
-      <c r="B82" s="71" t="s">
+      <c r="C84" s="119"/>
+      <c r="D84" s="119"/>
+      <c r="E84" s="119"/>
+      <c r="F84" s="119"/>
+    </row>
+    <row r="85" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="90"/>
+      <c r="B85" s="71" t="s">
         <v>38</v>
       </c>
-      <c r="C82" s="72" t="s">
+      <c r="C85" s="72" t="s">
         <v>163</v>
       </c>
-      <c r="D82" s="72"/>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A83" s="119" t="s">
+      <c r="D85" s="72"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86" s="119" t="s">
         <v>257</v>
       </c>
-      <c r="B83" s="71" t="s">
+      <c r="B86" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="C83" s="72" t="s">
+      <c r="C86" s="72" t="s">
         <v>157</v>
       </c>
-      <c r="D83" s="72"/>
-    </row>
-    <row r="84" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="90"/>
-      <c r="B84" s="71" t="s">
+      <c r="D86" s="72"/>
+    </row>
+    <row r="87" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="90"/>
+      <c r="B87" s="71" t="s">
         <v>200</v>
       </c>
-      <c r="C84" s="110" t="s">
+      <c r="C87" s="110" t="s">
         <v>201</v>
       </c>
-      <c r="D84" s="72"/>
-    </row>
-    <row r="85" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="91"/>
-      <c r="B85" s="71" t="s">
-        <v>203</v>
-      </c>
-      <c r="C85" s="110" t="s">
-        <v>204</v>
-      </c>
-      <c r="D85" s="72"/>
-    </row>
-    <row r="86" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="91"/>
-      <c r="B86" s="71" t="s">
-        <v>323</v>
-      </c>
-      <c r="C86" s="110" t="s">
-        <v>322</v>
-      </c>
-      <c r="D86" s="72"/>
-    </row>
-    <row r="87" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="91"/>
-      <c r="B87" s="142" t="s">
-        <v>324</v>
-      </c>
-      <c r="C87" s="119"/>
-      <c r="D87" s="119"/>
-      <c r="E87" s="119"/>
-      <c r="F87" s="119"/>
+      <c r="D87" s="72"/>
     </row>
     <row r="88" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A88" s="91"/>
-      <c r="B88" s="75" t="s">
+      <c r="B88" s="71" t="s">
+        <v>203</v>
+      </c>
+      <c r="C88" s="110" t="s">
+        <v>204</v>
+      </c>
+      <c r="D88" s="72"/>
+    </row>
+    <row r="89" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="91"/>
+      <c r="B89" s="71" t="s">
+        <v>323</v>
+      </c>
+      <c r="C89" s="110" t="s">
+        <v>322</v>
+      </c>
+      <c r="D89" s="72"/>
+    </row>
+    <row r="90" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="91"/>
+      <c r="B90" s="142" t="s">
+        <v>324</v>
+      </c>
+      <c r="C90" s="119"/>
+      <c r="D90" s="119"/>
+      <c r="E90" s="119"/>
+      <c r="F90" s="119"/>
+    </row>
+    <row r="91" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="91"/>
+      <c r="B91" s="75" t="s">
         <v>259</v>
-      </c>
-      <c r="C88" s="93"/>
-      <c r="D88" s="93"/>
-      <c r="E88" s="93"/>
-      <c r="F88" s="93"/>
-    </row>
-    <row r="89" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="119" t="s">
-        <v>258</v>
-      </c>
-      <c r="B89" s="84" t="s">
-        <v>90</v>
-      </c>
-      <c r="C89" s="72" t="s">
-        <v>160</v>
-      </c>
-      <c r="D89" s="72"/>
-    </row>
-    <row r="90" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="92"/>
-      <c r="B90" s="84" t="s">
-        <v>89</v>
-      </c>
-      <c r="C90" s="72" t="s">
-        <v>161</v>
-      </c>
-      <c r="D90" s="72"/>
-    </row>
-    <row r="91" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="94"/>
-      <c r="B91" s="75" t="s">
-        <v>260</v>
       </c>
       <c r="C91" s="93"/>
       <c r="D91" s="93"/>
       <c r="E91" s="93"/>
       <c r="F91" s="93"/>
     </row>
-    <row r="92" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="94"/>
-      <c r="B92" s="118" t="s">
-        <v>137</v>
+    <row r="92" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="119" t="s">
+        <v>258</v>
+      </c>
+      <c r="B92" s="84" t="s">
+        <v>90</v>
       </c>
       <c r="C92" s="72" t="s">
-        <v>138</v>
+        <v>160</v>
       </c>
       <c r="D92" s="72"/>
     </row>
     <row r="93" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A93" s="92"/>
-      <c r="B93" s="118" t="s">
-        <v>137</v>
+      <c r="B93" s="84" t="s">
+        <v>89</v>
       </c>
       <c r="C93" s="72" t="s">
-        <v>234</v>
+        <v>161</v>
       </c>
       <c r="D93" s="72"/>
     </row>
     <row r="94" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A94" s="94"/>
-      <c r="B94" s="118" t="s">
+      <c r="B94" s="75" t="s">
+        <v>260</v>
+      </c>
+      <c r="C94" s="93"/>
+      <c r="D94" s="93"/>
+      <c r="E94" s="93"/>
+      <c r="F94" s="93"/>
+    </row>
+    <row r="95" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="94"/>
+      <c r="B95" s="118" t="s">
+        <v>137</v>
+      </c>
+      <c r="C95" s="72" t="s">
+        <v>138</v>
+      </c>
+      <c r="D95" s="72"/>
+    </row>
+    <row r="96" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="92"/>
+      <c r="B96" s="118" t="s">
+        <v>137</v>
+      </c>
+      <c r="C96" s="72" t="s">
+        <v>234</v>
+      </c>
+      <c r="D96" s="72"/>
+    </row>
+    <row r="97" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="94"/>
+      <c r="B97" s="118" t="s">
         <v>192</v>
       </c>
-      <c r="C94" s="72" t="s">
+      <c r="C97" s="72" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="95" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B97" s="106" t="s">
+    <row r="98" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2"/>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B100" s="106" t="s">
         <v>193</v>
       </c>
-      <c r="C97" s="106" t="s">
+      <c r="C100" s="106" t="s">
         <v>197</v>
       </c>
-      <c r="D97" s="149" t="s">
+      <c r="D100" s="149" t="s">
         <v>198</v>
       </c>
-      <c r="E97" s="149"/>
-      <c r="F97" s="149"/>
-    </row>
-    <row r="98" spans="2:6" ht="127.5" x14ac:dyDescent="0.2">
-      <c r="B98" s="109" t="s">
+      <c r="E100" s="149"/>
+      <c r="F100" s="149"/>
+    </row>
+    <row r="101" spans="1:6" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="B101" s="109" t="s">
         <v>194</v>
       </c>
-      <c r="C98" s="108" t="s">
+      <c r="C101" s="108" t="s">
         <v>206</v>
       </c>
-      <c r="D98" s="150" t="s">
+      <c r="D101" s="150" t="s">
         <v>199</v>
       </c>
-      <c r="E98" s="150"/>
-      <c r="F98" s="150"/>
-    </row>
-    <row r="99" spans="2:6" ht="102" x14ac:dyDescent="0.2">
-      <c r="B99" s="109" t="s">
+      <c r="E101" s="150"/>
+      <c r="F101" s="150"/>
+    </row>
+    <row r="102" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+      <c r="B102" s="109" t="s">
         <v>195</v>
       </c>
-      <c r="C99" s="115" t="s">
+      <c r="C102" s="115" t="s">
         <v>205</v>
       </c>
-      <c r="D99" s="150" t="s">
+      <c r="D102" s="150" t="s">
         <v>202</v>
       </c>
-      <c r="E99" s="150"/>
-      <c r="F99" s="150"/>
-    </row>
-    <row r="100" spans="2:6" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="B100" s="109" t="s">
+      <c r="E102" s="150"/>
+      <c r="F102" s="150"/>
+    </row>
+    <row r="103" spans="1:6" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="B103" s="109" t="s">
         <v>196</v>
       </c>
-      <c r="C100" s="108" t="s">
+      <c r="C103" s="108" t="s">
         <v>210</v>
       </c>
-      <c r="D100" s="150" t="s">
+      <c r="D103" s="150" t="s">
         <v>211</v>
       </c>
-      <c r="E100" s="150"/>
-      <c r="F100" s="150"/>
-    </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B101" s="117"/>
-    </row>
-    <row r="102" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B102" s="116" t="s">
+      <c r="E103" s="150"/>
+      <c r="F103" s="150"/>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B104" s="117"/>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B105" s="116" t="s">
         <v>219</v>
       </c>
-      <c r="C102" s="116" t="s">
+      <c r="C105" s="116" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="103" spans="2:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="B103" s="117" t="s">
+    <row r="106" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="B106" s="117" t="s">
         <v>220</v>
       </c>
-      <c r="C103" s="108" t="s">
+      <c r="C106" s="108" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="104" spans="2:6" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="B104" s="117" t="s">
+    <row r="107" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="B107" s="117" t="s">
         <v>221</v>
       </c>
-      <c r="C104" s="108" t="s">
+      <c r="C107" s="108" t="s">
         <v>223</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
+    <mergeCell ref="D103:F103"/>
+    <mergeCell ref="D102:F102"/>
+    <mergeCell ref="D101:F101"/>
     <mergeCell ref="D100:F100"/>
-    <mergeCell ref="D99:F99"/>
-    <mergeCell ref="D98:F98"/>
-    <mergeCell ref="D97:F97"/>
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D98" r:id="rId1"/>
-    <hyperlink ref="D99" r:id="rId2"/>
-    <hyperlink ref="D100" r:id="rId3"/>
+    <hyperlink ref="D101" r:id="rId1"/>
+    <hyperlink ref="D102" r:id="rId2"/>
+    <hyperlink ref="D103" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>

</xml_diff>

<commit_message>
Actualizacion administracion de la configuracion
</commit_message>
<xml_diff>
--- a/Organización/Procesos/Soporte Organizacional/2. Administración de Configuración/IWM_Administración de la Configuración.xlsx
+++ b/Organización/Procesos/Soporte Organizacional/2. Administración de Configuración/IWM_Administración de la Configuración.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gus\Documents\IWM\CMMI\GitHUB\Organización\Procesos\Soporte Organizacional\2. Administración de Configuración\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\IWM\Repositorio IWM\Organización\Procesos\Soporte Organizacional\2. Administración de Configuración\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="353">
   <si>
     <t>Adapiaciones al Estándar de Administración de Datos</t>
   </si>
@@ -1442,12 +1442,6 @@
 -Drush Commands
 -Eclipse
 -Mantis</t>
-  </si>
-  <si>
-    <t>Checklist verificacion del manual de requerimientos</t>
-  </si>
-  <si>
-    <t>PTLL_Checklist_Manual_Requerimientos</t>
   </si>
   <si>
     <r>
@@ -4829,7 +4823,7 @@
         <v>136</v>
       </c>
       <c r="B15" s="70" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C15" s="70"/>
     </row>
@@ -5229,10 +5223,10 @@
     </row>
     <row r="55" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="132" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B55" s="131" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C55" s="131"/>
       <c r="D55" s="131"/>
@@ -5328,10 +5322,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I107"/>
+  <dimension ref="A1:I106"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B11" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+      <selection activeCell="B31" sqref="A31:XFD31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -5381,25 +5375,25 @@
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="49"/>
       <c r="B4" s="48" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C4" s="48" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="49"/>
       <c r="B5" s="48" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C5" s="48" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="49"/>
       <c r="B6" s="59" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C6" s="53"/>
       <c r="D6" s="53"/>
@@ -5412,22 +5406,22 @@
         <v>268</v>
       </c>
       <c r="C7" s="48" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="49"/>
       <c r="B8" s="48" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C8" s="48" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="49"/>
       <c r="B9" s="127" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C9" s="128"/>
       <c r="D9" s="128"/>
@@ -5437,17 +5431,17 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="49"/>
       <c r="B10" s="88" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C10" s="89" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D10" s="88"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="49"/>
       <c r="B11" s="127" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C11" s="128"/>
       <c r="D11" s="128"/>
@@ -5457,17 +5451,17 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="49"/>
       <c r="B12" s="88" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C12" s="89" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D12" s="88"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="62"/>
       <c r="B13" s="127" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C13" s="128"/>
       <c r="D13" s="128"/>
@@ -5480,10 +5474,10 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="63"/>
       <c r="B14" s="88" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C14" s="89" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D14" s="88"/>
     </row>
@@ -5602,10 +5596,10 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="63"/>
       <c r="B25" s="69" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C25" s="64" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D25" s="64" t="s">
         <v>77</v>
@@ -5614,10 +5608,10 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="63"/>
       <c r="B26" s="69" t="s">
+        <v>348</v>
+      </c>
+      <c r="C26" s="64" t="s">
         <v>350</v>
-      </c>
-      <c r="C26" s="64" t="s">
-        <v>352</v>
       </c>
       <c r="D26" s="64"/>
     </row>
@@ -5673,173 +5667,173 @@
     </row>
     <row r="31" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A31" s="68"/>
-      <c r="B31" s="69" t="s">
-        <v>310</v>
-      </c>
-      <c r="C31" s="64" t="s">
-        <v>311</v>
-      </c>
-      <c r="D31" s="64"/>
+      <c r="B31" s="71" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" s="72" t="s">
+        <v>118</v>
+      </c>
+      <c r="D31" s="70" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="32" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A32" s="68"/>
-      <c r="B32" s="71" t="s">
-        <v>91</v>
-      </c>
-      <c r="C32" s="72" t="s">
-        <v>118</v>
-      </c>
-      <c r="D32" s="70" t="s">
-        <v>159</v>
-      </c>
+      <c r="B32" s="66" t="s">
+        <v>238</v>
+      </c>
+      <c r="C32" s="67" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" s="67"/>
+      <c r="E32" s="113"/>
+      <c r="F32" s="113"/>
     </row>
     <row r="33" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A33" s="68"/>
-      <c r="B33" s="66" t="s">
-        <v>238</v>
-      </c>
-      <c r="C33" s="67" t="s">
-        <v>14</v>
-      </c>
-      <c r="D33" s="67"/>
-      <c r="E33" s="113"/>
-      <c r="F33" s="113"/>
-    </row>
-    <row r="34" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="68"/>
-      <c r="B34" s="75" t="s">
+      <c r="B33" s="75" t="s">
         <v>240</v>
       </c>
-      <c r="C34" s="76"/>
-      <c r="D34" s="76"/>
-      <c r="E34" s="114"/>
-      <c r="F34" s="114"/>
-    </row>
-    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="73" t="s">
+      <c r="C33" s="76"/>
+      <c r="D33" s="76"/>
+      <c r="E33" s="114"/>
+      <c r="F33" s="114"/>
+    </row>
+    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="73" t="s">
         <v>81</v>
       </c>
+      <c r="B34" s="77" t="s">
+        <v>136</v>
+      </c>
+      <c r="C34" s="70" t="s">
+        <v>252</v>
+      </c>
+      <c r="D34" s="70"/>
+    </row>
+    <row r="35" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="74"/>
       <c r="B35" s="77" t="s">
-        <v>136</v>
+        <v>78</v>
       </c>
       <c r="C35" s="70" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D35" s="70"/>
     </row>
     <row r="36" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A36" s="74"/>
       <c r="B36" s="77" t="s">
-        <v>78</v>
+        <v>101</v>
       </c>
       <c r="C36" s="70" t="s">
-        <v>253</v>
-      </c>
-      <c r="D36" s="70"/>
+        <v>114</v>
+      </c>
+      <c r="D36" s="70" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="37" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A37" s="74"/>
-      <c r="B37" s="77" t="s">
-        <v>101</v>
-      </c>
-      <c r="C37" s="70" t="s">
-        <v>114</v>
-      </c>
-      <c r="D37" s="70" t="s">
-        <v>159</v>
-      </c>
+      <c r="B37" s="75" t="s">
+        <v>239</v>
+      </c>
+      <c r="C37" s="76"/>
+      <c r="D37" s="76"/>
+      <c r="E37" s="114"/>
+      <c r="F37" s="114"/>
     </row>
     <row r="38" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A38" s="74"/>
-      <c r="B38" s="75" t="s">
-        <v>239</v>
-      </c>
-      <c r="C38" s="76"/>
-      <c r="D38" s="76"/>
-      <c r="E38" s="114"/>
-      <c r="F38" s="114"/>
+      <c r="B38" s="77" t="s">
+        <v>104</v>
+      </c>
+      <c r="C38" s="78" t="s">
+        <v>133</v>
+      </c>
+      <c r="D38" s="70" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="39" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A39" s="74"/>
       <c r="B39" s="77" t="s">
-        <v>104</v>
-      </c>
-      <c r="C39" s="78" t="s">
-        <v>133</v>
-      </c>
-      <c r="D39" s="70" t="s">
-        <v>159</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="C39" s="70" t="s">
+        <v>254</v>
+      </c>
+      <c r="D39" s="72"/>
+      <c r="E39" s="64"/>
     </row>
     <row r="40" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A40" s="74"/>
       <c r="B40" s="77" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C40" s="70" t="s">
-        <v>254</v>
+        <v>144</v>
       </c>
       <c r="D40" s="72"/>
-      <c r="E40" s="64"/>
     </row>
     <row r="41" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A41" s="74"/>
-      <c r="B41" s="77" t="s">
-        <v>143</v>
-      </c>
-      <c r="C41" s="70" t="s">
-        <v>144</v>
-      </c>
-      <c r="D41" s="72"/>
+      <c r="B41" s="66" t="s">
+        <v>241</v>
+      </c>
+      <c r="C41" s="67"/>
+      <c r="D41" s="67"/>
+      <c r="E41" s="113"/>
+      <c r="F41" s="113"/>
     </row>
     <row r="42" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A42" s="74"/>
-      <c r="B42" s="66" t="s">
-        <v>241</v>
-      </c>
-      <c r="C42" s="67"/>
-      <c r="D42" s="67"/>
-      <c r="E42" s="113"/>
-      <c r="F42" s="113"/>
-    </row>
-    <row r="43" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="80" t="s">
+        <v>242</v>
+      </c>
+      <c r="C42" s="81"/>
+      <c r="D42" s="81"/>
+      <c r="E42" s="114"/>
+      <c r="F42" s="114"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="74"/>
-      <c r="B43" s="80" t="s">
-        <v>242</v>
-      </c>
-      <c r="C43" s="81"/>
-      <c r="D43" s="81"/>
-      <c r="E43" s="114"/>
-      <c r="F43" s="114"/>
+      <c r="B43" s="77" t="s">
+        <v>103</v>
+      </c>
+      <c r="C43" s="83" t="s">
+        <v>251</v>
+      </c>
+      <c r="D43" s="72" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="74"/>
       <c r="B44" s="77" t="s">
-        <v>103</v>
+        <v>351</v>
       </c>
       <c r="C44" s="83" t="s">
-        <v>251</v>
-      </c>
-      <c r="D44" s="72" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="74"/>
-      <c r="B45" s="77" t="s">
-        <v>353</v>
-      </c>
-      <c r="C45" s="83" t="s">
-        <v>354</v>
-      </c>
-      <c r="D45" s="72"/>
+        <v>352</v>
+      </c>
+      <c r="D44" s="72"/>
+    </row>
+    <row r="45" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="79" t="s">
+        <v>82</v>
+      </c>
+      <c r="B45" s="80" t="s">
+        <v>243</v>
+      </c>
+      <c r="C45" s="81"/>
+      <c r="D45" s="81"/>
+      <c r="E45" s="114"/>
+      <c r="F45" s="114"/>
     </row>
     <row r="46" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="79" t="s">
-        <v>82</v>
-      </c>
+      <c r="A46" s="82"/>
       <c r="B46" s="80" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C46" s="81"/>
       <c r="D46" s="81"/>
@@ -5848,63 +5842,65 @@
     </row>
     <row r="47" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A47" s="82"/>
-      <c r="B47" s="80" t="s">
-        <v>244</v>
-      </c>
-      <c r="C47" s="81"/>
-      <c r="D47" s="81"/>
-      <c r="E47" s="114"/>
-      <c r="F47" s="114"/>
+      <c r="B47" s="84" t="s">
+        <v>207</v>
+      </c>
+      <c r="C47" s="86" t="s">
+        <v>217</v>
+      </c>
+      <c r="D47" s="72"/>
     </row>
     <row r="48" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A48" s="82"/>
       <c r="B48" s="84" t="s">
-        <v>207</v>
-      </c>
-      <c r="C48" s="86" t="s">
-        <v>217</v>
-      </c>
-      <c r="D48" s="72"/>
+        <v>208</v>
+      </c>
+      <c r="C48" s="48" t="s">
+        <v>209</v>
+      </c>
+      <c r="D48" s="72" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="49" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A49" s="82"/>
       <c r="B49" s="84" t="s">
-        <v>208</v>
-      </c>
-      <c r="C49" s="48" t="s">
-        <v>209</v>
-      </c>
-      <c r="D49" s="72" t="s">
-        <v>77</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="C49" s="85" t="s">
+        <v>216</v>
+      </c>
+      <c r="D49" s="72"/>
     </row>
     <row r="50" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A50" s="82"/>
-      <c r="B50" s="84" t="s">
-        <v>170</v>
-      </c>
-      <c r="C50" s="85" t="s">
-        <v>216</v>
-      </c>
-      <c r="D50" s="72"/>
+      <c r="B50" s="80" t="s">
+        <v>245</v>
+      </c>
+      <c r="C50" s="81"/>
+      <c r="D50" s="81"/>
+      <c r="E50" s="114"/>
+      <c r="F50" s="114"/>
     </row>
     <row r="51" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A51" s="82"/>
-      <c r="B51" s="80" t="s">
-        <v>245</v>
-      </c>
-      <c r="C51" s="81"/>
-      <c r="D51" s="81"/>
-      <c r="E51" s="114"/>
-      <c r="F51" s="114"/>
+      <c r="B51" s="84" t="s">
+        <v>85</v>
+      </c>
+      <c r="C51" s="86" t="s">
+        <v>255</v>
+      </c>
+      <c r="D51" s="72" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="52" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A52" s="82"/>
       <c r="B52" s="84" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C52" s="86" t="s">
-        <v>255</v>
+        <v>134</v>
       </c>
       <c r="D52" s="72" t="s">
         <v>77</v>
@@ -5912,121 +5908,121 @@
     </row>
     <row r="53" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A53" s="82"/>
-      <c r="B53" s="84" t="s">
-        <v>84</v>
-      </c>
-      <c r="C53" s="86" t="s">
-        <v>134</v>
-      </c>
-      <c r="D53" s="72" t="s">
-        <v>77</v>
-      </c>
+      <c r="B53" s="66" t="s">
+        <v>246</v>
+      </c>
+      <c r="C53" s="67"/>
+      <c r="D53" s="67"/>
+      <c r="E53" s="113"/>
+      <c r="F53" s="113"/>
     </row>
     <row r="54" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A54" s="82"/>
-      <c r="B54" s="66" t="s">
-        <v>246</v>
-      </c>
-      <c r="C54" s="67"/>
-      <c r="D54" s="67"/>
-      <c r="E54" s="113"/>
-      <c r="F54" s="113"/>
-    </row>
-    <row r="55" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="82"/>
-      <c r="B55" s="71" t="s">
+      <c r="B54" s="71" t="s">
         <v>86</v>
       </c>
-      <c r="C55" s="72" t="s">
+      <c r="C54" s="72" t="s">
         <v>135</v>
       </c>
-      <c r="D55" s="72" t="s">
+      <c r="D54" s="72" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" s="65" t="s">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="65" t="s">
         <v>83</v>
       </c>
-      <c r="B56" s="66" t="s">
+      <c r="B55" s="66" t="s">
         <v>247</v>
       </c>
-      <c r="C56" s="67"/>
-      <c r="D56" s="67"/>
-      <c r="E56" s="113"/>
-      <c r="F56" s="113"/>
-    </row>
-    <row r="57" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="65"/>
+      <c r="C55" s="67"/>
+      <c r="D55" s="67"/>
+      <c r="E55" s="113"/>
+      <c r="F55" s="113"/>
+    </row>
+    <row r="56" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="65"/>
+      <c r="B56" s="71" t="s">
+        <v>153</v>
+      </c>
+      <c r="C56" s="72" t="s">
+        <v>152</v>
+      </c>
+      <c r="D56" s="70"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B57" s="71" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C57" s="72" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="D57" s="70"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B58" s="71" t="s">
-        <v>154</v>
-      </c>
-      <c r="C58" s="72" t="s">
-        <v>155</v>
-      </c>
-      <c r="D58" s="70"/>
+    <row r="58" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B58" s="66" t="s">
+        <v>248</v>
+      </c>
+      <c r="C58" s="67"/>
+      <c r="D58" s="67"/>
+      <c r="E58" s="67"/>
+      <c r="F58" s="67"/>
     </row>
     <row r="59" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B59" s="66" t="s">
-        <v>248</v>
-      </c>
-      <c r="C59" s="67"/>
-      <c r="D59" s="67"/>
-      <c r="E59" s="67"/>
-      <c r="F59" s="67"/>
-    </row>
-    <row r="60" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B60" s="54"/>
-      <c r="C60" s="55"/>
-      <c r="D60" s="55"/>
-      <c r="E60" s="55"/>
-      <c r="F60" s="55"/>
+      <c r="B59" s="54"/>
+      <c r="C59" s="55"/>
+      <c r="D59" s="55"/>
+      <c r="E59" s="55"/>
+      <c r="F59" s="55"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" s="51"/>
+      <c r="B60" s="122" t="s">
+        <v>323</v>
+      </c>
+      <c r="C60" s="67"/>
+      <c r="D60" s="67"/>
+      <c r="E60" s="113"/>
+      <c r="F60" s="113"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" s="51"/>
-      <c r="B61" s="122" t="s">
+      <c r="B61" s="71" t="s">
+        <v>324</v>
+      </c>
+      <c r="C61" s="72" t="s">
         <v>325</v>
       </c>
-      <c r="C61" s="67"/>
-      <c r="D61" s="67"/>
-      <c r="E61" s="113"/>
-      <c r="F61" s="113"/>
+      <c r="D61" s="70"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B62" s="71" t="s">
-        <v>326</v>
-      </c>
-      <c r="C62" s="72" t="s">
-        <v>327</v>
-      </c>
-      <c r="D62" s="70"/>
+      <c r="A62" s="51"/>
+      <c r="B62" s="122" t="s">
+        <v>266</v>
+      </c>
+      <c r="C62" s="67"/>
+      <c r="D62" s="67"/>
+      <c r="E62" s="113"/>
+      <c r="F62" s="113"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="51"/>
-      <c r="B63" s="122" t="s">
-        <v>266</v>
-      </c>
-      <c r="C63" s="67"/>
-      <c r="D63" s="67"/>
-      <c r="E63" s="113"/>
-      <c r="F63" s="113"/>
+      <c r="B63" s="123" t="s">
+        <v>262</v>
+      </c>
+      <c r="C63" s="105" t="s">
+        <v>269</v>
+      </c>
+      <c r="D63" s="55"/>
+      <c r="E63" s="64"/>
+      <c r="F63" s="64"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="51"/>
       <c r="B64" s="123" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="C64" s="105" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D64" s="55"/>
       <c r="E64" s="64"/>
@@ -6035,10 +6031,10 @@
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="51"/>
       <c r="B65" s="123" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="C65" s="105" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D65" s="55"/>
       <c r="E65" s="64"/>
@@ -6047,10 +6043,10 @@
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="51"/>
       <c r="B66" s="123" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C66" s="105" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D66" s="55"/>
       <c r="E66" s="64"/>
@@ -6059,10 +6055,10 @@
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="51"/>
       <c r="B67" s="123" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C67" s="105" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D67" s="55"/>
       <c r="E67" s="64"/>
@@ -6070,403 +6066,391 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="51"/>
-      <c r="B68" s="123" t="s">
-        <v>264</v>
-      </c>
-      <c r="C68" s="105" t="s">
-        <v>273</v>
-      </c>
-      <c r="D68" s="55"/>
-      <c r="E68" s="64"/>
-      <c r="F68" s="64"/>
+      <c r="B68" s="122" t="s">
+        <v>267</v>
+      </c>
+      <c r="C68" s="67"/>
+      <c r="D68" s="67"/>
+      <c r="E68" s="113"/>
+      <c r="F68" s="113"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="51"/>
-      <c r="B69" s="122" t="s">
-        <v>267</v>
-      </c>
-      <c r="C69" s="67"/>
-      <c r="D69" s="67"/>
-      <c r="E69" s="113"/>
-      <c r="F69" s="113"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70" s="51"/>
+      <c r="B69" s="123" t="s">
+        <v>345</v>
+      </c>
+      <c r="C69" t="s">
+        <v>346</v>
+      </c>
+      <c r="D69"/>
+      <c r="E69"/>
+      <c r="F69"/>
+    </row>
+    <row r="70" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B70" s="123" t="s">
-        <v>347</v>
+        <v>268</v>
       </c>
       <c r="C70" t="s">
-        <v>348</v>
-      </c>
-      <c r="D70"/>
-      <c r="E70"/>
-      <c r="F70"/>
+        <v>274</v>
+      </c>
     </row>
     <row r="71" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B71" s="123" t="s">
-        <v>268</v>
-      </c>
-      <c r="C71" t="s">
-        <v>274</v>
-      </c>
+      <c r="B71" s="122" t="s">
+        <v>281</v>
+      </c>
+      <c r="C71" s="130"/>
+      <c r="D71" s="130"/>
+      <c r="E71" s="130"/>
+      <c r="F71" s="130"/>
     </row>
     <row r="72" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B72" s="122" t="s">
-        <v>281</v>
-      </c>
-      <c r="C72" s="130"/>
-      <c r="D72" s="130"/>
-      <c r="E72" s="130"/>
-      <c r="F72" s="130"/>
-    </row>
-    <row r="73" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B73" s="132" t="s">
-        <v>313</v>
-      </c>
-      <c r="C73" s="131" t="s">
+      <c r="B72" s="132" t="s">
+        <v>311</v>
+      </c>
+      <c r="C72" s="131" t="s">
         <v>282</v>
       </c>
-      <c r="D73" s="131"/>
-      <c r="E73" s="131"/>
-      <c r="F73" s="131"/>
+      <c r="D72" s="131"/>
+      <c r="E72" s="131"/>
+      <c r="F72" s="131"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" s="51"/>
+      <c r="B73" s="127" t="s">
+        <v>249</v>
+      </c>
+      <c r="C73" s="129"/>
+      <c r="D73" s="129"/>
+      <c r="E73" s="129"/>
+      <c r="F73" s="129"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="51"/>
-      <c r="B74" s="127" t="s">
-        <v>249</v>
-      </c>
-      <c r="C74" s="129"/>
-      <c r="D74" s="129"/>
-      <c r="E74" s="129"/>
-      <c r="F74" s="129"/>
+      <c r="B74" s="88" t="s">
+        <v>117</v>
+      </c>
+      <c r="C74" s="89" t="s">
+        <v>116</v>
+      </c>
+      <c r="D74" s="88"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="51"/>
       <c r="B75" s="88" t="s">
-        <v>117</v>
+        <v>312</v>
       </c>
       <c r="C75" s="89" t="s">
-        <v>116</v>
+        <v>313</v>
       </c>
       <c r="D75" s="88"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A76" s="51"/>
+      <c r="A76" s="52"/>
       <c r="B76" s="88" t="s">
-        <v>314</v>
+        <v>140</v>
       </c>
       <c r="C76" s="89" t="s">
-        <v>315</v>
+        <v>141</v>
       </c>
       <c r="D76" s="88"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="52"/>
       <c r="B77" s="88" t="s">
-        <v>140</v>
+        <v>324</v>
       </c>
       <c r="C77" s="89" t="s">
-        <v>141</v>
+        <v>326</v>
       </c>
       <c r="D77" s="88"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A78" s="52"/>
-      <c r="B78" s="88" t="s">
-        <v>326</v>
-      </c>
-      <c r="C78" s="89" t="s">
-        <v>328</v>
-      </c>
-      <c r="D78" s="88"/>
+      <c r="A78" s="87"/>
+      <c r="B78" s="69" t="s">
+        <v>111</v>
+      </c>
+      <c r="C78" s="64" t="s">
+        <v>115</v>
+      </c>
+      <c r="D78" s="64"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="87"/>
-      <c r="B79" s="69" t="s">
-        <v>111</v>
-      </c>
-      <c r="C79" s="64" t="s">
-        <v>115</v>
-      </c>
-      <c r="D79" s="64"/>
+      <c r="B79" s="142" t="s">
+        <v>314</v>
+      </c>
+      <c r="C79" s="119"/>
+      <c r="D79" s="119"/>
+      <c r="E79" s="119"/>
+      <c r="F79" s="119"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="87"/>
-      <c r="B80" s="142" t="s">
-        <v>316</v>
-      </c>
-      <c r="C80" s="119"/>
-      <c r="D80" s="119"/>
-      <c r="E80" s="119"/>
-      <c r="F80" s="119"/>
+      <c r="B80" s="71" t="s">
+        <v>119</v>
+      </c>
+      <c r="C80" s="72" t="s">
+        <v>158</v>
+      </c>
+      <c r="D80" s="72"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="87"/>
       <c r="B81" s="71" t="s">
-        <v>119</v>
+        <v>316</v>
       </c>
       <c r="C81" s="72" t="s">
-        <v>158</v>
+        <v>315</v>
       </c>
       <c r="D81" s="72"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="87"/>
       <c r="B82" s="71" t="s">
+        <v>317</v>
+      </c>
+      <c r="C82" s="72" t="s">
         <v>318</v>
       </c>
-      <c r="C82" s="72" t="s">
-        <v>317</v>
-      </c>
       <c r="D82" s="72"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A83" s="87"/>
-      <c r="B83" s="71" t="s">
+      <c r="A83" s="119" t="s">
+        <v>250</v>
+      </c>
+      <c r="B83" s="142" t="s">
         <v>319</v>
       </c>
-      <c r="C83" s="72" t="s">
-        <v>320</v>
-      </c>
-      <c r="D83" s="72"/>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A84" s="119" t="s">
-        <v>250</v>
-      </c>
-      <c r="B84" s="142" t="s">
-        <v>321</v>
-      </c>
-      <c r="C84" s="119"/>
-      <c r="D84" s="119"/>
-      <c r="E84" s="119"/>
-      <c r="F84" s="119"/>
-    </row>
-    <row r="85" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="90"/>
+      <c r="C83" s="119"/>
+      <c r="D83" s="119"/>
+      <c r="E83" s="119"/>
+      <c r="F83" s="119"/>
+    </row>
+    <row r="84" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="90"/>
+      <c r="B84" s="71" t="s">
+        <v>38</v>
+      </c>
+      <c r="C84" s="72" t="s">
+        <v>163</v>
+      </c>
+      <c r="D84" s="72"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A85" s="119" t="s">
+        <v>257</v>
+      </c>
       <c r="B85" s="71" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C85" s="72" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D85" s="72"/>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A86" s="119" t="s">
-        <v>257</v>
-      </c>
+    <row r="86" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="90"/>
       <c r="B86" s="71" t="s">
-        <v>32</v>
-      </c>
-      <c r="C86" s="72" t="s">
-        <v>157</v>
+        <v>200</v>
+      </c>
+      <c r="C86" s="110" t="s">
+        <v>201</v>
       </c>
       <c r="D86" s="72"/>
     </row>
     <row r="87" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="90"/>
+      <c r="A87" s="91"/>
       <c r="B87" s="71" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C87" s="110" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="D87" s="72"/>
     </row>
     <row r="88" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A88" s="91"/>
       <c r="B88" s="71" t="s">
-        <v>203</v>
+        <v>321</v>
       </c>
       <c r="C88" s="110" t="s">
-        <v>204</v>
+        <v>320</v>
       </c>
       <c r="D88" s="72"/>
     </row>
     <row r="89" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A89" s="91"/>
-      <c r="B89" s="71" t="s">
-        <v>323</v>
-      </c>
-      <c r="C89" s="110" t="s">
+      <c r="B89" s="142" t="s">
         <v>322</v>
       </c>
-      <c r="D89" s="72"/>
+      <c r="C89" s="119"/>
+      <c r="D89" s="119"/>
+      <c r="E89" s="119"/>
+      <c r="F89" s="119"/>
     </row>
     <row r="90" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A90" s="91"/>
-      <c r="B90" s="142" t="s">
-        <v>324</v>
-      </c>
-      <c r="C90" s="119"/>
-      <c r="D90" s="119"/>
-      <c r="E90" s="119"/>
-      <c r="F90" s="119"/>
-    </row>
-    <row r="91" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="91"/>
-      <c r="B91" s="75" t="s">
+      <c r="B90" s="75" t="s">
         <v>259</v>
       </c>
-      <c r="C91" s="93"/>
-      <c r="D91" s="93"/>
-      <c r="E91" s="93"/>
-      <c r="F91" s="93"/>
-    </row>
-    <row r="92" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="119" t="s">
+      <c r="C90" s="93"/>
+      <c r="D90" s="93"/>
+      <c r="E90" s="93"/>
+      <c r="F90" s="93"/>
+    </row>
+    <row r="91" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="119" t="s">
         <v>258</v>
       </c>
+      <c r="B91" s="84" t="s">
+        <v>90</v>
+      </c>
+      <c r="C91" s="72" t="s">
+        <v>160</v>
+      </c>
+      <c r="D91" s="72"/>
+    </row>
+    <row r="92" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="92"/>
       <c r="B92" s="84" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C92" s="72" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D92" s="72"/>
     </row>
     <row r="93" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="92"/>
-      <c r="B93" s="84" t="s">
-        <v>89</v>
-      </c>
-      <c r="C93" s="72" t="s">
-        <v>161</v>
-      </c>
-      <c r="D93" s="72"/>
+      <c r="A93" s="94"/>
+      <c r="B93" s="75" t="s">
+        <v>260</v>
+      </c>
+      <c r="C93" s="93"/>
+      <c r="D93" s="93"/>
+      <c r="E93" s="93"/>
+      <c r="F93" s="93"/>
     </row>
     <row r="94" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A94" s="94"/>
-      <c r="B94" s="75" t="s">
-        <v>260</v>
-      </c>
-      <c r="C94" s="93"/>
-      <c r="D94" s="93"/>
-      <c r="E94" s="93"/>
-      <c r="F94" s="93"/>
+      <c r="B94" s="118" t="s">
+        <v>137</v>
+      </c>
+      <c r="C94" s="72" t="s">
+        <v>138</v>
+      </c>
+      <c r="D94" s="72"/>
     </row>
     <row r="95" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="94"/>
+      <c r="A95" s="92"/>
       <c r="B95" s="118" t="s">
         <v>137</v>
       </c>
       <c r="C95" s="72" t="s">
-        <v>138</v>
+        <v>234</v>
       </c>
       <c r="D95" s="72"/>
     </row>
     <row r="96" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="92"/>
+      <c r="A96" s="94"/>
       <c r="B96" s="118" t="s">
-        <v>137</v>
+        <v>192</v>
       </c>
       <c r="C96" s="72" t="s">
-        <v>234</v>
-      </c>
-      <c r="D96" s="72"/>
-    </row>
-    <row r="97" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="94"/>
-      <c r="B97" s="118" t="s">
-        <v>192</v>
-      </c>
-      <c r="C97" s="72" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="98" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B100" s="106" t="s">
+    <row r="97" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.2"/>
+    <row r="99" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B99" s="106" t="s">
         <v>193</v>
       </c>
-      <c r="C100" s="106" t="s">
+      <c r="C99" s="106" t="s">
         <v>197</v>
       </c>
-      <c r="D100" s="149" t="s">
+      <c r="D99" s="149" t="s">
         <v>198</v>
       </c>
-      <c r="E100" s="149"/>
-      <c r="F100" s="149"/>
-    </row>
-    <row r="101" spans="1:6" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="E99" s="149"/>
+      <c r="F99" s="149"/>
+    </row>
+    <row r="100" spans="2:6" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="B100" s="109" t="s">
+        <v>194</v>
+      </c>
+      <c r="C100" s="108" t="s">
+        <v>206</v>
+      </c>
+      <c r="D100" s="150" t="s">
+        <v>199</v>
+      </c>
+      <c r="E100" s="150"/>
+      <c r="F100" s="150"/>
+    </row>
+    <row r="101" spans="2:6" ht="102" x14ac:dyDescent="0.2">
       <c r="B101" s="109" t="s">
-        <v>194</v>
-      </c>
-      <c r="C101" s="108" t="s">
-        <v>206</v>
+        <v>195</v>
+      </c>
+      <c r="C101" s="115" t="s">
+        <v>205</v>
       </c>
       <c r="D101" s="150" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="E101" s="150"/>
       <c r="F101" s="150"/>
     </row>
-    <row r="102" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:6" ht="89.25" x14ac:dyDescent="0.2">
       <c r="B102" s="109" t="s">
-        <v>195</v>
-      </c>
-      <c r="C102" s="115" t="s">
-        <v>205</v>
+        <v>196</v>
+      </c>
+      <c r="C102" s="108" t="s">
+        <v>210</v>
       </c>
       <c r="D102" s="150" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="E102" s="150"/>
       <c r="F102" s="150"/>
     </row>
-    <row r="103" spans="1:6" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="B103" s="109" t="s">
-        <v>196</v>
-      </c>
-      <c r="C103" s="108" t="s">
-        <v>210</v>
-      </c>
-      <c r="D103" s="150" t="s">
-        <v>211</v>
-      </c>
-      <c r="E103" s="150"/>
-      <c r="F103" s="150"/>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B104" s="117"/>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B105" s="116" t="s">
+    <row r="103" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B103" s="117"/>
+    </row>
+    <row r="104" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B104" s="116" t="s">
         <v>219</v>
       </c>
-      <c r="C105" s="116" t="s">
+      <c r="C104" s="116" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="B105" s="117" t="s">
+        <v>220</v>
+      </c>
+      <c r="C105" s="108" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="106" spans="2:6" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B106" s="117" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C106" s="108" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="B107" s="117" t="s">
-        <v>221</v>
-      </c>
-      <c r="C107" s="108" t="s">
         <v>223</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="D103:F103"/>
     <mergeCell ref="D102:F102"/>
     <mergeCell ref="D101:F101"/>
     <mergeCell ref="D100:F100"/>
+    <mergeCell ref="D99:F99"/>
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D101" r:id="rId1"/>
-    <hyperlink ref="D102" r:id="rId2"/>
-    <hyperlink ref="D103" r:id="rId3"/>
+    <hyperlink ref="D100" r:id="rId1"/>
+    <hyperlink ref="D101" r:id="rId2"/>
+    <hyperlink ref="D102" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>

</xml_diff>

<commit_message>
Se actualizo el acomodo y nombre de los archiovs en Mejora y Capacitación
</commit_message>
<xml_diff>
--- a/Organización/Procesos/Soporte Organizacional/2. Administración de Configuración/IWM_Administración de la Configuración.xlsx
+++ b/Organización/Procesos/Soporte Organizacional/2. Administración de Configuración/IWM_Administración de la Configuración.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\IWM\Repositorio IWM\Organización\Procesos\Soporte Organizacional\2. Administración de Configuración\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gus\Documents\IWM\CMMI\GitHUB\Organización\Procesos\Soporte Organizacional\2. Administración de Configuración\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="363">
   <si>
     <t>Adapiaciones al Estándar de Administración de Datos</t>
   </si>
@@ -1597,9 +1597,6 @@
     <t>Minuta de juntas</t>
   </si>
   <si>
-    <t>IWM_&lt;C/R&gt;_aammdd</t>
-  </si>
-  <si>
     <t>&lt;proyecto&gt;_Toma_Decision</t>
   </si>
   <si>
@@ -1643,12 +1640,6 @@
     <t>Solicitud Mejora</t>
   </si>
   <si>
-    <t>Solicitud_Mejora_mm_aaaa</t>
-  </si>
-  <si>
-    <t>IWM_Plan_Mejora_aaaa</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -1674,15 +1665,9 @@
     <t>Reporte de Actividades</t>
   </si>
   <si>
-    <t>Reporte_Actividades_aaaa</t>
-  </si>
-  <si>
     <t>Concentrado de Mejoras</t>
   </si>
   <si>
-    <t>Concentrado_Mejoras</t>
-  </si>
-  <si>
     <t>Solicitud de mejora</t>
   </si>
   <si>
@@ -1705,6 +1690,108 @@
   </si>
   <si>
     <t>PTLL_Verificacion_Analisis_y_Diseño</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="9"/>
+        <rFont val="Wingdings"/>
+        <charset val="2"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Capacitacion</t>
+    </r>
+  </si>
+  <si>
+    <t>Plan de capacitacion</t>
+  </si>
+  <si>
+    <t>Plan_Capacitacion_aaaa</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="9"/>
+        <rFont val="Wingdings"/>
+        <charset val="2"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Evaluaciónes</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="9"/>
+        <rFont val="Wingdings"/>
+        <charset val="2"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Lista de asistencia</t>
+    </r>
+  </si>
+  <si>
+    <t>Solicitud de Capacitación</t>
+  </si>
+  <si>
+    <t>Plan_Mejora_aaaa</t>
+  </si>
+  <si>
+    <t>Concentrado_Mejoras_aaaa</t>
+  </si>
+  <si>
+    <t>IWM_&lt;tipo de capacitación o proceso&gt;_aammdd</t>
+  </si>
+  <si>
+    <t>EC_&lt;tipo de capacitación o proceso&gt;_aammdd</t>
+  </si>
+  <si>
+    <t>LA_&lt;tipo de capacitación o proceso&gt;_aammdd</t>
+  </si>
+  <si>
+    <t>SC_&lt;tipo de capacitación o proceso&gt;_aammdd</t>
+  </si>
+  <si>
+    <t>M_&lt;tipo de capacitación o proceso&gt;_aammdd</t>
+  </si>
+  <si>
+    <t>SM_&lt;tipo de capacitación o proceso&gt;_aammdd</t>
+  </si>
+  <si>
+    <t>R_&lt;tipo de actividado&gt;_aammdd</t>
   </si>
 </sst>
 </file>
@@ -4823,7 +4910,7 @@
         <v>136</v>
       </c>
       <c r="B15" s="70" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C15" s="70"/>
     </row>
@@ -5226,7 +5313,7 @@
         <v>311</v>
       </c>
       <c r="B55" s="131" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C55" s="131"/>
       <c r="D55" s="131"/>
@@ -5322,10 +5409,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I106"/>
+  <dimension ref="A1:I116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B11" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B31" sqref="A31:XFD31"/>
+    <sheetView tabSelected="1" topLeftCell="C2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -5375,19 +5462,19 @@
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="49"/>
       <c r="B4" s="48" t="s">
+        <v>330</v>
+      </c>
+      <c r="C4" s="48" t="s">
         <v>331</v>
-      </c>
-      <c r="C4" s="48" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="49"/>
       <c r="B5" s="48" t="s">
+        <v>333</v>
+      </c>
+      <c r="C5" s="48" t="s">
         <v>334</v>
-      </c>
-      <c r="C5" s="48" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -5406,22 +5493,22 @@
         <v>268</v>
       </c>
       <c r="C7" s="48" t="s">
-        <v>339</v>
+        <v>354</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="49"/>
       <c r="B8" s="48" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="C8" s="48" t="s">
-        <v>344</v>
+        <v>355</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="49"/>
       <c r="B9" s="127" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C9" s="128"/>
       <c r="D9" s="128"/>
@@ -5431,17 +5518,17 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="49"/>
       <c r="B10" s="88" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C10" s="89" t="s">
-        <v>342</v>
+        <v>362</v>
       </c>
       <c r="D10" s="88"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="49"/>
       <c r="B11" s="127" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C11" s="128"/>
       <c r="D11" s="128"/>
@@ -5451,10 +5538,10 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="49"/>
       <c r="B12" s="88" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C12" s="89" t="s">
-        <v>338</v>
+        <v>361</v>
       </c>
       <c r="D12" s="88"/>
     </row>
@@ -5477,980 +5564,1082 @@
         <v>328</v>
       </c>
       <c r="C14" s="89" t="s">
-        <v>329</v>
+        <v>356</v>
       </c>
       <c r="D14" s="88"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="51"/>
-      <c r="B15" s="51"/>
-      <c r="C15" s="51"/>
-      <c r="D15" s="51"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="51"/>
-      <c r="I15" s="125" t="s">
-        <v>276</v>
-      </c>
+      <c r="A15" s="49"/>
+      <c r="B15" s="59" t="s">
+        <v>348</v>
+      </c>
+      <c r="C15" s="53"/>
+      <c r="D15" s="53"/>
+      <c r="E15" s="53"/>
+      <c r="F15" s="53"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="52"/>
-      <c r="B16" s="59" t="s">
-        <v>235</v>
-      </c>
-      <c r="C16" s="53"/>
-      <c r="D16" s="53"/>
-      <c r="E16" s="53"/>
-      <c r="F16" s="53"/>
+      <c r="A16" s="49"/>
+      <c r="B16" s="48" t="s">
+        <v>349</v>
+      </c>
+      <c r="C16" s="48" t="s">
+        <v>350</v>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B17" s="48" t="s">
-        <v>112</v>
-      </c>
-      <c r="C17" s="48" t="s">
-        <v>87</v>
-      </c>
-      <c r="H17" s="124"/>
-      <c r="I17" s="48" t="s">
-        <v>275</v>
-      </c>
+      <c r="A17" s="49"/>
+      <c r="B17" s="127" t="s">
+        <v>351</v>
+      </c>
+      <c r="C17" s="128"/>
+      <c r="D17" s="128"/>
+      <c r="E17" s="126"/>
+      <c r="F17" s="126"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H18" s="126"/>
-      <c r="I18" s="48" t="s">
-        <v>277</v>
-      </c>
+      <c r="A18" s="49"/>
+      <c r="B18" s="88" t="s">
+        <v>262</v>
+      </c>
+      <c r="C18" s="89" t="s">
+        <v>357</v>
+      </c>
+      <c r="D18" s="88"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="51"/>
-      <c r="B19" s="51"/>
-      <c r="C19" s="51"/>
-      <c r="D19" s="51"/>
-      <c r="E19" s="51"/>
-      <c r="F19" s="51"/>
-      <c r="H19" s="113"/>
-      <c r="I19" s="48" t="s">
-        <v>278</v>
-      </c>
+      <c r="A19" s="49"/>
+      <c r="B19" s="127" t="s">
+        <v>352</v>
+      </c>
+      <c r="C19" s="128"/>
+      <c r="D19" s="128"/>
+      <c r="E19" s="126"/>
+      <c r="F19" s="126"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="52"/>
-      <c r="B20" s="60" t="s">
-        <v>236</v>
-      </c>
-      <c r="C20" s="61"/>
-      <c r="D20" s="61"/>
-      <c r="E20" s="52"/>
-      <c r="F20" s="52"/>
-      <c r="H20" s="114"/>
-      <c r="I20" s="48" t="s">
-        <v>280</v>
-      </c>
+      <c r="A20" s="49"/>
+      <c r="B20" s="88" t="s">
+        <v>264</v>
+      </c>
+      <c r="C20" s="89" t="s">
+        <v>358</v>
+      </c>
+      <c r="D20" s="88"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="62"/>
+      <c r="A21" s="49"/>
       <c r="B21" s="127" t="s">
-        <v>256</v>
+        <v>335</v>
       </c>
       <c r="C21" s="128"/>
       <c r="D21" s="128"/>
       <c r="E21" s="126"/>
       <c r="F21" s="126"/>
-      <c r="I21" s="48" t="s">
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="49"/>
+      <c r="B22" s="88" t="s">
+        <v>353</v>
+      </c>
+      <c r="C22" s="89" t="s">
+        <v>359</v>
+      </c>
+      <c r="D22" s="88"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="62"/>
+      <c r="B23" s="127" t="s">
+        <v>327</v>
+      </c>
+      <c r="C23" s="128"/>
+      <c r="D23" s="128"/>
+      <c r="E23" s="126"/>
+      <c r="F23" s="126"/>
+      <c r="I23" s="48" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="63"/>
-      <c r="B22" s="121" t="s">
-        <v>64</v>
-      </c>
-      <c r="C22" s="121" t="s">
-        <v>14</v>
-      </c>
-      <c r="D22" s="121" t="s">
-        <v>58</v>
-      </c>
-      <c r="E22" s="120"/>
-      <c r="F22" s="120"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="63"/>
-      <c r="B23" s="88" t="s">
-        <v>42</v>
-      </c>
-      <c r="C23" s="89" t="s">
-        <v>144</v>
-      </c>
-      <c r="D23" s="88"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="63"/>
-      <c r="B24" s="66" t="s">
+      <c r="B24" s="88" t="s">
+        <v>328</v>
+      </c>
+      <c r="C24" s="89" t="s">
+        <v>360</v>
+      </c>
+      <c r="D24" s="88"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="51"/>
+      <c r="B25" s="51"/>
+      <c r="C25" s="51"/>
+      <c r="D25" s="51"/>
+      <c r="E25" s="51"/>
+      <c r="F25" s="51"/>
+      <c r="I25" s="125" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="52"/>
+      <c r="B26" s="59" t="s">
+        <v>235</v>
+      </c>
+      <c r="C26" s="53"/>
+      <c r="D26" s="53"/>
+      <c r="E26" s="53"/>
+      <c r="F26" s="53"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B27" s="48" t="s">
+        <v>112</v>
+      </c>
+      <c r="C27" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="H27" s="124"/>
+      <c r="I27" s="48" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H28" s="126"/>
+      <c r="I28" s="48" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="51"/>
+      <c r="B29" s="51"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="51"/>
+      <c r="F29" s="51"/>
+      <c r="H29" s="113"/>
+      <c r="I29" s="48" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="52"/>
+      <c r="B30" s="60" t="s">
+        <v>236</v>
+      </c>
+      <c r="C30" s="61"/>
+      <c r="D30" s="61"/>
+      <c r="E30" s="52"/>
+      <c r="F30" s="52"/>
+      <c r="H30" s="114"/>
+      <c r="I30" s="48" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="62"/>
+      <c r="B31" s="127" t="s">
+        <v>256</v>
+      </c>
+      <c r="C31" s="128"/>
+      <c r="D31" s="128"/>
+      <c r="E31" s="126"/>
+      <c r="F31" s="126"/>
+      <c r="I31" s="48" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="63"/>
+      <c r="B32" s="121" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" s="121" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" s="121" t="s">
+        <v>58</v>
+      </c>
+      <c r="E32" s="120"/>
+      <c r="F32" s="120"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="63"/>
+      <c r="B33" s="88" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" s="89" t="s">
+        <v>144</v>
+      </c>
+      <c r="D33" s="88"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="63"/>
+      <c r="B34" s="66" t="s">
         <v>237</v>
       </c>
-      <c r="C24" s="67"/>
-      <c r="D24" s="67"/>
-      <c r="E24" s="113"/>
-      <c r="F24" s="113"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="63"/>
-      <c r="B25" s="69" t="s">
-        <v>349</v>
-      </c>
-      <c r="C25" s="64" t="s">
-        <v>347</v>
-      </c>
-      <c r="D25" s="64" t="s">
+      <c r="C34" s="67"/>
+      <c r="D34" s="67"/>
+      <c r="E34" s="113"/>
+      <c r="F34" s="113"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="63"/>
+      <c r="B35" s="69" t="s">
+        <v>344</v>
+      </c>
+      <c r="C35" s="64" t="s">
+        <v>342</v>
+      </c>
+      <c r="D35" s="64" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="63"/>
-      <c r="B26" s="69" t="s">
-        <v>348</v>
-      </c>
-      <c r="C26" s="64" t="s">
-        <v>350</v>
-      </c>
-      <c r="D26" s="64"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="63"/>
-      <c r="B27" s="69" t="s">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="63"/>
+      <c r="B36" s="69" t="s">
+        <v>343</v>
+      </c>
+      <c r="C36" s="64" t="s">
+        <v>345</v>
+      </c>
+      <c r="D36" s="64"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="63"/>
+      <c r="B37" s="69" t="s">
         <v>76</v>
       </c>
-      <c r="C27" s="64" t="s">
+      <c r="C37" s="64" t="s">
         <v>131</v>
       </c>
-      <c r="D27" s="64" t="s">
+      <c r="D37" s="64" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="65" t="s">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="65" t="s">
         <v>80</v>
       </c>
-      <c r="B28" s="69" t="s">
+      <c r="B38" s="69" t="s">
         <v>102</v>
       </c>
-      <c r="C28" s="64" t="s">
+      <c r="C38" s="64" t="s">
         <v>130</v>
-      </c>
-      <c r="D28" s="70" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="68"/>
-      <c r="B29" s="69" t="s">
-        <v>99</v>
-      </c>
-      <c r="C29" s="64" t="s">
-        <v>113</v>
-      </c>
-      <c r="D29" s="70" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="68"/>
-      <c r="B30" s="69" t="s">
-        <v>100</v>
-      </c>
-      <c r="C30" s="64" t="s">
-        <v>132</v>
-      </c>
-      <c r="D30" s="64" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="68"/>
-      <c r="B31" s="71" t="s">
-        <v>91</v>
-      </c>
-      <c r="C31" s="72" t="s">
-        <v>118</v>
-      </c>
-      <c r="D31" s="70" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="68"/>
-      <c r="B32" s="66" t="s">
-        <v>238</v>
-      </c>
-      <c r="C32" s="67" t="s">
-        <v>14</v>
-      </c>
-      <c r="D32" s="67"/>
-      <c r="E32" s="113"/>
-      <c r="F32" s="113"/>
-    </row>
-    <row r="33" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="68"/>
-      <c r="B33" s="75" t="s">
-        <v>240</v>
-      </c>
-      <c r="C33" s="76"/>
-      <c r="D33" s="76"/>
-      <c r="E33" s="114"/>
-      <c r="F33" s="114"/>
-    </row>
-    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="73" t="s">
-        <v>81</v>
-      </c>
-      <c r="B34" s="77" t="s">
-        <v>136</v>
-      </c>
-      <c r="C34" s="70" t="s">
-        <v>252</v>
-      </c>
-      <c r="D34" s="70"/>
-    </row>
-    <row r="35" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="74"/>
-      <c r="B35" s="77" t="s">
-        <v>78</v>
-      </c>
-      <c r="C35" s="70" t="s">
-        <v>253</v>
-      </c>
-      <c r="D35" s="70"/>
-    </row>
-    <row r="36" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="74"/>
-      <c r="B36" s="77" t="s">
-        <v>101</v>
-      </c>
-      <c r="C36" s="70" t="s">
-        <v>114</v>
-      </c>
-      <c r="D36" s="70" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="74"/>
-      <c r="B37" s="75" t="s">
-        <v>239</v>
-      </c>
-      <c r="C37" s="76"/>
-      <c r="D37" s="76"/>
-      <c r="E37" s="114"/>
-      <c r="F37" s="114"/>
-    </row>
-    <row r="38" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="74"/>
-      <c r="B38" s="77" t="s">
-        <v>104</v>
-      </c>
-      <c r="C38" s="78" t="s">
-        <v>133</v>
       </c>
       <c r="D38" s="70" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="39" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="74"/>
-      <c r="B39" s="77" t="s">
+      <c r="A39" s="68"/>
+      <c r="B39" s="69" t="s">
+        <v>99</v>
+      </c>
+      <c r="C39" s="64" t="s">
+        <v>113</v>
+      </c>
+      <c r="D39" s="70" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="68"/>
+      <c r="B40" s="69" t="s">
+        <v>100</v>
+      </c>
+      <c r="C40" s="64" t="s">
+        <v>132</v>
+      </c>
+      <c r="D40" s="64" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="68"/>
+      <c r="B41" s="71" t="s">
+        <v>91</v>
+      </c>
+      <c r="C41" s="72" t="s">
+        <v>118</v>
+      </c>
+      <c r="D41" s="70" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="68"/>
+      <c r="B42" s="66" t="s">
+        <v>238</v>
+      </c>
+      <c r="C42" s="67" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" s="67"/>
+      <c r="E42" s="113"/>
+      <c r="F42" s="113"/>
+    </row>
+    <row r="43" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="68"/>
+      <c r="B43" s="75" t="s">
+        <v>240</v>
+      </c>
+      <c r="C43" s="76"/>
+      <c r="D43" s="76"/>
+      <c r="E43" s="114"/>
+      <c r="F43" s="114"/>
+    </row>
+    <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="73" t="s">
+        <v>81</v>
+      </c>
+      <c r="B44" s="77" t="s">
+        <v>136</v>
+      </c>
+      <c r="C44" s="70" t="s">
+        <v>252</v>
+      </c>
+      <c r="D44" s="70"/>
+    </row>
+    <row r="45" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="74"/>
+      <c r="B45" s="77" t="s">
+        <v>78</v>
+      </c>
+      <c r="C45" s="70" t="s">
+        <v>253</v>
+      </c>
+      <c r="D45" s="70"/>
+    </row>
+    <row r="46" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="74"/>
+      <c r="B46" s="77" t="s">
+        <v>101</v>
+      </c>
+      <c r="C46" s="70" t="s">
+        <v>114</v>
+      </c>
+      <c r="D46" s="70" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="74"/>
+      <c r="B47" s="75" t="s">
+        <v>239</v>
+      </c>
+      <c r="C47" s="76"/>
+      <c r="D47" s="76"/>
+      <c r="E47" s="114"/>
+      <c r="F47" s="114"/>
+    </row>
+    <row r="48" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="74"/>
+      <c r="B48" s="77" t="s">
+        <v>104</v>
+      </c>
+      <c r="C48" s="78" t="s">
+        <v>133</v>
+      </c>
+      <c r="D48" s="70" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="74"/>
+      <c r="B49" s="77" t="s">
         <v>142</v>
       </c>
-      <c r="C39" s="70" t="s">
+      <c r="C49" s="70" t="s">
         <v>254</v>
       </c>
-      <c r="D39" s="72"/>
-      <c r="E39" s="64"/>
-    </row>
-    <row r="40" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="74"/>
-      <c r="B40" s="77" t="s">
+      <c r="D49" s="72"/>
+      <c r="E49" s="64"/>
+    </row>
+    <row r="50" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="74"/>
+      <c r="B50" s="77" t="s">
         <v>143</v>
       </c>
-      <c r="C40" s="70" t="s">
+      <c r="C50" s="70" t="s">
         <v>144</v>
       </c>
-      <c r="D40" s="72"/>
-    </row>
-    <row r="41" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="74"/>
-      <c r="B41" s="66" t="s">
+      <c r="D50" s="72"/>
+    </row>
+    <row r="51" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="74"/>
+      <c r="B51" s="66" t="s">
         <v>241</v>
       </c>
-      <c r="C41" s="67"/>
-      <c r="D41" s="67"/>
-      <c r="E41" s="113"/>
-      <c r="F41" s="113"/>
-    </row>
-    <row r="42" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="74"/>
-      <c r="B42" s="80" t="s">
+      <c r="C51" s="67"/>
+      <c r="D51" s="67"/>
+      <c r="E51" s="113"/>
+      <c r="F51" s="113"/>
+    </row>
+    <row r="52" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="74"/>
+      <c r="B52" s="80" t="s">
         <v>242</v>
       </c>
-      <c r="C42" s="81"/>
-      <c r="D42" s="81"/>
-      <c r="E42" s="114"/>
-      <c r="F42" s="114"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="74"/>
-      <c r="B43" s="77" t="s">
+      <c r="C52" s="81"/>
+      <c r="D52" s="81"/>
+      <c r="E52" s="114"/>
+      <c r="F52" s="114"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="74"/>
+      <c r="B53" s="77" t="s">
         <v>103</v>
       </c>
-      <c r="C43" s="83" t="s">
+      <c r="C53" s="83" t="s">
         <v>251</v>
       </c>
-      <c r="D43" s="72" t="s">
+      <c r="D53" s="72" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="74"/>
-      <c r="B44" s="77" t="s">
-        <v>351</v>
-      </c>
-      <c r="C44" s="83" t="s">
-        <v>352</v>
-      </c>
-      <c r="D44" s="72"/>
-    </row>
-    <row r="45" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="79" t="s">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="74"/>
+      <c r="B54" s="77" t="s">
+        <v>346</v>
+      </c>
+      <c r="C54" s="83" t="s">
+        <v>347</v>
+      </c>
+      <c r="D54" s="72"/>
+    </row>
+    <row r="55" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="79" t="s">
         <v>82</v>
       </c>
-      <c r="B45" s="80" t="s">
+      <c r="B55" s="80" t="s">
         <v>243</v>
       </c>
-      <c r="C45" s="81"/>
-      <c r="D45" s="81"/>
-      <c r="E45" s="114"/>
-      <c r="F45" s="114"/>
-    </row>
-    <row r="46" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="82"/>
-      <c r="B46" s="80" t="s">
+      <c r="C55" s="81"/>
+      <c r="D55" s="81"/>
+      <c r="E55" s="114"/>
+      <c r="F55" s="114"/>
+    </row>
+    <row r="56" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="82"/>
+      <c r="B56" s="80" t="s">
         <v>244</v>
       </c>
-      <c r="C46" s="81"/>
-      <c r="D46" s="81"/>
-      <c r="E46" s="114"/>
-      <c r="F46" s="114"/>
-    </row>
-    <row r="47" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="82"/>
-      <c r="B47" s="84" t="s">
+      <c r="C56" s="81"/>
+      <c r="D56" s="81"/>
+      <c r="E56" s="114"/>
+      <c r="F56" s="114"/>
+    </row>
+    <row r="57" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="82"/>
+      <c r="B57" s="84" t="s">
         <v>207</v>
       </c>
-      <c r="C47" s="86" t="s">
+      <c r="C57" s="86" t="s">
         <v>217</v>
       </c>
-      <c r="D47" s="72"/>
-    </row>
-    <row r="48" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="82"/>
-      <c r="B48" s="84" t="s">
+      <c r="D57" s="72"/>
+    </row>
+    <row r="58" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="82"/>
+      <c r="B58" s="84" t="s">
         <v>208</v>
       </c>
-      <c r="C48" s="48" t="s">
+      <c r="C58" s="48" t="s">
         <v>209</v>
       </c>
-      <c r="D48" s="72" t="s">
+      <c r="D58" s="72" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="49" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="82"/>
-      <c r="B49" s="84" t="s">
+    <row r="59" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="82"/>
+      <c r="B59" s="84" t="s">
         <v>170</v>
       </c>
-      <c r="C49" s="85" t="s">
+      <c r="C59" s="85" t="s">
         <v>216</v>
       </c>
-      <c r="D49" s="72"/>
-    </row>
-    <row r="50" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="82"/>
-      <c r="B50" s="80" t="s">
+      <c r="D59" s="72"/>
+    </row>
+    <row r="60" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="82"/>
+      <c r="B60" s="80" t="s">
         <v>245</v>
       </c>
-      <c r="C50" s="81"/>
-      <c r="D50" s="81"/>
-      <c r="E50" s="114"/>
-      <c r="F50" s="114"/>
-    </row>
-    <row r="51" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="82"/>
-      <c r="B51" s="84" t="s">
+      <c r="C60" s="81"/>
+      <c r="D60" s="81"/>
+      <c r="E60" s="114"/>
+      <c r="F60" s="114"/>
+    </row>
+    <row r="61" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="82"/>
+      <c r="B61" s="84" t="s">
         <v>85</v>
       </c>
-      <c r="C51" s="86" t="s">
+      <c r="C61" s="86" t="s">
         <v>255</v>
       </c>
-      <c r="D51" s="72" t="s">
+      <c r="D61" s="72" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="52" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="82"/>
-      <c r="B52" s="84" t="s">
+    <row r="62" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="82"/>
+      <c r="B62" s="84" t="s">
         <v>84</v>
       </c>
-      <c r="C52" s="86" t="s">
+      <c r="C62" s="86" t="s">
         <v>134</v>
       </c>
-      <c r="D52" s="72" t="s">
+      <c r="D62" s="72" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="53" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="82"/>
-      <c r="B53" s="66" t="s">
+    <row r="63" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="82"/>
+      <c r="B63" s="66" t="s">
         <v>246</v>
       </c>
-      <c r="C53" s="67"/>
-      <c r="D53" s="67"/>
-      <c r="E53" s="113"/>
-      <c r="F53" s="113"/>
-    </row>
-    <row r="54" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="82"/>
-      <c r="B54" s="71" t="s">
+      <c r="C63" s="67"/>
+      <c r="D63" s="67"/>
+      <c r="E63" s="113"/>
+      <c r="F63" s="113"/>
+    </row>
+    <row r="64" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="82"/>
+      <c r="B64" s="71" t="s">
         <v>86</v>
       </c>
-      <c r="C54" s="72" t="s">
+      <c r="C64" s="72" t="s">
         <v>135</v>
       </c>
-      <c r="D54" s="72" t="s">
+      <c r="D64" s="72" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" s="65" t="s">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" s="65" t="s">
         <v>83</v>
       </c>
-      <c r="B55" s="66" t="s">
+      <c r="B65" s="66" t="s">
         <v>247</v>
       </c>
-      <c r="C55" s="67"/>
-      <c r="D55" s="67"/>
-      <c r="E55" s="113"/>
-      <c r="F55" s="113"/>
-    </row>
-    <row r="56" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="65"/>
-      <c r="B56" s="71" t="s">
+      <c r="C65" s="67"/>
+      <c r="D65" s="67"/>
+      <c r="E65" s="113"/>
+      <c r="F65" s="113"/>
+    </row>
+    <row r="66" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="65"/>
+      <c r="B66" s="71" t="s">
         <v>153</v>
       </c>
-      <c r="C56" s="72" t="s">
+      <c r="C66" s="72" t="s">
         <v>152</v>
       </c>
-      <c r="D56" s="70"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B57" s="71" t="s">
+      <c r="D66" s="70"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B67" s="71" t="s">
         <v>154</v>
       </c>
-      <c r="C57" s="72" t="s">
+      <c r="C67" s="72" t="s">
         <v>155</v>
       </c>
-      <c r="D57" s="70"/>
-    </row>
-    <row r="58" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B58" s="66" t="s">
+      <c r="D67" s="70"/>
+    </row>
+    <row r="68" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B68" s="66" t="s">
         <v>248</v>
-      </c>
-      <c r="C58" s="67"/>
-      <c r="D58" s="67"/>
-      <c r="E58" s="67"/>
-      <c r="F58" s="67"/>
-    </row>
-    <row r="59" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B59" s="54"/>
-      <c r="C59" s="55"/>
-      <c r="D59" s="55"/>
-      <c r="E59" s="55"/>
-      <c r="F59" s="55"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" s="51"/>
-      <c r="B60" s="122" t="s">
-        <v>323</v>
-      </c>
-      <c r="C60" s="67"/>
-      <c r="D60" s="67"/>
-      <c r="E60" s="113"/>
-      <c r="F60" s="113"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B61" s="71" t="s">
-        <v>324</v>
-      </c>
-      <c r="C61" s="72" t="s">
-        <v>325</v>
-      </c>
-      <c r="D61" s="70"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A62" s="51"/>
-      <c r="B62" s="122" t="s">
-        <v>266</v>
-      </c>
-      <c r="C62" s="67"/>
-      <c r="D62" s="67"/>
-      <c r="E62" s="113"/>
-      <c r="F62" s="113"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" s="51"/>
-      <c r="B63" s="123" t="s">
-        <v>262</v>
-      </c>
-      <c r="C63" s="105" t="s">
-        <v>269</v>
-      </c>
-      <c r="D63" s="55"/>
-      <c r="E63" s="64"/>
-      <c r="F63" s="64"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A64" s="51"/>
-      <c r="B64" s="123" t="s">
-        <v>265</v>
-      </c>
-      <c r="C64" s="105" t="s">
-        <v>270</v>
-      </c>
-      <c r="D64" s="55"/>
-      <c r="E64" s="64"/>
-      <c r="F64" s="64"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" s="51"/>
-      <c r="B65" s="123" t="s">
-        <v>261</v>
-      </c>
-      <c r="C65" s="105" t="s">
-        <v>271</v>
-      </c>
-      <c r="D65" s="55"/>
-      <c r="E65" s="64"/>
-      <c r="F65" s="64"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66" s="51"/>
-      <c r="B66" s="123" t="s">
-        <v>263</v>
-      </c>
-      <c r="C66" s="105" t="s">
-        <v>272</v>
-      </c>
-      <c r="D66" s="55"/>
-      <c r="E66" s="64"/>
-      <c r="F66" s="64"/>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" s="51"/>
-      <c r="B67" s="123" t="s">
-        <v>264</v>
-      </c>
-      <c r="C67" s="105" t="s">
-        <v>273</v>
-      </c>
-      <c r="D67" s="55"/>
-      <c r="E67" s="64"/>
-      <c r="F67" s="64"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68" s="51"/>
-      <c r="B68" s="122" t="s">
-        <v>267</v>
       </c>
       <c r="C68" s="67"/>
       <c r="D68" s="67"/>
-      <c r="E68" s="113"/>
-      <c r="F68" s="113"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69" s="51"/>
-      <c r="B69" s="123" t="s">
-        <v>345</v>
-      </c>
-      <c r="C69" t="s">
-        <v>346</v>
-      </c>
-      <c r="D69"/>
-      <c r="E69"/>
-      <c r="F69"/>
-    </row>
-    <row r="70" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B70" s="123" t="s">
-        <v>268</v>
-      </c>
-      <c r="C70" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B71" s="122" t="s">
-        <v>281</v>
-      </c>
-      <c r="C71" s="130"/>
-      <c r="D71" s="130"/>
-      <c r="E71" s="130"/>
-      <c r="F71" s="130"/>
-    </row>
-    <row r="72" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B72" s="132" t="s">
-        <v>311</v>
-      </c>
-      <c r="C72" s="131" t="s">
-        <v>282</v>
-      </c>
-      <c r="D72" s="131"/>
-      <c r="E72" s="131"/>
-      <c r="F72" s="131"/>
+      <c r="E68" s="67"/>
+      <c r="F68" s="67"/>
+    </row>
+    <row r="69" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B69" s="54"/>
+      <c r="C69" s="55"/>
+      <c r="D69" s="55"/>
+      <c r="E69" s="55"/>
+      <c r="F69" s="55"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" s="51"/>
+      <c r="B70" s="122" t="s">
+        <v>323</v>
+      </c>
+      <c r="C70" s="67"/>
+      <c r="D70" s="67"/>
+      <c r="E70" s="113"/>
+      <c r="F70" s="113"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B71" s="71" t="s">
+        <v>324</v>
+      </c>
+      <c r="C71" s="72" t="s">
+        <v>325</v>
+      </c>
+      <c r="D71" s="70"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" s="51"/>
+      <c r="B72" s="122" t="s">
+        <v>266</v>
+      </c>
+      <c r="C72" s="67"/>
+      <c r="D72" s="67"/>
+      <c r="E72" s="113"/>
+      <c r="F72" s="113"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="51"/>
-      <c r="B73" s="127" t="s">
-        <v>249</v>
-      </c>
-      <c r="C73" s="129"/>
-      <c r="D73" s="129"/>
-      <c r="E73" s="129"/>
-      <c r="F73" s="129"/>
+      <c r="B73" s="123" t="s">
+        <v>262</v>
+      </c>
+      <c r="C73" s="105" t="s">
+        <v>269</v>
+      </c>
+      <c r="D73" s="55"/>
+      <c r="E73" s="64"/>
+      <c r="F73" s="64"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="51"/>
-      <c r="B74" s="88" t="s">
-        <v>117</v>
-      </c>
-      <c r="C74" s="89" t="s">
-        <v>116</v>
-      </c>
-      <c r="D74" s="88"/>
+      <c r="B74" s="123" t="s">
+        <v>265</v>
+      </c>
+      <c r="C74" s="105" t="s">
+        <v>270</v>
+      </c>
+      <c r="D74" s="55"/>
+      <c r="E74" s="64"/>
+      <c r="F74" s="64"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="51"/>
-      <c r="B75" s="88" t="s">
+      <c r="B75" s="123" t="s">
+        <v>261</v>
+      </c>
+      <c r="C75" s="105" t="s">
+        <v>271</v>
+      </c>
+      <c r="D75" s="55"/>
+      <c r="E75" s="64"/>
+      <c r="F75" s="64"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" s="51"/>
+      <c r="B76" s="123" t="s">
+        <v>263</v>
+      </c>
+      <c r="C76" s="105" t="s">
+        <v>272</v>
+      </c>
+      <c r="D76" s="55"/>
+      <c r="E76" s="64"/>
+      <c r="F76" s="64"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" s="51"/>
+      <c r="B77" s="123" t="s">
+        <v>264</v>
+      </c>
+      <c r="C77" s="105" t="s">
+        <v>273</v>
+      </c>
+      <c r="D77" s="55"/>
+      <c r="E77" s="64"/>
+      <c r="F77" s="64"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" s="51"/>
+      <c r="B78" s="122" t="s">
+        <v>267</v>
+      </c>
+      <c r="C78" s="67"/>
+      <c r="D78" s="67"/>
+      <c r="E78" s="113"/>
+      <c r="F78" s="113"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79" s="51"/>
+      <c r="B79" s="123" t="s">
+        <v>340</v>
+      </c>
+      <c r="C79" t="s">
+        <v>341</v>
+      </c>
+      <c r="D79"/>
+      <c r="E79"/>
+      <c r="F79"/>
+    </row>
+    <row r="80" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B80" s="123" t="s">
+        <v>268</v>
+      </c>
+      <c r="C80" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B81" s="122" t="s">
+        <v>281</v>
+      </c>
+      <c r="C81" s="130"/>
+      <c r="D81" s="130"/>
+      <c r="E81" s="130"/>
+      <c r="F81" s="130"/>
+    </row>
+    <row r="82" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B82" s="132" t="s">
+        <v>311</v>
+      </c>
+      <c r="C82" s="131" t="s">
+        <v>282</v>
+      </c>
+      <c r="D82" s="131"/>
+      <c r="E82" s="131"/>
+      <c r="F82" s="131"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83" s="51"/>
+      <c r="B83" s="127" t="s">
+        <v>249</v>
+      </c>
+      <c r="C83" s="129"/>
+      <c r="D83" s="129"/>
+      <c r="E83" s="129"/>
+      <c r="F83" s="129"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84" s="51"/>
+      <c r="B84" s="88" t="s">
+        <v>117</v>
+      </c>
+      <c r="C84" s="89" t="s">
+        <v>116</v>
+      </c>
+      <c r="D84" s="88"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A85" s="51"/>
+      <c r="B85" s="88" t="s">
         <v>312</v>
       </c>
-      <c r="C75" s="89" t="s">
+      <c r="C85" s="89" t="s">
         <v>313</v>
       </c>
-      <c r="D75" s="88"/>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A76" s="52"/>
-      <c r="B76" s="88" t="s">
+      <c r="D85" s="88"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86" s="52"/>
+      <c r="B86" s="88" t="s">
         <v>140</v>
       </c>
-      <c r="C76" s="89" t="s">
+      <c r="C86" s="89" t="s">
         <v>141</v>
       </c>
-      <c r="D76" s="88"/>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A77" s="52"/>
-      <c r="B77" s="88" t="s">
+      <c r="D86" s="88"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87" s="52"/>
+      <c r="B87" s="88" t="s">
         <v>324</v>
       </c>
-      <c r="C77" s="89" t="s">
+      <c r="C87" s="89" t="s">
         <v>326</v>
       </c>
-      <c r="D77" s="88"/>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A78" s="87"/>
-      <c r="B78" s="69" t="s">
+      <c r="D87" s="88"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A88" s="87"/>
+      <c r="B88" s="69" t="s">
         <v>111</v>
       </c>
-      <c r="C78" s="64" t="s">
+      <c r="C88" s="64" t="s">
         <v>115</v>
       </c>
-      <c r="D78" s="64"/>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A79" s="87"/>
-      <c r="B79" s="142" t="s">
+      <c r="D88" s="64"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A89" s="87"/>
+      <c r="B89" s="142" t="s">
         <v>314</v>
-      </c>
-      <c r="C79" s="119"/>
-      <c r="D79" s="119"/>
-      <c r="E79" s="119"/>
-      <c r="F79" s="119"/>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A80" s="87"/>
-      <c r="B80" s="71" t="s">
-        <v>119</v>
-      </c>
-      <c r="C80" s="72" t="s">
-        <v>158</v>
-      </c>
-      <c r="D80" s="72"/>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A81" s="87"/>
-      <c r="B81" s="71" t="s">
-        <v>316</v>
-      </c>
-      <c r="C81" s="72" t="s">
-        <v>315</v>
-      </c>
-      <c r="D81" s="72"/>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A82" s="87"/>
-      <c r="B82" s="71" t="s">
-        <v>317</v>
-      </c>
-      <c r="C82" s="72" t="s">
-        <v>318</v>
-      </c>
-      <c r="D82" s="72"/>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A83" s="119" t="s">
-        <v>250</v>
-      </c>
-      <c r="B83" s="142" t="s">
-        <v>319</v>
-      </c>
-      <c r="C83" s="119"/>
-      <c r="D83" s="119"/>
-      <c r="E83" s="119"/>
-      <c r="F83" s="119"/>
-    </row>
-    <row r="84" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="90"/>
-      <c r="B84" s="71" t="s">
-        <v>38</v>
-      </c>
-      <c r="C84" s="72" t="s">
-        <v>163</v>
-      </c>
-      <c r="D84" s="72"/>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A85" s="119" t="s">
-        <v>257</v>
-      </c>
-      <c r="B85" s="71" t="s">
-        <v>32</v>
-      </c>
-      <c r="C85" s="72" t="s">
-        <v>157</v>
-      </c>
-      <c r="D85" s="72"/>
-    </row>
-    <row r="86" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="90"/>
-      <c r="B86" s="71" t="s">
-        <v>200</v>
-      </c>
-      <c r="C86" s="110" t="s">
-        <v>201</v>
-      </c>
-      <c r="D86" s="72"/>
-    </row>
-    <row r="87" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="91"/>
-      <c r="B87" s="71" t="s">
-        <v>203</v>
-      </c>
-      <c r="C87" s="110" t="s">
-        <v>204</v>
-      </c>
-      <c r="D87" s="72"/>
-    </row>
-    <row r="88" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="91"/>
-      <c r="B88" s="71" t="s">
-        <v>321</v>
-      </c>
-      <c r="C88" s="110" t="s">
-        <v>320</v>
-      </c>
-      <c r="D88" s="72"/>
-    </row>
-    <row r="89" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="91"/>
-      <c r="B89" s="142" t="s">
-        <v>322</v>
       </c>
       <c r="C89" s="119"/>
       <c r="D89" s="119"/>
       <c r="E89" s="119"/>
       <c r="F89" s="119"/>
     </row>
-    <row r="90" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="91"/>
-      <c r="B90" s="75" t="s">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90" s="87"/>
+      <c r="B90" s="71" t="s">
+        <v>119</v>
+      </c>
+      <c r="C90" s="72" t="s">
+        <v>158</v>
+      </c>
+      <c r="D90" s="72"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A91" s="87"/>
+      <c r="B91" s="71" t="s">
+        <v>316</v>
+      </c>
+      <c r="C91" s="72" t="s">
+        <v>315</v>
+      </c>
+      <c r="D91" s="72"/>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A92" s="87"/>
+      <c r="B92" s="71" t="s">
+        <v>317</v>
+      </c>
+      <c r="C92" s="72" t="s">
+        <v>318</v>
+      </c>
+      <c r="D92" s="72"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A93" s="119" t="s">
+        <v>250</v>
+      </c>
+      <c r="B93" s="142" t="s">
+        <v>319</v>
+      </c>
+      <c r="C93" s="119"/>
+      <c r="D93" s="119"/>
+      <c r="E93" s="119"/>
+      <c r="F93" s="119"/>
+    </row>
+    <row r="94" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="90"/>
+      <c r="B94" s="71" t="s">
+        <v>38</v>
+      </c>
+      <c r="C94" s="72" t="s">
+        <v>163</v>
+      </c>
+      <c r="D94" s="72"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A95" s="119" t="s">
+        <v>257</v>
+      </c>
+      <c r="B95" s="71" t="s">
+        <v>32</v>
+      </c>
+      <c r="C95" s="72" t="s">
+        <v>157</v>
+      </c>
+      <c r="D95" s="72"/>
+    </row>
+    <row r="96" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="90"/>
+      <c r="B96" s="71" t="s">
+        <v>200</v>
+      </c>
+      <c r="C96" s="110" t="s">
+        <v>201</v>
+      </c>
+      <c r="D96" s="72"/>
+    </row>
+    <row r="97" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="91"/>
+      <c r="B97" s="71" t="s">
+        <v>203</v>
+      </c>
+      <c r="C97" s="110" t="s">
+        <v>204</v>
+      </c>
+      <c r="D97" s="72"/>
+    </row>
+    <row r="98" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="91"/>
+      <c r="B98" s="71" t="s">
+        <v>321</v>
+      </c>
+      <c r="C98" s="110" t="s">
+        <v>320</v>
+      </c>
+      <c r="D98" s="72"/>
+    </row>
+    <row r="99" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="91"/>
+      <c r="B99" s="142" t="s">
+        <v>322</v>
+      </c>
+      <c r="C99" s="119"/>
+      <c r="D99" s="119"/>
+      <c r="E99" s="119"/>
+      <c r="F99" s="119"/>
+    </row>
+    <row r="100" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="91"/>
+      <c r="B100" s="75" t="s">
         <v>259</v>
       </c>
-      <c r="C90" s="93"/>
-      <c r="D90" s="93"/>
-      <c r="E90" s="93"/>
-      <c r="F90" s="93"/>
-    </row>
-    <row r="91" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="119" t="s">
+      <c r="C100" s="93"/>
+      <c r="D100" s="93"/>
+      <c r="E100" s="93"/>
+      <c r="F100" s="93"/>
+    </row>
+    <row r="101" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="119" t="s">
         <v>258</v>
       </c>
-      <c r="B91" s="84" t="s">
+      <c r="B101" s="84" t="s">
         <v>90</v>
       </c>
-      <c r="C91" s="72" t="s">
+      <c r="C101" s="72" t="s">
         <v>160</v>
       </c>
-      <c r="D91" s="72"/>
-    </row>
-    <row r="92" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="92"/>
-      <c r="B92" s="84" t="s">
+      <c r="D101" s="72"/>
+    </row>
+    <row r="102" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A102" s="92"/>
+      <c r="B102" s="84" t="s">
         <v>89</v>
       </c>
-      <c r="C92" s="72" t="s">
+      <c r="C102" s="72" t="s">
         <v>161</v>
       </c>
-      <c r="D92" s="72"/>
-    </row>
-    <row r="93" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="94"/>
-      <c r="B93" s="75" t="s">
+      <c r="D102" s="72"/>
+    </row>
+    <row r="103" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A103" s="94"/>
+      <c r="B103" s="75" t="s">
         <v>260</v>
       </c>
-      <c r="C93" s="93"/>
-      <c r="D93" s="93"/>
-      <c r="E93" s="93"/>
-      <c r="F93" s="93"/>
-    </row>
-    <row r="94" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="94"/>
-      <c r="B94" s="118" t="s">
+      <c r="C103" s="93"/>
+      <c r="D103" s="93"/>
+      <c r="E103" s="93"/>
+      <c r="F103" s="93"/>
+    </row>
+    <row r="104" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="94"/>
+      <c r="B104" s="118" t="s">
         <v>137</v>
       </c>
-      <c r="C94" s="72" t="s">
+      <c r="C104" s="72" t="s">
         <v>138</v>
       </c>
-      <c r="D94" s="72"/>
-    </row>
-    <row r="95" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="92"/>
-      <c r="B95" s="118" t="s">
+      <c r="D104" s="72"/>
+    </row>
+    <row r="105" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="92"/>
+      <c r="B105" s="118" t="s">
         <v>137</v>
       </c>
-      <c r="C95" s="72" t="s">
+      <c r="C105" s="72" t="s">
         <v>234</v>
       </c>
-      <c r="D95" s="72"/>
-    </row>
-    <row r="96" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="94"/>
-      <c r="B96" s="118" t="s">
+      <c r="D105" s="72"/>
+    </row>
+    <row r="106" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="94"/>
+      <c r="B106" s="118" t="s">
         <v>192</v>
       </c>
-      <c r="C96" s="72" t="s">
+      <c r="C106" s="72" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="97" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="99" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B99" s="106" t="s">
+    <row r="107" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2"/>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B109" s="106" t="s">
         <v>193</v>
       </c>
-      <c r="C99" s="106" t="s">
+      <c r="C109" s="106" t="s">
         <v>197</v>
       </c>
-      <c r="D99" s="149" t="s">
+      <c r="D109" s="149" t="s">
         <v>198</v>
       </c>
-      <c r="E99" s="149"/>
-      <c r="F99" s="149"/>
-    </row>
-    <row r="100" spans="2:6" ht="127.5" x14ac:dyDescent="0.2">
-      <c r="B100" s="109" t="s">
+      <c r="E109" s="149"/>
+      <c r="F109" s="149"/>
+    </row>
+    <row r="110" spans="1:6" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="B110" s="109" t="s">
         <v>194</v>
       </c>
-      <c r="C100" s="108" t="s">
+      <c r="C110" s="108" t="s">
         <v>206</v>
       </c>
-      <c r="D100" s="150" t="s">
+      <c r="D110" s="150" t="s">
         <v>199</v>
       </c>
-      <c r="E100" s="150"/>
-      <c r="F100" s="150"/>
-    </row>
-    <row r="101" spans="2:6" ht="102" x14ac:dyDescent="0.2">
-      <c r="B101" s="109" t="s">
+      <c r="E110" s="150"/>
+      <c r="F110" s="150"/>
+    </row>
+    <row r="111" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+      <c r="B111" s="109" t="s">
         <v>195</v>
       </c>
-      <c r="C101" s="115" t="s">
+      <c r="C111" s="115" t="s">
         <v>205</v>
       </c>
-      <c r="D101" s="150" t="s">
+      <c r="D111" s="150" t="s">
         <v>202</v>
       </c>
-      <c r="E101" s="150"/>
-      <c r="F101" s="150"/>
-    </row>
-    <row r="102" spans="2:6" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="B102" s="109" t="s">
+      <c r="E111" s="150"/>
+      <c r="F111" s="150"/>
+    </row>
+    <row r="112" spans="1:6" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="B112" s="109" t="s">
         <v>196</v>
       </c>
-      <c r="C102" s="108" t="s">
+      <c r="C112" s="108" t="s">
         <v>210</v>
       </c>
-      <c r="D102" s="150" t="s">
+      <c r="D112" s="150" t="s">
         <v>211</v>
       </c>
-      <c r="E102" s="150"/>
-      <c r="F102" s="150"/>
-    </row>
-    <row r="103" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B103" s="117"/>
-    </row>
-    <row r="104" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B104" s="116" t="s">
+      <c r="E112" s="150"/>
+      <c r="F112" s="150"/>
+    </row>
+    <row r="113" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B113" s="117"/>
+    </row>
+    <row r="114" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B114" s="116" t="s">
         <v>219</v>
       </c>
-      <c r="C104" s="116" t="s">
+      <c r="C114" s="116" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="105" spans="2:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="B105" s="117" t="s">
+    <row r="115" spans="2:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="B115" s="117" t="s">
         <v>220</v>
       </c>
-      <c r="C105" s="108" t="s">
+      <c r="C115" s="108" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="106" spans="2:6" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="B106" s="117" t="s">
+    <row r="116" spans="2:3" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="B116" s="117" t="s">
         <v>221</v>
       </c>
-      <c r="C106" s="108" t="s">
+      <c r="C116" s="108" t="s">
         <v>223</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="D102:F102"/>
-    <mergeCell ref="D101:F101"/>
-    <mergeCell ref="D100:F100"/>
-    <mergeCell ref="D99:F99"/>
+    <mergeCell ref="D112:F112"/>
+    <mergeCell ref="D111:F111"/>
+    <mergeCell ref="D110:F110"/>
+    <mergeCell ref="D109:F109"/>
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D100" r:id="rId1"/>
-    <hyperlink ref="D101" r:id="rId2"/>
-    <hyperlink ref="D102" r:id="rId3"/>
+    <hyperlink ref="D110" r:id="rId1"/>
+    <hyperlink ref="D111" r:id="rId2"/>
+    <hyperlink ref="D112" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>

</xml_diff>

<commit_message>
Para la carpeta de Mejora se intento poner nombres mas claros
</commit_message>
<xml_diff>
--- a/Organización/Procesos/Soporte Organizacional/2. Administración de Configuración/IWM_Administración de la Configuración.xlsx
+++ b/Organización/Procesos/Soporte Organizacional/2. Administración de Configuración/IWM_Administración de la Configuración.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="362">
   <si>
     <t>Adapiaciones al Estándar de Administración de Datos</t>
   </si>
@@ -1773,9 +1773,6 @@
     <t>Concentrado_Mejoras_aaaa</t>
   </si>
   <si>
-    <t>IWM_&lt;tipo de capacitación o proceso&gt;_aammdd</t>
-  </si>
-  <si>
     <t>EC_&lt;tipo de capacitación o proceso&gt;_aammdd</t>
   </si>
   <si>
@@ -1791,7 +1788,7 @@
     <t>SM_&lt;tipo de capacitación o proceso&gt;_aammdd</t>
   </si>
   <si>
-    <t>R_&lt;tipo de actividado&gt;_aammdd</t>
+    <t>IWM_Reporte de actividades_aammdd</t>
   </si>
 </sst>
 </file>
@@ -5411,8 +5408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -5521,7 +5518,7 @@
         <v>338</v>
       </c>
       <c r="C10" s="89" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D10" s="88"/>
     </row>
@@ -5541,7 +5538,7 @@
         <v>336</v>
       </c>
       <c r="C12" s="89" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D12" s="88"/>
     </row>
@@ -5564,7 +5561,7 @@
         <v>328</v>
       </c>
       <c r="C14" s="89" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="D14" s="88"/>
     </row>
@@ -5603,7 +5600,7 @@
         <v>262</v>
       </c>
       <c r="C18" s="89" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D18" s="88"/>
     </row>
@@ -5623,7 +5620,7 @@
         <v>264</v>
       </c>
       <c r="C20" s="89" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D20" s="88"/>
     </row>
@@ -5643,7 +5640,7 @@
         <v>353</v>
       </c>
       <c r="C22" s="89" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D22" s="88"/>
     </row>
@@ -5666,7 +5663,7 @@
         <v>328</v>
       </c>
       <c r="C24" s="89" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D24" s="88"/>
     </row>

</xml_diff>

<commit_message>
reacomodo de archivos y actualización en la administracion de la configuración
</commit_message>
<xml_diff>
--- a/Organización/Procesos/Soporte Organizacional/2. Administración de Configuración/IWM_Administración de la Configuración.xlsx
+++ b/Organización/Procesos/Soporte Organizacional/2. Administración de Configuración/IWM_Administración de la Configuración.xlsx
@@ -505,9 +505,6 @@
     <t>IWM_Manual_Configuración</t>
   </si>
   <si>
-    <t>IWM_Plan del aseguramiento de la Calidad</t>
-  </si>
-  <si>
     <t>Sí</t>
   </si>
   <si>
@@ -1789,6 +1786,9 @@
   </si>
   <si>
     <t>IWM_Reporte de actividades_aammdd</t>
+  </si>
+  <si>
+    <t>IWM_PlanAseguramientoCalidad</t>
   </si>
 </sst>
 </file>
@@ -4817,7 +4817,7 @@
         <v>77</v>
       </c>
       <c r="D7" s="70" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -4838,10 +4838,10 @@
         <v>122</v>
       </c>
       <c r="C9" s="70" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D9" s="70" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -4852,7 +4852,7 @@
         <v>123</v>
       </c>
       <c r="C10" s="70" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D10" s="56" t="s">
         <v>77</v>
@@ -4880,10 +4880,10 @@
         <v>139</v>
       </c>
       <c r="C12" s="70" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D12" s="70" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -4907,16 +4907,16 @@
         <v>136</v>
       </c>
       <c r="B15" s="70" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C15" s="70"/>
     </row>
     <row r="16" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A16" s="103" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B16" s="104" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C16" s="70"/>
       <c r="D16" s="70"/>
@@ -4940,7 +4940,7 @@
       </c>
       <c r="C18" s="70"/>
       <c r="D18" s="70" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -4951,7 +4951,7 @@
         <v>127</v>
       </c>
       <c r="C19" s="70" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D19" s="70"/>
     </row>
@@ -4968,20 +4968,20 @@
         <v>104</v>
       </c>
       <c r="B21" s="78" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C21" s="70"/>
       <c r="D21" s="70"/>
     </row>
     <row r="22" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A22" s="77" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B22" s="78" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C22" s="70" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D22" s="70"/>
     </row>
@@ -4990,7 +4990,7 @@
         <v>142</v>
       </c>
       <c r="B23" s="70" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C23" s="70"/>
       <c r="D23" s="70"/>
@@ -5000,7 +5000,7 @@
         <v>143</v>
       </c>
       <c r="B24" s="70" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C24" s="70"/>
       <c r="D24" s="70"/>
@@ -5010,17 +5010,17 @@
         <v>143</v>
       </c>
       <c r="B25" s="70" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C25" s="70"/>
       <c r="D25" s="70"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="77" t="s">
+        <v>223</v>
+      </c>
+      <c r="B26" s="70" t="s">
         <v>224</v>
-      </c>
-      <c r="B26" s="70" t="s">
-        <v>225</v>
       </c>
       <c r="C26" s="70"/>
       <c r="D26" s="70"/>
@@ -5046,7 +5046,7 @@
         <v>103</v>
       </c>
       <c r="B29" s="83" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C29" s="70" t="s">
         <v>77</v>
@@ -5063,77 +5063,77 @@
     </row>
     <row r="31" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A31" s="77" t="s">
+        <v>177</v>
+      </c>
+      <c r="B31" s="105" t="s">
         <v>178</v>
-      </c>
-      <c r="B31" s="105" t="s">
-        <v>179</v>
       </c>
       <c r="C31" s="105"/>
       <c r="D31" s="105"/>
     </row>
     <row r="32" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A32" s="77" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B32" s="105" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C32" s="105"/>
       <c r="D32" s="105"/>
     </row>
     <row r="33" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A33" s="77" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B33" s="105" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C33" s="105"/>
       <c r="D33" s="105"/>
     </row>
     <row r="34" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A34" s="77" t="s">
+        <v>181</v>
+      </c>
+      <c r="B34" s="105" t="s">
         <v>182</v>
-      </c>
-      <c r="B34" s="105" t="s">
-        <v>183</v>
       </c>
       <c r="C34" s="105"/>
       <c r="D34" s="105"/>
     </row>
     <row r="35" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A35" s="77" t="s">
+        <v>183</v>
+      </c>
+      <c r="B35" s="105" t="s">
         <v>184</v>
-      </c>
-      <c r="B35" s="105" t="s">
-        <v>185</v>
       </c>
       <c r="C35" s="105"/>
       <c r="D35" s="105"/>
     </row>
     <row r="36" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A36" s="77" t="s">
+        <v>185</v>
+      </c>
+      <c r="B36" s="105" t="s">
         <v>186</v>
-      </c>
-      <c r="B36" s="105" t="s">
-        <v>187</v>
       </c>
       <c r="C36" s="105"/>
       <c r="D36" s="105"/>
     </row>
     <row r="37" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A37" s="84" t="s">
+        <v>187</v>
+      </c>
+      <c r="B37" s="85" t="s">
         <v>188</v>
-      </c>
-      <c r="B37" s="85" t="s">
-        <v>189</v>
       </c>
       <c r="C37" s="70"/>
       <c r="D37" s="70"/>
     </row>
     <row r="38" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A38" s="81" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B38" s="81"/>
       <c r="C38" s="81"/>
@@ -5141,20 +5141,20 @@
     </row>
     <row r="39" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A39" s="84" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B39" s="86" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C39" s="70"/>
       <c r="D39" s="70"/>
     </row>
     <row r="40" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A40" s="84" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B40" s="85" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C40" s="70" t="s">
         <v>77</v>
@@ -5166,14 +5166,14 @@
         <v>45</v>
       </c>
       <c r="B41" s="85" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C41" s="70"/>
       <c r="D41" s="70"/>
     </row>
     <row r="42" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A42" s="81" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B42" s="81"/>
       <c r="C42" s="81"/>
@@ -5190,7 +5190,7 @@
         <v>77</v>
       </c>
       <c r="D43" s="70" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -5204,7 +5204,7 @@
         <v>77</v>
       </c>
       <c r="D44" s="70" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="45" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -5220,13 +5220,13 @@
         <v>86</v>
       </c>
       <c r="B46" s="99" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C46" s="99" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D46" s="70" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -5234,7 +5234,7 @@
         <v>86</v>
       </c>
       <c r="B47" s="99" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C47" s="99"/>
       <c r="D47" s="70"/>
@@ -5252,7 +5252,7 @@
         <v>153</v>
       </c>
       <c r="B49" s="99" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C49" s="56"/>
       <c r="D49" s="56"/>
@@ -5262,7 +5262,7 @@
         <v>154</v>
       </c>
       <c r="B50" s="99" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C50" s="56"/>
       <c r="D50" s="56"/>
@@ -5277,17 +5277,17 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="107" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B52" s="56" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C52" s="56"/>
       <c r="D52" s="56"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="88" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B53" s="72" t="s">
         <v>157</v>
@@ -5298,7 +5298,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="122" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B54" s="130"/>
       <c r="C54" s="130"/>
@@ -5307,10 +5307,10 @@
     </row>
     <row r="55" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="132" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B55" s="131" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C55" s="131"/>
       <c r="D55" s="131"/>
@@ -5349,7 +5349,7 @@
         <v>98</v>
       </c>
       <c r="C59" s="147" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D59" s="147"/>
     </row>
@@ -5358,10 +5358,10 @@
         <v>79</v>
       </c>
       <c r="B60" s="102" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C60" s="147" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D60" s="147"/>
     </row>
@@ -5370,10 +5370,10 @@
         <v>97</v>
       </c>
       <c r="B61" s="102" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C61" s="145" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D61" s="145"/>
     </row>
@@ -5382,10 +5382,10 @@
         <v>71</v>
       </c>
       <c r="B62" s="102" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C62" s="144" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D62" s="144"/>
     </row>
@@ -5408,8 +5408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="B82" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C90" sqref="C90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -5459,25 +5459,25 @@
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="49"/>
       <c r="B4" s="48" t="s">
+        <v>329</v>
+      </c>
+      <c r="C4" s="48" t="s">
         <v>330</v>
-      </c>
-      <c r="C4" s="48" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="49"/>
       <c r="B5" s="48" t="s">
+        <v>332</v>
+      </c>
+      <c r="C5" s="48" t="s">
         <v>333</v>
-      </c>
-      <c r="C5" s="48" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="49"/>
       <c r="B6" s="59" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C6" s="53"/>
       <c r="D6" s="53"/>
@@ -5487,25 +5487,25 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="49"/>
       <c r="B7" s="48" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C7" s="48" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="49"/>
       <c r="B8" s="48" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C8" s="48" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="49"/>
       <c r="B9" s="127" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C9" s="128"/>
       <c r="D9" s="128"/>
@@ -5515,17 +5515,17 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="49"/>
       <c r="B10" s="88" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C10" s="89" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D10" s="88"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="49"/>
       <c r="B11" s="127" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C11" s="128"/>
       <c r="D11" s="128"/>
@@ -5535,40 +5535,40 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="49"/>
       <c r="B12" s="88" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C12" s="89" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D12" s="88"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="62"/>
       <c r="B13" s="127" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C13" s="128"/>
       <c r="D13" s="128"/>
       <c r="E13" s="126"/>
       <c r="F13" s="126"/>
       <c r="I13" s="48" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="63"/>
       <c r="B14" s="88" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C14" s="89" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D14" s="88"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="49"/>
       <c r="B15" s="59" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C15" s="53"/>
       <c r="D15" s="53"/>
@@ -5578,16 +5578,16 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="49"/>
       <c r="B16" s="48" t="s">
+        <v>348</v>
+      </c>
+      <c r="C16" s="48" t="s">
         <v>349</v>
-      </c>
-      <c r="C16" s="48" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="49"/>
       <c r="B17" s="127" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C17" s="128"/>
       <c r="D17" s="128"/>
@@ -5597,17 +5597,17 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="49"/>
       <c r="B18" s="88" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C18" s="89" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D18" s="88"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="49"/>
       <c r="B19" s="127" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C19" s="128"/>
       <c r="D19" s="128"/>
@@ -5617,17 +5617,17 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="49"/>
       <c r="B20" s="88" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C20" s="89" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D20" s="88"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="49"/>
       <c r="B21" s="127" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C21" s="128"/>
       <c r="D21" s="128"/>
@@ -5637,33 +5637,33 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="49"/>
       <c r="B22" s="88" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C22" s="89" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D22" s="88"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="62"/>
       <c r="B23" s="127" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C23" s="128"/>
       <c r="D23" s="128"/>
       <c r="E23" s="126"/>
       <c r="F23" s="126"/>
       <c r="I23" s="48" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="63"/>
       <c r="B24" s="88" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C24" s="89" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D24" s="88"/>
     </row>
@@ -5675,13 +5675,13 @@
       <c r="E25" s="51"/>
       <c r="F25" s="51"/>
       <c r="I25" s="125" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="52"/>
       <c r="B26" s="59" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C26" s="53"/>
       <c r="D26" s="53"/>
@@ -5697,13 +5697,13 @@
       </c>
       <c r="H27" s="124"/>
       <c r="I27" s="48" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H28" s="126"/>
       <c r="I28" s="48" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
@@ -5715,13 +5715,13 @@
       <c r="F29" s="51"/>
       <c r="H29" s="113"/>
       <c r="I29" s="48" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="52"/>
       <c r="B30" s="60" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C30" s="61"/>
       <c r="D30" s="61"/>
@@ -5729,20 +5729,20 @@
       <c r="F30" s="52"/>
       <c r="H30" s="114"/>
       <c r="I30" s="48" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="62"/>
       <c r="B31" s="127" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C31" s="128"/>
       <c r="D31" s="128"/>
       <c r="E31" s="126"/>
       <c r="F31" s="126"/>
       <c r="I31" s="48" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -5772,7 +5772,7 @@
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="63"/>
       <c r="B34" s="66" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C34" s="67"/>
       <c r="D34" s="67"/>
@@ -5782,10 +5782,10 @@
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="63"/>
       <c r="B35" s="69" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C35" s="64" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D35" s="64" t="s">
         <v>77</v>
@@ -5794,10 +5794,10 @@
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="63"/>
       <c r="B36" s="69" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C36" s="64" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D36" s="64"/>
     </row>
@@ -5824,7 +5824,7 @@
         <v>130</v>
       </c>
       <c r="D38" s="70" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="39" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -5836,7 +5836,7 @@
         <v>113</v>
       </c>
       <c r="D39" s="70" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="40" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -5860,13 +5860,13 @@
         <v>118</v>
       </c>
       <c r="D41" s="70" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="42" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A42" s="68"/>
       <c r="B42" s="66" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C42" s="67" t="s">
         <v>14</v>
@@ -5878,7 +5878,7 @@
     <row r="43" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A43" s="68"/>
       <c r="B43" s="75" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C43" s="76"/>
       <c r="D43" s="76"/>
@@ -5893,7 +5893,7 @@
         <v>136</v>
       </c>
       <c r="C44" s="70" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D44" s="70"/>
     </row>
@@ -5903,7 +5903,7 @@
         <v>78</v>
       </c>
       <c r="C45" s="70" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D45" s="70"/>
     </row>
@@ -5916,13 +5916,13 @@
         <v>114</v>
       </c>
       <c r="D46" s="70" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="47" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A47" s="74"/>
       <c r="B47" s="75" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C47" s="76"/>
       <c r="D47" s="76"/>
@@ -5938,7 +5938,7 @@
         <v>133</v>
       </c>
       <c r="D48" s="70" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="49" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -5947,7 +5947,7 @@
         <v>142</v>
       </c>
       <c r="C49" s="70" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D49" s="72"/>
       <c r="E49" s="64"/>
@@ -5965,7 +5965,7 @@
     <row r="51" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A51" s="74"/>
       <c r="B51" s="66" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C51" s="67"/>
       <c r="D51" s="67"/>
@@ -5975,7 +5975,7 @@
     <row r="52" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A52" s="74"/>
       <c r="B52" s="80" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C52" s="81"/>
       <c r="D52" s="81"/>
@@ -5988,7 +5988,7 @@
         <v>103</v>
       </c>
       <c r="C53" s="83" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D53" s="72" t="s">
         <v>77</v>
@@ -5997,10 +5997,10 @@
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="74"/>
       <c r="B54" s="77" t="s">
+        <v>345</v>
+      </c>
+      <c r="C54" s="83" t="s">
         <v>346</v>
-      </c>
-      <c r="C54" s="83" t="s">
-        <v>347</v>
       </c>
       <c r="D54" s="72"/>
     </row>
@@ -6009,7 +6009,7 @@
         <v>82</v>
       </c>
       <c r="B55" s="80" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C55" s="81"/>
       <c r="D55" s="81"/>
@@ -6019,7 +6019,7 @@
     <row r="56" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A56" s="82"/>
       <c r="B56" s="80" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C56" s="81"/>
       <c r="D56" s="81"/>
@@ -6029,20 +6029,20 @@
     <row r="57" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A57" s="82"/>
       <c r="B57" s="84" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C57" s="86" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D57" s="72"/>
     </row>
     <row r="58" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A58" s="82"/>
       <c r="B58" s="84" t="s">
+        <v>207</v>
+      </c>
+      <c r="C58" s="48" t="s">
         <v>208</v>
-      </c>
-      <c r="C58" s="48" t="s">
-        <v>209</v>
       </c>
       <c r="D58" s="72" t="s">
         <v>77</v>
@@ -6051,17 +6051,17 @@
     <row r="59" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A59" s="82"/>
       <c r="B59" s="84" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C59" s="85" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D59" s="72"/>
     </row>
     <row r="60" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A60" s="82"/>
       <c r="B60" s="80" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C60" s="81"/>
       <c r="D60" s="81"/>
@@ -6074,7 +6074,7 @@
         <v>85</v>
       </c>
       <c r="C61" s="86" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D61" s="72" t="s">
         <v>77</v>
@@ -6095,7 +6095,7 @@
     <row r="63" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A63" s="82"/>
       <c r="B63" s="66" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C63" s="67"/>
       <c r="D63" s="67"/>
@@ -6111,7 +6111,7 @@
         <v>135</v>
       </c>
       <c r="D64" s="72" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
@@ -6119,7 +6119,7 @@
         <v>83</v>
       </c>
       <c r="B65" s="66" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C65" s="67"/>
       <c r="D65" s="67"/>
@@ -6147,7 +6147,7 @@
     </row>
     <row r="68" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B68" s="66" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C68" s="67"/>
       <c r="D68" s="67"/>
@@ -6164,7 +6164,7 @@
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="51"/>
       <c r="B70" s="122" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C70" s="67"/>
       <c r="D70" s="67"/>
@@ -6173,17 +6173,17 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B71" s="71" t="s">
+        <v>323</v>
+      </c>
+      <c r="C71" s="72" t="s">
         <v>324</v>
-      </c>
-      <c r="C71" s="72" t="s">
-        <v>325</v>
       </c>
       <c r="D71" s="70"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="51"/>
       <c r="B72" s="122" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C72" s="67"/>
       <c r="D72" s="67"/>
@@ -6193,10 +6193,10 @@
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="51"/>
       <c r="B73" s="123" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C73" s="105" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D73" s="55"/>
       <c r="E73" s="64"/>
@@ -6205,10 +6205,10 @@
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="51"/>
       <c r="B74" s="123" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C74" s="105" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D74" s="55"/>
       <c r="E74" s="64"/>
@@ -6217,10 +6217,10 @@
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="51"/>
       <c r="B75" s="123" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C75" s="105" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D75" s="55"/>
       <c r="E75" s="64"/>
@@ -6229,10 +6229,10 @@
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="51"/>
       <c r="B76" s="123" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C76" s="105" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D76" s="55"/>
       <c r="E76" s="64"/>
@@ -6241,10 +6241,10 @@
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="51"/>
       <c r="B77" s="123" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C77" s="105" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D77" s="55"/>
       <c r="E77" s="64"/>
@@ -6253,7 +6253,7 @@
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="51"/>
       <c r="B78" s="122" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C78" s="67"/>
       <c r="D78" s="67"/>
@@ -6263,10 +6263,10 @@
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="51"/>
       <c r="B79" s="123" t="s">
+        <v>339</v>
+      </c>
+      <c r="C79" t="s">
         <v>340</v>
-      </c>
-      <c r="C79" t="s">
-        <v>341</v>
       </c>
       <c r="D79"/>
       <c r="E79"/>
@@ -6274,15 +6274,15 @@
     </row>
     <row r="80" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B80" s="123" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C80" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="81" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B81" s="122" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C81" s="130"/>
       <c r="D81" s="130"/>
@@ -6291,10 +6291,10 @@
     </row>
     <row r="82" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B82" s="132" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C82" s="131" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D82" s="131"/>
       <c r="E82" s="131"/>
@@ -6303,7 +6303,7 @@
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="51"/>
       <c r="B83" s="127" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C83" s="129"/>
       <c r="D83" s="129"/>
@@ -6323,10 +6323,10 @@
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="51"/>
       <c r="B85" s="88" t="s">
+        <v>311</v>
+      </c>
+      <c r="C85" s="89" t="s">
         <v>312</v>
-      </c>
-      <c r="C85" s="89" t="s">
-        <v>313</v>
       </c>
       <c r="D85" s="88"/>
     </row>
@@ -6343,10 +6343,10 @@
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="52"/>
       <c r="B87" s="88" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C87" s="89" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D87" s="88"/>
     </row>
@@ -6363,7 +6363,7 @@
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="87"/>
       <c r="B89" s="142" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C89" s="119"/>
       <c r="D89" s="119"/>
@@ -6376,36 +6376,36 @@
         <v>119</v>
       </c>
       <c r="C90" s="72" t="s">
-        <v>158</v>
+        <v>361</v>
       </c>
       <c r="D90" s="72"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="87"/>
       <c r="B91" s="71" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C91" s="72" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D91" s="72"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" s="87"/>
       <c r="B92" s="71" t="s">
+        <v>316</v>
+      </c>
+      <c r="C92" s="72" t="s">
         <v>317</v>
-      </c>
-      <c r="C92" s="72" t="s">
-        <v>318</v>
       </c>
       <c r="D92" s="72"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="119" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B93" s="142" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C93" s="119"/>
       <c r="D93" s="119"/>
@@ -6418,13 +6418,13 @@
         <v>38</v>
       </c>
       <c r="C94" s="72" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D94" s="72"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="119" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B95" s="71" t="s">
         <v>32</v>
@@ -6437,37 +6437,37 @@
     <row r="96" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A96" s="90"/>
       <c r="B96" s="71" t="s">
+        <v>199</v>
+      </c>
+      <c r="C96" s="110" t="s">
         <v>200</v>
-      </c>
-      <c r="C96" s="110" t="s">
-        <v>201</v>
       </c>
       <c r="D96" s="72"/>
     </row>
     <row r="97" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A97" s="91"/>
       <c r="B97" s="71" t="s">
+        <v>202</v>
+      </c>
+      <c r="C97" s="110" t="s">
         <v>203</v>
-      </c>
-      <c r="C97" s="110" t="s">
-        <v>204</v>
       </c>
       <c r="D97" s="72"/>
     </row>
     <row r="98" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A98" s="91"/>
       <c r="B98" s="71" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C98" s="110" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D98" s="72"/>
     </row>
     <row r="99" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A99" s="91"/>
       <c r="B99" s="142" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C99" s="119"/>
       <c r="D99" s="119"/>
@@ -6477,7 +6477,7 @@
     <row r="100" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A100" s="91"/>
       <c r="B100" s="75" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C100" s="93"/>
       <c r="D100" s="93"/>
@@ -6486,13 +6486,13 @@
     </row>
     <row r="101" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="119" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B101" s="84" t="s">
         <v>90</v>
       </c>
       <c r="C101" s="72" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D101" s="72"/>
     </row>
@@ -6502,14 +6502,14 @@
         <v>89</v>
       </c>
       <c r="C102" s="72" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D102" s="72"/>
     </row>
     <row r="103" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A103" s="94"/>
       <c r="B103" s="75" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C103" s="93"/>
       <c r="D103" s="93"/>
@@ -6532,68 +6532,68 @@
         <v>137</v>
       </c>
       <c r="C105" s="72" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D105" s="72"/>
     </row>
     <row r="106" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A106" s="94"/>
       <c r="B106" s="118" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C106" s="72" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="107" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2"/>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B109" s="106" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C109" s="106" t="s">
+        <v>196</v>
+      </c>
+      <c r="D109" s="149" t="s">
         <v>197</v>
-      </c>
-      <c r="D109" s="149" t="s">
-        <v>198</v>
       </c>
       <c r="E109" s="149"/>
       <c r="F109" s="149"/>
     </row>
     <row r="110" spans="1:6" ht="127.5" x14ac:dyDescent="0.2">
       <c r="B110" s="109" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C110" s="108" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D110" s="150" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E110" s="150"/>
       <c r="F110" s="150"/>
     </row>
     <row r="111" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="B111" s="109" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C111" s="115" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D111" s="150" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E111" s="150"/>
       <c r="F111" s="150"/>
     </row>
     <row r="112" spans="1:6" ht="89.25" x14ac:dyDescent="0.2">
       <c r="B112" s="109" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C112" s="108" t="s">
+        <v>209</v>
+      </c>
+      <c r="D112" s="150" t="s">
         <v>210</v>
-      </c>
-      <c r="D112" s="150" t="s">
-        <v>211</v>
       </c>
       <c r="E112" s="150"/>
       <c r="F112" s="150"/>
@@ -6603,26 +6603,26 @@
     </row>
     <row r="114" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B114" s="116" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C114" s="116" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="115" spans="2:3" ht="51" x14ac:dyDescent="0.2">
       <c r="B115" s="117" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C115" s="108" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="116" spans="2:3" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B116" s="117" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C116" s="108" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -6661,142 +6661,142 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="136" t="s">
+        <v>282</v>
+      </c>
+      <c r="B1" s="136" t="s">
         <v>283</v>
       </c>
-      <c r="B1" s="136" t="s">
+      <c r="C1" s="136" t="s">
         <v>284</v>
       </c>
-      <c r="C1" s="136" t="s">
+      <c r="D1" s="136" t="s">
         <v>285</v>
-      </c>
-      <c r="D1" s="136" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="133" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B2" s="134" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C2" s="135" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D2" s="135" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="133" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B3" s="135" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C3" s="135" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D3" s="135" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="133" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B4" s="135" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C4" s="135" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D4" s="135" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="133" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B5" s="135" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C5" s="135" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D5" s="135" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="133" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B6" s="135" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C6" s="135" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D6" s="135" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="133" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B7" s="135" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C7" s="135" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D7" s="135" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="177.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="133" t="s">
+        <v>294</v>
+      </c>
+      <c r="B8" s="137" t="s">
+        <v>308</v>
+      </c>
+      <c r="C8" s="137" t="s">
+        <v>305</v>
+      </c>
+      <c r="D8" s="137" t="s">
         <v>295</v>
-      </c>
-      <c r="B8" s="137" t="s">
-        <v>309</v>
-      </c>
-      <c r="C8" s="137" t="s">
-        <v>306</v>
-      </c>
-      <c r="D8" s="137" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="133" t="s">
+        <v>296</v>
+      </c>
+      <c r="B9" s="135" t="s">
+        <v>307</v>
+      </c>
+      <c r="C9" s="135" t="s">
+        <v>306</v>
+      </c>
+      <c r="D9" s="135" t="s">
         <v>297</v>
-      </c>
-      <c r="B9" s="135" t="s">
-        <v>308</v>
-      </c>
-      <c r="C9" s="135" t="s">
-        <v>307</v>
-      </c>
-      <c r="D9" s="135" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="133" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B10" s="135" t="s">
+        <v>288</v>
+      </c>
+      <c r="C10" s="135" t="s">
+        <v>303</v>
+      </c>
+      <c r="D10" s="135" t="s">
         <v>289</v>
-      </c>
-      <c r="C10" s="135" t="s">
-        <v>304</v>
-      </c>
-      <c r="D10" s="135" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Se contemplo las Evaluaciones de Efectividad en la organizacion de carpetas
</commit_message>
<xml_diff>
--- a/Organización/Procesos/Soporte Organizacional/2. Administración de Configuración/IWM_Administración de la Configuración.xlsx
+++ b/Organización/Procesos/Soporte Organizacional/2. Administración de Configuración/IWM_Administración de la Configuración.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="364">
   <si>
     <t>Adapiaciones al Estándar de Administración de Datos</t>
   </si>
@@ -1789,6 +1789,12 @@
   </si>
   <si>
     <t>IWM_PlanAseguramientoCalidad</t>
+  </si>
+  <si>
+    <t>EE_&lt;tipo de capacitación o proceso&gt;_aammdd</t>
+  </si>
+  <si>
+    <t>Evaluación de Efectividad</t>
   </si>
 </sst>
 </file>
@@ -5406,10 +5412,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I116"/>
+  <dimension ref="A1:I117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B82" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C90" sqref="C90"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -5606,234 +5612,232 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="49"/>
-      <c r="B19" s="127" t="s">
-        <v>351</v>
-      </c>
-      <c r="C19" s="128"/>
-      <c r="D19" s="128"/>
-      <c r="E19" s="126"/>
-      <c r="F19" s="126"/>
+      <c r="B19" s="88" t="s">
+        <v>363</v>
+      </c>
+      <c r="C19" s="89" t="s">
+        <v>362</v>
+      </c>
+      <c r="D19" s="88"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="49"/>
-      <c r="B20" s="88" t="s">
-        <v>263</v>
-      </c>
-      <c r="C20" s="89" t="s">
-        <v>356</v>
-      </c>
-      <c r="D20" s="88"/>
+      <c r="B20" s="127" t="s">
+        <v>351</v>
+      </c>
+      <c r="C20" s="128"/>
+      <c r="D20" s="128"/>
+      <c r="E20" s="126"/>
+      <c r="F20" s="126"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="49"/>
-      <c r="B21" s="127" t="s">
-        <v>334</v>
-      </c>
-      <c r="C21" s="128"/>
-      <c r="D21" s="128"/>
-      <c r="E21" s="126"/>
-      <c r="F21" s="126"/>
+      <c r="B21" s="88" t="s">
+        <v>263</v>
+      </c>
+      <c r="C21" s="89" t="s">
+        <v>356</v>
+      </c>
+      <c r="D21" s="88"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="49"/>
-      <c r="B22" s="88" t="s">
+      <c r="B22" s="127" t="s">
+        <v>334</v>
+      </c>
+      <c r="C22" s="128"/>
+      <c r="D22" s="128"/>
+      <c r="E22" s="126"/>
+      <c r="F22" s="126"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="49"/>
+      <c r="B23" s="88" t="s">
         <v>352</v>
       </c>
-      <c r="C22" s="89" t="s">
+      <c r="C23" s="89" t="s">
         <v>357</v>
       </c>
-      <c r="D22" s="88"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="62"/>
-      <c r="B23" s="127" t="s">
+      <c r="D23" s="88"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="62"/>
+      <c r="B24" s="127" t="s">
         <v>326</v>
       </c>
-      <c r="C23" s="128"/>
-      <c r="D23" s="128"/>
-      <c r="E23" s="126"/>
-      <c r="F23" s="126"/>
-      <c r="I23" s="48" t="s">
+      <c r="C24" s="128"/>
+      <c r="D24" s="128"/>
+      <c r="E24" s="126"/>
+      <c r="F24" s="126"/>
+      <c r="I24" s="48" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="63"/>
-      <c r="B24" s="88" t="s">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="63"/>
+      <c r="B25" s="88" t="s">
         <v>327</v>
       </c>
-      <c r="C24" s="89" t="s">
+      <c r="C25" s="89" t="s">
         <v>358</v>
       </c>
-      <c r="D24" s="88"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="51"/>
-      <c r="B25" s="51"/>
-      <c r="C25" s="51"/>
-      <c r="D25" s="51"/>
-      <c r="E25" s="51"/>
-      <c r="F25" s="51"/>
-      <c r="I25" s="125" t="s">
+      <c r="D25" s="88"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="51"/>
+      <c r="B26" s="51"/>
+      <c r="C26" s="51"/>
+      <c r="D26" s="51"/>
+      <c r="E26" s="51"/>
+      <c r="F26" s="51"/>
+      <c r="I26" s="125" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="52"/>
-      <c r="B26" s="59" t="s">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="52"/>
+      <c r="B27" s="59" t="s">
         <v>234</v>
       </c>
-      <c r="C26" s="53"/>
-      <c r="D26" s="53"/>
-      <c r="E26" s="53"/>
-      <c r="F26" s="53"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B27" s="48" t="s">
+      <c r="C27" s="53"/>
+      <c r="D27" s="53"/>
+      <c r="E27" s="53"/>
+      <c r="F27" s="53"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B28" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="C27" s="48" t="s">
+      <c r="C28" s="48" t="s">
         <v>87</v>
       </c>
-      <c r="H27" s="124"/>
-      <c r="I27" s="48" t="s">
+      <c r="H28" s="124"/>
+      <c r="I28" s="48" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H28" s="126"/>
-      <c r="I28" s="48" t="s">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H29" s="126"/>
+      <c r="I29" s="48" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="51"/>
-      <c r="B29" s="51"/>
-      <c r="C29" s="51"/>
-      <c r="D29" s="51"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="51"/>
-      <c r="H29" s="113"/>
-      <c r="I29" s="48" t="s">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="51"/>
+      <c r="B30" s="51"/>
+      <c r="C30" s="51"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="51"/>
+      <c r="F30" s="51"/>
+      <c r="H30" s="113"/>
+      <c r="I30" s="48" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="52"/>
-      <c r="B30" s="60" t="s">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="52"/>
+      <c r="B31" s="60" t="s">
         <v>235</v>
       </c>
-      <c r="C30" s="61"/>
-      <c r="D30" s="61"/>
-      <c r="E30" s="52"/>
-      <c r="F30" s="52"/>
-      <c r="H30" s="114"/>
-      <c r="I30" s="48" t="s">
+      <c r="C31" s="61"/>
+      <c r="D31" s="61"/>
+      <c r="E31" s="52"/>
+      <c r="F31" s="52"/>
+      <c r="H31" s="114"/>
+      <c r="I31" s="48" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="62"/>
-      <c r="B31" s="127" t="s">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="62"/>
+      <c r="B32" s="127" t="s">
         <v>255</v>
       </c>
-      <c r="C31" s="128"/>
-      <c r="D31" s="128"/>
-      <c r="E31" s="126"/>
-      <c r="F31" s="126"/>
-      <c r="I31" s="48" t="s">
+      <c r="C32" s="128"/>
+      <c r="D32" s="128"/>
+      <c r="E32" s="126"/>
+      <c r="F32" s="126"/>
+      <c r="I32" s="48" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="63"/>
-      <c r="B32" s="121" t="s">
-        <v>64</v>
-      </c>
-      <c r="C32" s="121" t="s">
-        <v>14</v>
-      </c>
-      <c r="D32" s="121" t="s">
-        <v>58</v>
-      </c>
-      <c r="E32" s="120"/>
-      <c r="F32" s="120"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="63"/>
-      <c r="B33" s="88" t="s">
-        <v>42</v>
-      </c>
-      <c r="C33" s="89" t="s">
-        <v>144</v>
-      </c>
-      <c r="D33" s="88"/>
+      <c r="B33" s="121" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" s="121" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="121" t="s">
+        <v>58</v>
+      </c>
+      <c r="E33" s="120"/>
+      <c r="F33" s="120"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="63"/>
-      <c r="B34" s="66" t="s">
-        <v>236</v>
-      </c>
-      <c r="C34" s="67"/>
-      <c r="D34" s="67"/>
-      <c r="E34" s="113"/>
-      <c r="F34" s="113"/>
+      <c r="B34" s="88" t="s">
+        <v>42</v>
+      </c>
+      <c r="C34" s="89" t="s">
+        <v>144</v>
+      </c>
+      <c r="D34" s="88"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="63"/>
-      <c r="B35" s="69" t="s">
-        <v>343</v>
-      </c>
-      <c r="C35" s="64" t="s">
-        <v>341</v>
-      </c>
-      <c r="D35" s="64" t="s">
-        <v>77</v>
-      </c>
+      <c r="B35" s="66" t="s">
+        <v>236</v>
+      </c>
+      <c r="C35" s="67"/>
+      <c r="D35" s="67"/>
+      <c r="E35" s="113"/>
+      <c r="F35" s="113"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="63"/>
       <c r="B36" s="69" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C36" s="64" t="s">
-        <v>344</v>
-      </c>
-      <c r="D36" s="64"/>
+        <v>341</v>
+      </c>
+      <c r="D36" s="64" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="63"/>
       <c r="B37" s="69" t="s">
+        <v>342</v>
+      </c>
+      <c r="C37" s="64" t="s">
+        <v>344</v>
+      </c>
+      <c r="D37" s="64"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="63"/>
+      <c r="B38" s="69" t="s">
         <v>76</v>
       </c>
-      <c r="C37" s="64" t="s">
+      <c r="C38" s="64" t="s">
         <v>131</v>
       </c>
-      <c r="D37" s="64" t="s">
+      <c r="D38" s="64" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="65" t="s">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="65" t="s">
         <v>80</v>
       </c>
-      <c r="B38" s="69" t="s">
+      <c r="B39" s="69" t="s">
         <v>102</v>
       </c>
-      <c r="C38" s="64" t="s">
+      <c r="C39" s="64" t="s">
         <v>130</v>
-      </c>
-      <c r="D38" s="70" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="68"/>
-      <c r="B39" s="69" t="s">
-        <v>99</v>
-      </c>
-      <c r="C39" s="64" t="s">
-        <v>113</v>
       </c>
       <c r="D39" s="70" t="s">
         <v>158</v>
@@ -5842,184 +5846,186 @@
     <row r="40" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A40" s="68"/>
       <c r="B40" s="69" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C40" s="64" t="s">
-        <v>132</v>
-      </c>
-      <c r="D40" s="64" t="s">
-        <v>77</v>
+        <v>113</v>
+      </c>
+      <c r="D40" s="70" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="41" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A41" s="68"/>
-      <c r="B41" s="71" t="s">
-        <v>91</v>
-      </c>
-      <c r="C41" s="72" t="s">
-        <v>118</v>
-      </c>
-      <c r="D41" s="70" t="s">
-        <v>158</v>
+      <c r="B41" s="69" t="s">
+        <v>100</v>
+      </c>
+      <c r="C41" s="64" t="s">
+        <v>132</v>
+      </c>
+      <c r="D41" s="64" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="42" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A42" s="68"/>
-      <c r="B42" s="66" t="s">
-        <v>237</v>
-      </c>
-      <c r="C42" s="67" t="s">
-        <v>14</v>
-      </c>
-      <c r="D42" s="67"/>
-      <c r="E42" s="113"/>
-      <c r="F42" s="113"/>
+      <c r="B42" s="71" t="s">
+        <v>91</v>
+      </c>
+      <c r="C42" s="72" t="s">
+        <v>118</v>
+      </c>
+      <c r="D42" s="70" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="43" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A43" s="68"/>
-      <c r="B43" s="75" t="s">
+      <c r="B43" s="66" t="s">
+        <v>237</v>
+      </c>
+      <c r="C43" s="67" t="s">
+        <v>14</v>
+      </c>
+      <c r="D43" s="67"/>
+      <c r="E43" s="113"/>
+      <c r="F43" s="113"/>
+    </row>
+    <row r="44" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="68"/>
+      <c r="B44" s="75" t="s">
         <v>239</v>
       </c>
-      <c r="C43" s="76"/>
-      <c r="D43" s="76"/>
-      <c r="E43" s="114"/>
-      <c r="F43" s="114"/>
-    </row>
-    <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="73" t="s">
+      <c r="C44" s="76"/>
+      <c r="D44" s="76"/>
+      <c r="E44" s="114"/>
+      <c r="F44" s="114"/>
+    </row>
+    <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="73" t="s">
         <v>81</v>
       </c>
-      <c r="B44" s="77" t="s">
+      <c r="B45" s="77" t="s">
         <v>136</v>
       </c>
-      <c r="C44" s="70" t="s">
+      <c r="C45" s="70" t="s">
         <v>251</v>
-      </c>
-      <c r="D44" s="70"/>
-    </row>
-    <row r="45" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="74"/>
-      <c r="B45" s="77" t="s">
-        <v>78</v>
-      </c>
-      <c r="C45" s="70" t="s">
-        <v>252</v>
       </c>
       <c r="D45" s="70"/>
     </row>
     <row r="46" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A46" s="74"/>
       <c r="B46" s="77" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="C46" s="70" t="s">
-        <v>114</v>
-      </c>
-      <c r="D46" s="70" t="s">
-        <v>158</v>
-      </c>
+        <v>252</v>
+      </c>
+      <c r="D46" s="70"/>
     </row>
     <row r="47" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A47" s="74"/>
-      <c r="B47" s="75" t="s">
-        <v>238</v>
-      </c>
-      <c r="C47" s="76"/>
-      <c r="D47" s="76"/>
-      <c r="E47" s="114"/>
-      <c r="F47" s="114"/>
+      <c r="B47" s="77" t="s">
+        <v>101</v>
+      </c>
+      <c r="C47" s="70" t="s">
+        <v>114</v>
+      </c>
+      <c r="D47" s="70" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="48" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A48" s="74"/>
-      <c r="B48" s="77" t="s">
-        <v>104</v>
-      </c>
-      <c r="C48" s="78" t="s">
-        <v>133</v>
-      </c>
-      <c r="D48" s="70" t="s">
-        <v>158</v>
-      </c>
+      <c r="B48" s="75" t="s">
+        <v>238</v>
+      </c>
+      <c r="C48" s="76"/>
+      <c r="D48" s="76"/>
+      <c r="E48" s="114"/>
+      <c r="F48" s="114"/>
     </row>
     <row r="49" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A49" s="74"/>
       <c r="B49" s="77" t="s">
-        <v>142</v>
-      </c>
-      <c r="C49" s="70" t="s">
-        <v>253</v>
-      </c>
-      <c r="D49" s="72"/>
-      <c r="E49" s="64"/>
+        <v>104</v>
+      </c>
+      <c r="C49" s="78" t="s">
+        <v>133</v>
+      </c>
+      <c r="D49" s="70" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="50" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A50" s="74"/>
       <c r="B50" s="77" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C50" s="70" t="s">
-        <v>144</v>
+        <v>253</v>
       </c>
       <c r="D50" s="72"/>
+      <c r="E50" s="64"/>
     </row>
     <row r="51" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A51" s="74"/>
-      <c r="B51" s="66" t="s">
-        <v>240</v>
-      </c>
-      <c r="C51" s="67"/>
-      <c r="D51" s="67"/>
-      <c r="E51" s="113"/>
-      <c r="F51" s="113"/>
+      <c r="B51" s="77" t="s">
+        <v>143</v>
+      </c>
+      <c r="C51" s="70" t="s">
+        <v>144</v>
+      </c>
+      <c r="D51" s="72"/>
     </row>
     <row r="52" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A52" s="74"/>
-      <c r="B52" s="80" t="s">
+      <c r="B52" s="66" t="s">
+        <v>240</v>
+      </c>
+      <c r="C52" s="67"/>
+      <c r="D52" s="67"/>
+      <c r="E52" s="113"/>
+      <c r="F52" s="113"/>
+    </row>
+    <row r="53" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="74"/>
+      <c r="B53" s="80" t="s">
         <v>241</v>
       </c>
-      <c r="C52" s="81"/>
-      <c r="D52" s="81"/>
-      <c r="E52" s="114"/>
-      <c r="F52" s="114"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="74"/>
-      <c r="B53" s="77" t="s">
-        <v>103</v>
-      </c>
-      <c r="C53" s="83" t="s">
-        <v>250</v>
-      </c>
-      <c r="D53" s="72" t="s">
-        <v>77</v>
-      </c>
+      <c r="C53" s="81"/>
+      <c r="D53" s="81"/>
+      <c r="E53" s="114"/>
+      <c r="F53" s="114"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="74"/>
       <c r="B54" s="77" t="s">
+        <v>103</v>
+      </c>
+      <c r="C54" s="83" t="s">
+        <v>250</v>
+      </c>
+      <c r="D54" s="72" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="74"/>
+      <c r="B55" s="77" t="s">
         <v>345</v>
       </c>
-      <c r="C54" s="83" t="s">
+      <c r="C55" s="83" t="s">
         <v>346</v>
       </c>
-      <c r="D54" s="72"/>
-    </row>
-    <row r="55" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="79" t="s">
+      <c r="D55" s="72"/>
+    </row>
+    <row r="56" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="79" t="s">
         <v>82</v>
       </c>
-      <c r="B55" s="80" t="s">
+      <c r="B56" s="80" t="s">
         <v>242</v>
-      </c>
-      <c r="C55" s="81"/>
-      <c r="D55" s="81"/>
-      <c r="E55" s="114"/>
-      <c r="F55" s="114"/>
-    </row>
-    <row r="56" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="82"/>
-      <c r="B56" s="80" t="s">
-        <v>243</v>
       </c>
       <c r="C56" s="81"/>
       <c r="D56" s="81"/>
@@ -6028,65 +6034,63 @@
     </row>
     <row r="57" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A57" s="82"/>
-      <c r="B57" s="84" t="s">
-        <v>206</v>
-      </c>
-      <c r="C57" s="86" t="s">
-        <v>216</v>
-      </c>
-      <c r="D57" s="72"/>
+      <c r="B57" s="80" t="s">
+        <v>243</v>
+      </c>
+      <c r="C57" s="81"/>
+      <c r="D57" s="81"/>
+      <c r="E57" s="114"/>
+      <c r="F57" s="114"/>
     </row>
     <row r="58" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A58" s="82"/>
       <c r="B58" s="84" t="s">
-        <v>207</v>
-      </c>
-      <c r="C58" s="48" t="s">
-        <v>208</v>
-      </c>
-      <c r="D58" s="72" t="s">
-        <v>77</v>
-      </c>
+        <v>206</v>
+      </c>
+      <c r="C58" s="86" t="s">
+        <v>216</v>
+      </c>
+      <c r="D58" s="72"/>
     </row>
     <row r="59" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A59" s="82"/>
       <c r="B59" s="84" t="s">
-        <v>169</v>
-      </c>
-      <c r="C59" s="85" t="s">
-        <v>215</v>
-      </c>
-      <c r="D59" s="72"/>
+        <v>207</v>
+      </c>
+      <c r="C59" s="48" t="s">
+        <v>208</v>
+      </c>
+      <c r="D59" s="72" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="60" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A60" s="82"/>
-      <c r="B60" s="80" t="s">
-        <v>244</v>
-      </c>
-      <c r="C60" s="81"/>
-      <c r="D60" s="81"/>
-      <c r="E60" s="114"/>
-      <c r="F60" s="114"/>
+      <c r="B60" s="84" t="s">
+        <v>169</v>
+      </c>
+      <c r="C60" s="85" t="s">
+        <v>215</v>
+      </c>
+      <c r="D60" s="72"/>
     </row>
     <row r="61" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A61" s="82"/>
-      <c r="B61" s="84" t="s">
-        <v>85</v>
-      </c>
-      <c r="C61" s="86" t="s">
-        <v>254</v>
-      </c>
-      <c r="D61" s="72" t="s">
-        <v>77</v>
-      </c>
+      <c r="B61" s="80" t="s">
+        <v>244</v>
+      </c>
+      <c r="C61" s="81"/>
+      <c r="D61" s="81"/>
+      <c r="E61" s="114"/>
+      <c r="F61" s="114"/>
     </row>
     <row r="62" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A62" s="82"/>
       <c r="B62" s="84" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C62" s="86" t="s">
-        <v>134</v>
+        <v>254</v>
       </c>
       <c r="D62" s="72" t="s">
         <v>77</v>
@@ -6094,121 +6098,121 @@
     </row>
     <row r="63" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A63" s="82"/>
-      <c r="B63" s="66" t="s">
-        <v>245</v>
-      </c>
-      <c r="C63" s="67"/>
-      <c r="D63" s="67"/>
-      <c r="E63" s="113"/>
-      <c r="F63" s="113"/>
+      <c r="B63" s="84" t="s">
+        <v>84</v>
+      </c>
+      <c r="C63" s="86" t="s">
+        <v>134</v>
+      </c>
+      <c r="D63" s="72" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="64" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A64" s="82"/>
-      <c r="B64" s="71" t="s">
+      <c r="B64" s="66" t="s">
+        <v>245</v>
+      </c>
+      <c r="C64" s="67"/>
+      <c r="D64" s="67"/>
+      <c r="E64" s="113"/>
+      <c r="F64" s="113"/>
+    </row>
+    <row r="65" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="82"/>
+      <c r="B65" s="71" t="s">
         <v>86</v>
       </c>
-      <c r="C64" s="72" t="s">
+      <c r="C65" s="72" t="s">
         <v>135</v>
       </c>
-      <c r="D64" s="72" t="s">
+      <c r="D65" s="72" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" s="65" t="s">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" s="65" t="s">
         <v>83</v>
       </c>
-      <c r="B65" s="66" t="s">
+      <c r="B66" s="66" t="s">
         <v>246</v>
       </c>
-      <c r="C65" s="67"/>
-      <c r="D65" s="67"/>
-      <c r="E65" s="113"/>
-      <c r="F65" s="113"/>
-    </row>
-    <row r="66" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="65"/>
-      <c r="B66" s="71" t="s">
+      <c r="C66" s="67"/>
+      <c r="D66" s="67"/>
+      <c r="E66" s="113"/>
+      <c r="F66" s="113"/>
+    </row>
+    <row r="67" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="65"/>
+      <c r="B67" s="71" t="s">
         <v>153</v>
       </c>
-      <c r="C66" s="72" t="s">
+      <c r="C67" s="72" t="s">
         <v>152</v>
       </c>
-      <c r="D66" s="70"/>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B67" s="71" t="s">
+      <c r="D67" s="70"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B68" s="71" t="s">
         <v>154</v>
       </c>
-      <c r="C67" s="72" t="s">
+      <c r="C68" s="72" t="s">
         <v>155</v>
       </c>
-      <c r="D67" s="70"/>
-    </row>
-    <row r="68" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B68" s="66" t="s">
+      <c r="D68" s="70"/>
+    </row>
+    <row r="69" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B69" s="66" t="s">
         <v>247</v>
       </c>
-      <c r="C68" s="67"/>
-      <c r="D68" s="67"/>
-      <c r="E68" s="67"/>
-      <c r="F68" s="67"/>
-    </row>
-    <row r="69" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B69" s="54"/>
-      <c r="C69" s="55"/>
-      <c r="D69" s="55"/>
-      <c r="E69" s="55"/>
-      <c r="F69" s="55"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70" s="51"/>
-      <c r="B70" s="122" t="s">
+      <c r="C69" s="67"/>
+      <c r="D69" s="67"/>
+      <c r="E69" s="67"/>
+      <c r="F69" s="67"/>
+    </row>
+    <row r="70" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B70" s="54"/>
+      <c r="C70" s="55"/>
+      <c r="D70" s="55"/>
+      <c r="E70" s="55"/>
+      <c r="F70" s="55"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" s="51"/>
+      <c r="B71" s="122" t="s">
         <v>322</v>
       </c>
-      <c r="C70" s="67"/>
-      <c r="D70" s="67"/>
-      <c r="E70" s="113"/>
-      <c r="F70" s="113"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B71" s="71" t="s">
+      <c r="C71" s="67"/>
+      <c r="D71" s="67"/>
+      <c r="E71" s="113"/>
+      <c r="F71" s="113"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B72" s="71" t="s">
         <v>323</v>
       </c>
-      <c r="C71" s="72" t="s">
+      <c r="C72" s="72" t="s">
         <v>324</v>
       </c>
-      <c r="D71" s="70"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72" s="51"/>
-      <c r="B72" s="122" t="s">
-        <v>265</v>
-      </c>
-      <c r="C72" s="67"/>
-      <c r="D72" s="67"/>
-      <c r="E72" s="113"/>
-      <c r="F72" s="113"/>
+      <c r="D72" s="70"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="51"/>
-      <c r="B73" s="123" t="s">
-        <v>261</v>
-      </c>
-      <c r="C73" s="105" t="s">
-        <v>268</v>
-      </c>
-      <c r="D73" s="55"/>
-      <c r="E73" s="64"/>
-      <c r="F73" s="64"/>
+      <c r="B73" s="122" t="s">
+        <v>265</v>
+      </c>
+      <c r="C73" s="67"/>
+      <c r="D73" s="67"/>
+      <c r="E73" s="113"/>
+      <c r="F73" s="113"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="51"/>
       <c r="B74" s="123" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C74" s="105" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D74" s="55"/>
       <c r="E74" s="64"/>
@@ -6217,10 +6221,10 @@
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="51"/>
       <c r="B75" s="123" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="C75" s="105" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D75" s="55"/>
       <c r="E75" s="64"/>
@@ -6229,10 +6233,10 @@
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="51"/>
       <c r="B76" s="123" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C76" s="105" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D76" s="55"/>
       <c r="E76" s="64"/>
@@ -6241,10 +6245,10 @@
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="51"/>
       <c r="B77" s="123" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C77" s="105" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D77" s="55"/>
       <c r="E77" s="64"/>
@@ -6252,391 +6256,403 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="51"/>
-      <c r="B78" s="122" t="s">
-        <v>266</v>
-      </c>
-      <c r="C78" s="67"/>
-      <c r="D78" s="67"/>
-      <c r="E78" s="113"/>
-      <c r="F78" s="113"/>
+      <c r="B78" s="123" t="s">
+        <v>263</v>
+      </c>
+      <c r="C78" s="105" t="s">
+        <v>272</v>
+      </c>
+      <c r="D78" s="55"/>
+      <c r="E78" s="64"/>
+      <c r="F78" s="64"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="51"/>
-      <c r="B79" s="123" t="s">
+      <c r="B79" s="122" t="s">
+        <v>266</v>
+      </c>
+      <c r="C79" s="67"/>
+      <c r="D79" s="67"/>
+      <c r="E79" s="113"/>
+      <c r="F79" s="113"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A80" s="51"/>
+      <c r="B80" s="123" t="s">
         <v>339</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C80" t="s">
         <v>340</v>
       </c>
-      <c r="D79"/>
-      <c r="E79"/>
-      <c r="F79"/>
-    </row>
-    <row r="80" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B80" s="123" t="s">
+      <c r="D80"/>
+      <c r="E80"/>
+      <c r="F80"/>
+    </row>
+    <row r="81" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B81" s="123" t="s">
         <v>267</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C81" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="81" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B81" s="122" t="s">
+    <row r="82" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B82" s="122" t="s">
         <v>280</v>
       </c>
-      <c r="C81" s="130"/>
-      <c r="D81" s="130"/>
-      <c r="E81" s="130"/>
-      <c r="F81" s="130"/>
-    </row>
-    <row r="82" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B82" s="132" t="s">
+      <c r="C82" s="130"/>
+      <c r="D82" s="130"/>
+      <c r="E82" s="130"/>
+      <c r="F82" s="130"/>
+    </row>
+    <row r="83" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B83" s="132" t="s">
         <v>310</v>
       </c>
-      <c r="C82" s="131" t="s">
+      <c r="C83" s="131" t="s">
         <v>281</v>
       </c>
-      <c r="D82" s="131"/>
-      <c r="E82" s="131"/>
-      <c r="F82" s="131"/>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A83" s="51"/>
-      <c r="B83" s="127" t="s">
-        <v>248</v>
-      </c>
-      <c r="C83" s="129"/>
-      <c r="D83" s="129"/>
-      <c r="E83" s="129"/>
-      <c r="F83" s="129"/>
+      <c r="D83" s="131"/>
+      <c r="E83" s="131"/>
+      <c r="F83" s="131"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="51"/>
-      <c r="B84" s="88" t="s">
-        <v>117</v>
-      </c>
-      <c r="C84" s="89" t="s">
-        <v>116</v>
-      </c>
-      <c r="D84" s="88"/>
+      <c r="B84" s="127" t="s">
+        <v>248</v>
+      </c>
+      <c r="C84" s="129"/>
+      <c r="D84" s="129"/>
+      <c r="E84" s="129"/>
+      <c r="F84" s="129"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="51"/>
       <c r="B85" s="88" t="s">
+        <v>117</v>
+      </c>
+      <c r="C85" s="89" t="s">
+        <v>116</v>
+      </c>
+      <c r="D85" s="88"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86" s="51"/>
+      <c r="B86" s="88" t="s">
         <v>311</v>
       </c>
-      <c r="C85" s="89" t="s">
+      <c r="C86" s="89" t="s">
         <v>312</v>
-      </c>
-      <c r="D85" s="88"/>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A86" s="52"/>
-      <c r="B86" s="88" t="s">
-        <v>140</v>
-      </c>
-      <c r="C86" s="89" t="s">
-        <v>141</v>
       </c>
       <c r="D86" s="88"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="52"/>
       <c r="B87" s="88" t="s">
+        <v>140</v>
+      </c>
+      <c r="C87" s="89" t="s">
+        <v>141</v>
+      </c>
+      <c r="D87" s="88"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A88" s="52"/>
+      <c r="B88" s="88" t="s">
         <v>323</v>
       </c>
-      <c r="C87" s="89" t="s">
+      <c r="C88" s="89" t="s">
         <v>325</v>
       </c>
-      <c r="D87" s="88"/>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A88" s="87"/>
-      <c r="B88" s="69" t="s">
-        <v>111</v>
-      </c>
-      <c r="C88" s="64" t="s">
-        <v>115</v>
-      </c>
-      <c r="D88" s="64"/>
+      <c r="D88" s="88"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="87"/>
-      <c r="B89" s="142" t="s">
-        <v>313</v>
-      </c>
-      <c r="C89" s="119"/>
-      <c r="D89" s="119"/>
-      <c r="E89" s="119"/>
-      <c r="F89" s="119"/>
+      <c r="B89" s="69" t="s">
+        <v>111</v>
+      </c>
+      <c r="C89" s="64" t="s">
+        <v>115</v>
+      </c>
+      <c r="D89" s="64"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" s="87"/>
-      <c r="B90" s="71" t="s">
-        <v>119</v>
-      </c>
-      <c r="C90" s="72" t="s">
-        <v>361</v>
-      </c>
-      <c r="D90" s="72"/>
+      <c r="B90" s="142" t="s">
+        <v>313</v>
+      </c>
+      <c r="C90" s="119"/>
+      <c r="D90" s="119"/>
+      <c r="E90" s="119"/>
+      <c r="F90" s="119"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="87"/>
       <c r="B91" s="71" t="s">
-        <v>315</v>
+        <v>119</v>
       </c>
       <c r="C91" s="72" t="s">
-        <v>314</v>
+        <v>361</v>
       </c>
       <c r="D91" s="72"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" s="87"/>
       <c r="B92" s="71" t="s">
+        <v>315</v>
+      </c>
+      <c r="C92" s="72" t="s">
+        <v>314</v>
+      </c>
+      <c r="D92" s="72"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A93" s="87"/>
+      <c r="B93" s="71" t="s">
         <v>316</v>
       </c>
-      <c r="C92" s="72" t="s">
+      <c r="C93" s="72" t="s">
         <v>317</v>
       </c>
-      <c r="D92" s="72"/>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A93" s="119" t="s">
+      <c r="D93" s="72"/>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A94" s="119" t="s">
         <v>249</v>
       </c>
-      <c r="B93" s="142" t="s">
+      <c r="B94" s="142" t="s">
         <v>318</v>
       </c>
-      <c r="C93" s="119"/>
-      <c r="D93" s="119"/>
-      <c r="E93" s="119"/>
-      <c r="F93" s="119"/>
-    </row>
-    <row r="94" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="90"/>
-      <c r="B94" s="71" t="s">
+      <c r="C94" s="119"/>
+      <c r="D94" s="119"/>
+      <c r="E94" s="119"/>
+      <c r="F94" s="119"/>
+    </row>
+    <row r="95" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="90"/>
+      <c r="B95" s="71" t="s">
         <v>38</v>
       </c>
-      <c r="C94" s="72" t="s">
+      <c r="C95" s="72" t="s">
         <v>162</v>
       </c>
-      <c r="D94" s="72"/>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A95" s="119" t="s">
+      <c r="D95" s="72"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A96" s="119" t="s">
         <v>256</v>
       </c>
-      <c r="B95" s="71" t="s">
+      <c r="B96" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="C95" s="72" t="s">
+      <c r="C96" s="72" t="s">
         <v>157</v>
       </c>
-      <c r="D95" s="72"/>
-    </row>
-    <row r="96" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="90"/>
-      <c r="B96" s="71" t="s">
+      <c r="D96" s="72"/>
+    </row>
+    <row r="97" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="90"/>
+      <c r="B97" s="71" t="s">
         <v>199</v>
       </c>
-      <c r="C96" s="110" t="s">
+      <c r="C97" s="110" t="s">
         <v>200</v>
-      </c>
-      <c r="D96" s="72"/>
-    </row>
-    <row r="97" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="91"/>
-      <c r="B97" s="71" t="s">
-        <v>202</v>
-      </c>
-      <c r="C97" s="110" t="s">
-        <v>203</v>
       </c>
       <c r="D97" s="72"/>
     </row>
     <row r="98" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A98" s="91"/>
       <c r="B98" s="71" t="s">
-        <v>320</v>
+        <v>202</v>
       </c>
       <c r="C98" s="110" t="s">
-        <v>319</v>
+        <v>203</v>
       </c>
       <c r="D98" s="72"/>
     </row>
     <row r="99" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A99" s="91"/>
-      <c r="B99" s="142" t="s">
-        <v>321</v>
-      </c>
-      <c r="C99" s="119"/>
-      <c r="D99" s="119"/>
-      <c r="E99" s="119"/>
-      <c r="F99" s="119"/>
+      <c r="B99" s="71" t="s">
+        <v>320</v>
+      </c>
+      <c r="C99" s="110" t="s">
+        <v>319</v>
+      </c>
+      <c r="D99" s="72"/>
     </row>
     <row r="100" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A100" s="91"/>
-      <c r="B100" s="75" t="s">
+      <c r="B100" s="142" t="s">
+        <v>321</v>
+      </c>
+      <c r="C100" s="119"/>
+      <c r="D100" s="119"/>
+      <c r="E100" s="119"/>
+      <c r="F100" s="119"/>
+    </row>
+    <row r="101" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="91"/>
+      <c r="B101" s="75" t="s">
         <v>258</v>
       </c>
-      <c r="C100" s="93"/>
-      <c r="D100" s="93"/>
-      <c r="E100" s="93"/>
-      <c r="F100" s="93"/>
-    </row>
-    <row r="101" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="119" t="s">
+      <c r="C101" s="93"/>
+      <c r="D101" s="93"/>
+      <c r="E101" s="93"/>
+      <c r="F101" s="93"/>
+    </row>
+    <row r="102" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A102" s="119" t="s">
         <v>257</v>
       </c>
-      <c r="B101" s="84" t="s">
+      <c r="B102" s="84" t="s">
         <v>90</v>
       </c>
-      <c r="C101" s="72" t="s">
+      <c r="C102" s="72" t="s">
         <v>159</v>
       </c>
-      <c r="D101" s="72"/>
-    </row>
-    <row r="102" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="92"/>
-      <c r="B102" s="84" t="s">
+      <c r="D102" s="72"/>
+    </row>
+    <row r="103" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A103" s="92"/>
+      <c r="B103" s="84" t="s">
         <v>89</v>
       </c>
-      <c r="C102" s="72" t="s">
+      <c r="C103" s="72" t="s">
         <v>160</v>
       </c>
-      <c r="D102" s="72"/>
-    </row>
-    <row r="103" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="94"/>
-      <c r="B103" s="75" t="s">
-        <v>259</v>
-      </c>
-      <c r="C103" s="93"/>
-      <c r="D103" s="93"/>
-      <c r="E103" s="93"/>
-      <c r="F103" s="93"/>
+      <c r="D103" s="72"/>
     </row>
     <row r="104" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A104" s="94"/>
-      <c r="B104" s="118" t="s">
-        <v>137</v>
-      </c>
-      <c r="C104" s="72" t="s">
-        <v>138</v>
-      </c>
-      <c r="D104" s="72"/>
+      <c r="B104" s="75" t="s">
+        <v>259</v>
+      </c>
+      <c r="C104" s="93"/>
+      <c r="D104" s="93"/>
+      <c r="E104" s="93"/>
+      <c r="F104" s="93"/>
     </row>
     <row r="105" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="92"/>
+      <c r="A105" s="94"/>
       <c r="B105" s="118" t="s">
         <v>137</v>
       </c>
       <c r="C105" s="72" t="s">
+        <v>138</v>
+      </c>
+      <c r="D105" s="72"/>
+    </row>
+    <row r="106" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="92"/>
+      <c r="B106" s="118" t="s">
+        <v>137</v>
+      </c>
+      <c r="C106" s="72" t="s">
         <v>233</v>
       </c>
-      <c r="D105" s="72"/>
-    </row>
-    <row r="106" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="94"/>
-      <c r="B106" s="118" t="s">
+      <c r="D106" s="72"/>
+    </row>
+    <row r="107" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="94"/>
+      <c r="B107" s="118" t="s">
         <v>191</v>
       </c>
-      <c r="C106" s="72" t="s">
+      <c r="C107" s="72" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="107" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B109" s="106" t="s">
+    <row r="108" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2"/>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B110" s="106" t="s">
         <v>192</v>
       </c>
-      <c r="C109" s="106" t="s">
+      <c r="C110" s="106" t="s">
         <v>196</v>
       </c>
-      <c r="D109" s="149" t="s">
+      <c r="D110" s="149" t="s">
         <v>197</v>
       </c>
-      <c r="E109" s="149"/>
-      <c r="F109" s="149"/>
-    </row>
-    <row r="110" spans="1:6" ht="127.5" x14ac:dyDescent="0.2">
-      <c r="B110" s="109" t="s">
+      <c r="E110" s="149"/>
+      <c r="F110" s="149"/>
+    </row>
+    <row r="111" spans="1:6" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="B111" s="109" t="s">
         <v>193</v>
       </c>
-      <c r="C110" s="108" t="s">
+      <c r="C111" s="108" t="s">
         <v>205</v>
       </c>
-      <c r="D110" s="150" t="s">
+      <c r="D111" s="150" t="s">
         <v>198</v>
-      </c>
-      <c r="E110" s="150"/>
-      <c r="F110" s="150"/>
-    </row>
-    <row r="111" spans="1:6" ht="102" x14ac:dyDescent="0.2">
-      <c r="B111" s="109" t="s">
-        <v>194</v>
-      </c>
-      <c r="C111" s="115" t="s">
-        <v>204</v>
-      </c>
-      <c r="D111" s="150" t="s">
-        <v>201</v>
       </c>
       <c r="E111" s="150"/>
       <c r="F111" s="150"/>
     </row>
-    <row r="112" spans="1:6" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="B112" s="109" t="s">
-        <v>195</v>
-      </c>
-      <c r="C112" s="108" t="s">
-        <v>209</v>
+        <v>194</v>
+      </c>
+      <c r="C112" s="115" t="s">
+        <v>204</v>
       </c>
       <c r="D112" s="150" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="E112" s="150"/>
       <c r="F112" s="150"/>
     </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B113" s="117"/>
-    </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B114" s="116" t="s">
+    <row r="113" spans="2:6" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="B113" s="109" t="s">
+        <v>195</v>
+      </c>
+      <c r="C113" s="108" t="s">
+        <v>209</v>
+      </c>
+      <c r="D113" s="150" t="s">
+        <v>210</v>
+      </c>
+      <c r="E113" s="150"/>
+      <c r="F113" s="150"/>
+    </row>
+    <row r="114" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B114" s="117"/>
+    </row>
+    <row r="115" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B115" s="116" t="s">
         <v>218</v>
       </c>
-      <c r="C114" s="116" t="s">
+      <c r="C115" s="116" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="115" spans="2:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="B115" s="117" t="s">
+    <row r="116" spans="2:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="B116" s="117" t="s">
         <v>219</v>
       </c>
-      <c r="C115" s="108" t="s">
+      <c r="C116" s="108" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="116" spans="2:3" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="B116" s="117" t="s">
+    <row r="117" spans="2:6" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="B117" s="117" t="s">
         <v>220</v>
       </c>
-      <c r="C116" s="108" t="s">
+      <c r="C117" s="108" t="s">
         <v>222</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
+    <mergeCell ref="D113:F113"/>
     <mergeCell ref="D112:F112"/>
     <mergeCell ref="D111:F111"/>
     <mergeCell ref="D110:F110"/>
-    <mergeCell ref="D109:F109"/>
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D110" r:id="rId1"/>
-    <hyperlink ref="D111" r:id="rId2"/>
-    <hyperlink ref="D112" r:id="rId3"/>
+    <hyperlink ref="D111" r:id="rId1"/>
+    <hyperlink ref="D112" r:id="rId2"/>
+    <hyperlink ref="D113" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>

</xml_diff>

<commit_message>
Se tomó en cuenta el Informe de resultados dentro de la carpeta de Organización/Capacitaciones
</commit_message>
<xml_diff>
--- a/Organización/Procesos/Soporte Organizacional/2. Administración de Configuración/IWM_Administración de la Configuración.xlsx
+++ b/Organización/Procesos/Soporte Organizacional/2. Administración de Configuración/IWM_Administración de la Configuración.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="366">
   <si>
     <t>Adapiaciones al Estándar de Administración de Datos</t>
   </si>
@@ -729,12 +729,6 @@
   </si>
   <si>
     <t>Entrega del proyecto al cliente aprobada</t>
-  </si>
-  <si>
-    <t>IWM_Minuta_Seguimiento_aammdd</t>
-  </si>
-  <si>
-    <t>IWM_Presentación_Seguimiento_aammdd</t>
   </si>
   <si>
     <r>
@@ -1497,16 +1491,10 @@
     </r>
   </si>
   <si>
-    <t>IWM_Auditoria_Organizacional_aammdd</t>
-  </si>
-  <si>
     <t xml:space="preserve">Check list organizacional </t>
   </si>
   <si>
     <t>Reporte conformidades</t>
-  </si>
-  <si>
-    <t>IWM_Reporte_no conformidades_aammdd</t>
   </si>
   <si>
     <r>
@@ -1770,31 +1758,49 @@
     <t>Concentrado_Mejoras_aaaa</t>
   </si>
   <si>
-    <t>EC_&lt;tipo de capacitación o proceso&gt;_aammdd</t>
-  </si>
-  <si>
-    <t>LA_&lt;tipo de capacitación o proceso&gt;_aammdd</t>
-  </si>
-  <si>
-    <t>SC_&lt;tipo de capacitación o proceso&gt;_aammdd</t>
-  </si>
-  <si>
-    <t>M_&lt;tipo de capacitación o proceso&gt;_aammdd</t>
-  </si>
-  <si>
-    <t>SM_&lt;tipo de capacitación o proceso&gt;_aammdd</t>
-  </si>
-  <si>
-    <t>IWM_Reporte de actividades_aammdd</t>
-  </si>
-  <si>
     <t>IWM_PlanAseguramientoCalidad</t>
   </si>
   <si>
-    <t>EE_&lt;tipo de capacitación o proceso&gt;_aammdd</t>
-  </si>
-  <si>
     <t>Evaluación de Efectividad</t>
+  </si>
+  <si>
+    <t>Informe de Resultados</t>
+  </si>
+  <si>
+    <t>Informe de resultados_aaaa</t>
+  </si>
+  <si>
+    <t>IWM_Reporte de actividades_mmddaa</t>
+  </si>
+  <si>
+    <t>SM_&lt;tipo de capacitación o proceso&gt;_mmddaa</t>
+  </si>
+  <si>
+    <t>M_&lt;tipo de capacitación o proceso&gt;_mmddaa</t>
+  </si>
+  <si>
+    <t>EC_&lt;tipo de capacitación o proceso&gt;_mmddaa</t>
+  </si>
+  <si>
+    <t>EE_&lt;tipo de capacitación o proceso&gt;_mmddaa</t>
+  </si>
+  <si>
+    <t>LA_&lt;tipo de capacitación o proceso&gt;_mmddaa</t>
+  </si>
+  <si>
+    <t>SC_&lt;tipo de capacitación o proceso&gt;_mmddaa</t>
+  </si>
+  <si>
+    <t>IWM_Minuta_Seguimiento_mmddaa</t>
+  </si>
+  <si>
+    <t>IWM_Presentación_Seguimiento_mmddaa</t>
+  </si>
+  <si>
+    <t>IWM_Reporte_no conformidades_mmddaa</t>
+  </si>
+  <si>
+    <t>IWM_Auditoria_Organizacional_mmddaa</t>
   </si>
 </sst>
 </file>
@@ -4913,7 +4919,7 @@
         <v>136</v>
       </c>
       <c r="B15" s="70" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="C15" s="70"/>
     </row>
@@ -5304,7 +5310,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="122" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B54" s="130"/>
       <c r="C54" s="130"/>
@@ -5313,10 +5319,10 @@
     </row>
     <row r="55" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="132" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B55" s="131" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C55" s="131"/>
       <c r="D55" s="131"/>
@@ -5412,10 +5418,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I117"/>
+  <dimension ref="A1:I118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C97" sqref="C97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -5465,25 +5471,25 @@
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="49"/>
       <c r="B4" s="48" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="C4" s="48" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="49"/>
       <c r="B5" s="48" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C5" s="48" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="49"/>
       <c r="B6" s="59" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C6" s="53"/>
       <c r="D6" s="53"/>
@@ -5493,25 +5499,25 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="49"/>
       <c r="B7" s="48" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C7" s="48" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="49"/>
       <c r="B8" s="48" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="C8" s="48" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="49"/>
       <c r="B9" s="127" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="C9" s="128"/>
       <c r="D9" s="128"/>
@@ -5521,17 +5527,17 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="49"/>
       <c r="B10" s="88" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="C10" s="89" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="D10" s="88"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="49"/>
       <c r="B11" s="127" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="C11" s="128"/>
       <c r="D11" s="128"/>
@@ -5541,40 +5547,40 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="49"/>
       <c r="B12" s="88" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="C12" s="89" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="D12" s="88"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="62"/>
       <c r="B13" s="127" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="C13" s="128"/>
       <c r="D13" s="128"/>
       <c r="E13" s="126"/>
       <c r="F13" s="126"/>
       <c r="I13" s="48" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="63"/>
       <c r="B14" s="88" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="C14" s="89" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D14" s="88"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="49"/>
       <c r="B15" s="59" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="C15" s="53"/>
       <c r="D15" s="53"/>
@@ -5584,458 +5590,457 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="49"/>
       <c r="B16" s="48" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="C16" s="48" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="49"/>
-      <c r="B17" s="127" t="s">
-        <v>350</v>
-      </c>
-      <c r="C17" s="128"/>
-      <c r="D17" s="128"/>
-      <c r="E17" s="126"/>
-      <c r="F17" s="126"/>
+      <c r="B17" s="48" t="s">
+        <v>353</v>
+      </c>
+      <c r="C17" s="48" t="s">
+        <v>354</v>
+      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="49"/>
-      <c r="B18" s="88" t="s">
-        <v>261</v>
-      </c>
-      <c r="C18" s="89" t="s">
-        <v>355</v>
-      </c>
-      <c r="D18" s="88"/>
+      <c r="B18" s="127" t="s">
+        <v>346</v>
+      </c>
+      <c r="C18" s="128"/>
+      <c r="D18" s="128"/>
+      <c r="E18" s="126"/>
+      <c r="F18" s="126"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="49"/>
       <c r="B19" s="88" t="s">
-        <v>363</v>
+        <v>259</v>
       </c>
       <c r="C19" s="89" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="D19" s="88"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="49"/>
-      <c r="B20" s="127" t="s">
-        <v>351</v>
-      </c>
-      <c r="C20" s="128"/>
-      <c r="D20" s="128"/>
-      <c r="E20" s="126"/>
-      <c r="F20" s="126"/>
+      <c r="B20" s="88" t="s">
+        <v>352</v>
+      </c>
+      <c r="C20" s="89" t="s">
+        <v>359</v>
+      </c>
+      <c r="D20" s="88"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="49"/>
-      <c r="B21" s="88" t="s">
-        <v>263</v>
-      </c>
-      <c r="C21" s="89" t="s">
-        <v>356</v>
-      </c>
-      <c r="D21" s="88"/>
+      <c r="B21" s="127" t="s">
+        <v>347</v>
+      </c>
+      <c r="C21" s="128"/>
+      <c r="D21" s="128"/>
+      <c r="E21" s="126"/>
+      <c r="F21" s="126"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="49"/>
-      <c r="B22" s="127" t="s">
-        <v>334</v>
-      </c>
-      <c r="C22" s="128"/>
-      <c r="D22" s="128"/>
-      <c r="E22" s="126"/>
-      <c r="F22" s="126"/>
+      <c r="B22" s="88" t="s">
+        <v>261</v>
+      </c>
+      <c r="C22" s="89" t="s">
+        <v>360</v>
+      </c>
+      <c r="D22" s="88"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="49"/>
-      <c r="B23" s="88" t="s">
-        <v>352</v>
-      </c>
-      <c r="C23" s="89" t="s">
+      <c r="B23" s="127" t="s">
+        <v>330</v>
+      </c>
+      <c r="C23" s="128"/>
+      <c r="D23" s="128"/>
+      <c r="E23" s="126"/>
+      <c r="F23" s="126"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="49"/>
+      <c r="B24" s="88" t="s">
+        <v>348</v>
+      </c>
+      <c r="C24" s="89" t="s">
+        <v>361</v>
+      </c>
+      <c r="D24" s="88"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="62"/>
+      <c r="B25" s="127" t="s">
+        <v>322</v>
+      </c>
+      <c r="C25" s="128"/>
+      <c r="D25" s="128"/>
+      <c r="E25" s="126"/>
+      <c r="F25" s="126"/>
+      <c r="I25" s="48" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="63"/>
+      <c r="B26" s="88" t="s">
+        <v>323</v>
+      </c>
+      <c r="C26" s="89" t="s">
         <v>357</v>
       </c>
-      <c r="D23" s="88"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="62"/>
-      <c r="B24" s="127" t="s">
-        <v>326</v>
-      </c>
-      <c r="C24" s="128"/>
-      <c r="D24" s="128"/>
-      <c r="E24" s="126"/>
-      <c r="F24" s="126"/>
-      <c r="I24" s="48" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="63"/>
-      <c r="B25" s="88" t="s">
-        <v>327</v>
-      </c>
-      <c r="C25" s="89" t="s">
-        <v>358</v>
-      </c>
-      <c r="D25" s="88"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="51"/>
-      <c r="B26" s="51"/>
-      <c r="C26" s="51"/>
-      <c r="D26" s="51"/>
-      <c r="E26" s="51"/>
-      <c r="F26" s="51"/>
-      <c r="I26" s="125" t="s">
+      <c r="D26" s="88"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="51"/>
+      <c r="B27" s="51"/>
+      <c r="C27" s="51"/>
+      <c r="D27" s="51"/>
+      <c r="E27" s="51"/>
+      <c r="F27" s="51"/>
+      <c r="I27" s="125" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="52"/>
+      <c r="B28" s="59" t="s">
+        <v>232</v>
+      </c>
+      <c r="C28" s="53"/>
+      <c r="D28" s="53"/>
+      <c r="E28" s="53"/>
+      <c r="F28" s="53"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B29" s="48" t="s">
+        <v>112</v>
+      </c>
+      <c r="C29" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="H29" s="124"/>
+      <c r="I29" s="48" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H30" s="126"/>
+      <c r="I30" s="48" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="51"/>
+      <c r="B31" s="51"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="51"/>
+      <c r="F31" s="51"/>
+      <c r="H31" s="113"/>
+      <c r="I31" s="48" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="52"/>
-      <c r="B27" s="59" t="s">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="52"/>
+      <c r="B32" s="60" t="s">
+        <v>233</v>
+      </c>
+      <c r="C32" s="61"/>
+      <c r="D32" s="61"/>
+      <c r="E32" s="52"/>
+      <c r="F32" s="52"/>
+      <c r="H32" s="114"/>
+      <c r="I32" s="48" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="62"/>
+      <c r="B33" s="127" t="s">
+        <v>253</v>
+      </c>
+      <c r="C33" s="128"/>
+      <c r="D33" s="128"/>
+      <c r="E33" s="126"/>
+      <c r="F33" s="126"/>
+      <c r="I33" s="48" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="63"/>
+      <c r="B34" s="121" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" s="121" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" s="121" t="s">
+        <v>58</v>
+      </c>
+      <c r="E34" s="120"/>
+      <c r="F34" s="120"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="63"/>
+      <c r="B35" s="88" t="s">
+        <v>42</v>
+      </c>
+      <c r="C35" s="89" t="s">
+        <v>144</v>
+      </c>
+      <c r="D35" s="88"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="63"/>
+      <c r="B36" s="66" t="s">
         <v>234</v>
       </c>
-      <c r="C27" s="53"/>
-      <c r="D27" s="53"/>
-      <c r="E27" s="53"/>
-      <c r="F27" s="53"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B28" s="48" t="s">
-        <v>112</v>
-      </c>
-      <c r="C28" s="48" t="s">
-        <v>87</v>
-      </c>
-      <c r="H28" s="124"/>
-      <c r="I28" s="48" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H29" s="126"/>
-      <c r="I29" s="48" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="51"/>
-      <c r="B30" s="51"/>
-      <c r="C30" s="51"/>
-      <c r="D30" s="51"/>
-      <c r="E30" s="51"/>
-      <c r="F30" s="51"/>
-      <c r="H30" s="113"/>
-      <c r="I30" s="48" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="52"/>
-      <c r="B31" s="60" t="s">
-        <v>235</v>
-      </c>
-      <c r="C31" s="61"/>
-      <c r="D31" s="61"/>
-      <c r="E31" s="52"/>
-      <c r="F31" s="52"/>
-      <c r="H31" s="114"/>
-      <c r="I31" s="48" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="62"/>
-      <c r="B32" s="127" t="s">
-        <v>255</v>
-      </c>
-      <c r="C32" s="128"/>
-      <c r="D32" s="128"/>
-      <c r="E32" s="126"/>
-      <c r="F32" s="126"/>
-      <c r="I32" s="48" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="63"/>
-      <c r="B33" s="121" t="s">
-        <v>64</v>
-      </c>
-      <c r="C33" s="121" t="s">
-        <v>14</v>
-      </c>
-      <c r="D33" s="121" t="s">
-        <v>58</v>
-      </c>
-      <c r="E33" s="120"/>
-      <c r="F33" s="120"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="63"/>
-      <c r="B34" s="88" t="s">
-        <v>42</v>
-      </c>
-      <c r="C34" s="89" t="s">
-        <v>144</v>
-      </c>
-      <c r="D34" s="88"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="63"/>
-      <c r="B35" s="66" t="s">
-        <v>236</v>
-      </c>
-      <c r="C35" s="67"/>
-      <c r="D35" s="67"/>
-      <c r="E35" s="113"/>
-      <c r="F35" s="113"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="63"/>
-      <c r="B36" s="69" t="s">
-        <v>343</v>
-      </c>
-      <c r="C36" s="64" t="s">
-        <v>341</v>
-      </c>
-      <c r="D36" s="64" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C36" s="67"/>
+      <c r="D36" s="67"/>
+      <c r="E36" s="113"/>
+      <c r="F36" s="113"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="63"/>
       <c r="B37" s="69" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="C37" s="64" t="s">
-        <v>344</v>
-      </c>
-      <c r="D37" s="64"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+        <v>337</v>
+      </c>
+      <c r="D37" s="64" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="63"/>
       <c r="B38" s="69" t="s">
+        <v>338</v>
+      </c>
+      <c r="C38" s="64" t="s">
+        <v>340</v>
+      </c>
+      <c r="D38" s="64"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" s="63"/>
+      <c r="B39" s="69" t="s">
         <v>76</v>
       </c>
-      <c r="C38" s="64" t="s">
+      <c r="C39" s="64" t="s">
         <v>131</v>
       </c>
-      <c r="D38" s="64" t="s">
+      <c r="D39" s="64" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="65" t="s">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" s="65" t="s">
         <v>80</v>
       </c>
-      <c r="B39" s="69" t="s">
+      <c r="B40" s="69" t="s">
         <v>102</v>
       </c>
-      <c r="C39" s="64" t="s">
+      <c r="C40" s="64" t="s">
         <v>130</v>
-      </c>
-      <c r="D39" s="70" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="68"/>
-      <c r="B40" s="69" t="s">
-        <v>99</v>
-      </c>
-      <c r="C40" s="64" t="s">
-        <v>113</v>
       </c>
       <c r="D40" s="70" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="41" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A41" s="68"/>
       <c r="B41" s="69" t="s">
+        <v>99</v>
+      </c>
+      <c r="C41" s="64" t="s">
+        <v>113</v>
+      </c>
+      <c r="D41" s="70" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="68"/>
+      <c r="B42" s="69" t="s">
         <v>100</v>
       </c>
-      <c r="C41" s="64" t="s">
+      <c r="C42" s="64" t="s">
         <v>132</v>
       </c>
-      <c r="D41" s="64" t="s">
+      <c r="D42" s="64" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="42" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="68"/>
-      <c r="B42" s="71" t="s">
+    <row r="43" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="68"/>
+      <c r="B43" s="71" t="s">
         <v>91</v>
       </c>
-      <c r="C42" s="72" t="s">
+      <c r="C43" s="72" t="s">
         <v>118</v>
       </c>
-      <c r="D42" s="70" t="s">
+      <c r="D43" s="70" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="43" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="68"/>
-      <c r="B43" s="66" t="s">
+    <row r="44" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="68"/>
+      <c r="B44" s="66" t="s">
+        <v>235</v>
+      </c>
+      <c r="C44" s="67" t="s">
+        <v>14</v>
+      </c>
+      <c r="D44" s="67"/>
+      <c r="E44" s="113"/>
+      <c r="F44" s="113"/>
+    </row>
+    <row r="45" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="68"/>
+      <c r="B45" s="75" t="s">
         <v>237</v>
       </c>
-      <c r="C43" s="67" t="s">
-        <v>14</v>
-      </c>
-      <c r="D43" s="67"/>
-      <c r="E43" s="113"/>
-      <c r="F43" s="113"/>
-    </row>
-    <row r="44" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="68"/>
-      <c r="B44" s="75" t="s">
-        <v>239</v>
-      </c>
-      <c r="C44" s="76"/>
-      <c r="D44" s="76"/>
-      <c r="E44" s="114"/>
-      <c r="F44" s="114"/>
-    </row>
-    <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="73" t="s">
+      <c r="C45" s="76"/>
+      <c r="D45" s="76"/>
+      <c r="E45" s="114"/>
+      <c r="F45" s="114"/>
+    </row>
+    <row r="46" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="73" t="s">
         <v>81</v>
       </c>
-      <c r="B45" s="77" t="s">
+      <c r="B46" s="77" t="s">
         <v>136</v>
       </c>
-      <c r="C45" s="70" t="s">
-        <v>251</v>
-      </c>
-      <c r="D45" s="70"/>
-    </row>
-    <row r="46" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="74"/>
-      <c r="B46" s="77" t="s">
-        <v>78</v>
-      </c>
       <c r="C46" s="70" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D46" s="70"/>
     </row>
-    <row r="47" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A47" s="74"/>
       <c r="B47" s="77" t="s">
+        <v>78</v>
+      </c>
+      <c r="C47" s="70" t="s">
+        <v>250</v>
+      </c>
+      <c r="D47" s="70"/>
+    </row>
+    <row r="48" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="74"/>
+      <c r="B48" s="77" t="s">
         <v>101</v>
       </c>
-      <c r="C47" s="70" t="s">
+      <c r="C48" s="70" t="s">
         <v>114</v>
       </c>
-      <c r="D47" s="70" t="s">
+      <c r="D48" s="70" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="74"/>
-      <c r="B48" s="75" t="s">
-        <v>238</v>
-      </c>
-      <c r="C48" s="76"/>
-      <c r="D48" s="76"/>
-      <c r="E48" s="114"/>
-      <c r="F48" s="114"/>
     </row>
     <row r="49" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A49" s="74"/>
-      <c r="B49" s="77" t="s">
-        <v>104</v>
-      </c>
-      <c r="C49" s="78" t="s">
-        <v>133</v>
-      </c>
-      <c r="D49" s="70" t="s">
-        <v>158</v>
-      </c>
+      <c r="B49" s="75" t="s">
+        <v>236</v>
+      </c>
+      <c r="C49" s="76"/>
+      <c r="D49" s="76"/>
+      <c r="E49" s="114"/>
+      <c r="F49" s="114"/>
     </row>
     <row r="50" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A50" s="74"/>
       <c r="B50" s="77" t="s">
-        <v>142</v>
-      </c>
-      <c r="C50" s="70" t="s">
-        <v>253</v>
-      </c>
-      <c r="D50" s="72"/>
-      <c r="E50" s="64"/>
+        <v>104</v>
+      </c>
+      <c r="C50" s="78" t="s">
+        <v>133</v>
+      </c>
+      <c r="D50" s="70" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="51" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A51" s="74"/>
       <c r="B51" s="77" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C51" s="70" t="s">
-        <v>144</v>
+        <v>251</v>
       </c>
       <c r="D51" s="72"/>
+      <c r="E51" s="64"/>
     </row>
     <row r="52" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A52" s="74"/>
-      <c r="B52" s="66" t="s">
-        <v>240</v>
-      </c>
-      <c r="C52" s="67"/>
-      <c r="D52" s="67"/>
-      <c r="E52" s="113"/>
-      <c r="F52" s="113"/>
+      <c r="B52" s="77" t="s">
+        <v>143</v>
+      </c>
+      <c r="C52" s="70" t="s">
+        <v>144</v>
+      </c>
+      <c r="D52" s="72"/>
     </row>
     <row r="53" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A53" s="74"/>
-      <c r="B53" s="80" t="s">
-        <v>241</v>
-      </c>
-      <c r="C53" s="81"/>
-      <c r="D53" s="81"/>
-      <c r="E53" s="114"/>
-      <c r="F53" s="114"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B53" s="66" t="s">
+        <v>238</v>
+      </c>
+      <c r="C53" s="67"/>
+      <c r="D53" s="67"/>
+      <c r="E53" s="113"/>
+      <c r="F53" s="113"/>
+    </row>
+    <row r="54" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A54" s="74"/>
-      <c r="B54" s="77" t="s">
-        <v>103</v>
-      </c>
-      <c r="C54" s="83" t="s">
-        <v>250</v>
-      </c>
-      <c r="D54" s="72" t="s">
-        <v>77</v>
-      </c>
+      <c r="B54" s="80" t="s">
+        <v>239</v>
+      </c>
+      <c r="C54" s="81"/>
+      <c r="D54" s="81"/>
+      <c r="E54" s="114"/>
+      <c r="F54" s="114"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="74"/>
       <c r="B55" s="77" t="s">
-        <v>345</v>
+        <v>103</v>
       </c>
       <c r="C55" s="83" t="s">
-        <v>346</v>
-      </c>
-      <c r="D55" s="72"/>
-    </row>
-    <row r="56" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="79" t="s">
+        <v>248</v>
+      </c>
+      <c r="D55" s="72" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="74"/>
+      <c r="B56" s="77" t="s">
+        <v>341</v>
+      </c>
+      <c r="C56" s="83" t="s">
+        <v>342</v>
+      </c>
+      <c r="D56" s="72"/>
+    </row>
+    <row r="57" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="79" t="s">
         <v>82</v>
       </c>
-      <c r="B56" s="80" t="s">
-        <v>242</v>
-      </c>
-      <c r="C56" s="81"/>
-      <c r="D56" s="81"/>
-      <c r="E56" s="114"/>
-      <c r="F56" s="114"/>
-    </row>
-    <row r="57" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="82"/>
       <c r="B57" s="80" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C57" s="81"/>
       <c r="D57" s="81"/>
@@ -6044,65 +6049,63 @@
     </row>
     <row r="58" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A58" s="82"/>
-      <c r="B58" s="84" t="s">
-        <v>206</v>
-      </c>
-      <c r="C58" s="86" t="s">
-        <v>216</v>
-      </c>
-      <c r="D58" s="72"/>
+      <c r="B58" s="80" t="s">
+        <v>241</v>
+      </c>
+      <c r="C58" s="81"/>
+      <c r="D58" s="81"/>
+      <c r="E58" s="114"/>
+      <c r="F58" s="114"/>
     </row>
     <row r="59" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A59" s="82"/>
       <c r="B59" s="84" t="s">
-        <v>207</v>
-      </c>
-      <c r="C59" s="48" t="s">
-        <v>208</v>
-      </c>
-      <c r="D59" s="72" t="s">
-        <v>77</v>
-      </c>
+        <v>206</v>
+      </c>
+      <c r="C59" s="86" t="s">
+        <v>216</v>
+      </c>
+      <c r="D59" s="72"/>
     </row>
     <row r="60" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A60" s="82"/>
       <c r="B60" s="84" t="s">
-        <v>169</v>
-      </c>
-      <c r="C60" s="85" t="s">
-        <v>215</v>
-      </c>
-      <c r="D60" s="72"/>
+        <v>207</v>
+      </c>
+      <c r="C60" s="48" t="s">
+        <v>208</v>
+      </c>
+      <c r="D60" s="72" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="61" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A61" s="82"/>
-      <c r="B61" s="80" t="s">
-        <v>244</v>
-      </c>
-      <c r="C61" s="81"/>
-      <c r="D61" s="81"/>
-      <c r="E61" s="114"/>
-      <c r="F61" s="114"/>
+      <c r="B61" s="84" t="s">
+        <v>169</v>
+      </c>
+      <c r="C61" s="85" t="s">
+        <v>215</v>
+      </c>
+      <c r="D61" s="72"/>
     </row>
     <row r="62" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A62" s="82"/>
-      <c r="B62" s="84" t="s">
-        <v>85</v>
-      </c>
-      <c r="C62" s="86" t="s">
-        <v>254</v>
-      </c>
-      <c r="D62" s="72" t="s">
-        <v>77</v>
-      </c>
+      <c r="B62" s="80" t="s">
+        <v>242</v>
+      </c>
+      <c r="C62" s="81"/>
+      <c r="D62" s="81"/>
+      <c r="E62" s="114"/>
+      <c r="F62" s="114"/>
     </row>
     <row r="63" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A63" s="82"/>
       <c r="B63" s="84" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C63" s="86" t="s">
-        <v>134</v>
+        <v>252</v>
       </c>
       <c r="D63" s="72" t="s">
         <v>77</v>
@@ -6110,121 +6113,121 @@
     </row>
     <row r="64" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A64" s="82"/>
-      <c r="B64" s="66" t="s">
-        <v>245</v>
-      </c>
-      <c r="C64" s="67"/>
-      <c r="D64" s="67"/>
-      <c r="E64" s="113"/>
-      <c r="F64" s="113"/>
+      <c r="B64" s="84" t="s">
+        <v>84</v>
+      </c>
+      <c r="C64" s="86" t="s">
+        <v>134</v>
+      </c>
+      <c r="D64" s="72" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="65" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A65" s="82"/>
-      <c r="B65" s="71" t="s">
+      <c r="B65" s="66" t="s">
+        <v>243</v>
+      </c>
+      <c r="C65" s="67"/>
+      <c r="D65" s="67"/>
+      <c r="E65" s="113"/>
+      <c r="F65" s="113"/>
+    </row>
+    <row r="66" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="82"/>
+      <c r="B66" s="71" t="s">
         <v>86</v>
       </c>
-      <c r="C65" s="72" t="s">
+      <c r="C66" s="72" t="s">
         <v>135</v>
       </c>
-      <c r="D65" s="72" t="s">
+      <c r="D66" s="72" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66" s="65" t="s">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" s="65" t="s">
         <v>83</v>
       </c>
-      <c r="B66" s="66" t="s">
-        <v>246</v>
-      </c>
-      <c r="C66" s="67"/>
-      <c r="D66" s="67"/>
-      <c r="E66" s="113"/>
-      <c r="F66" s="113"/>
-    </row>
-    <row r="67" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="65"/>
-      <c r="B67" s="71" t="s">
+      <c r="B67" s="66" t="s">
+        <v>244</v>
+      </c>
+      <c r="C67" s="67"/>
+      <c r="D67" s="67"/>
+      <c r="E67" s="113"/>
+      <c r="F67" s="113"/>
+    </row>
+    <row r="68" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="65"/>
+      <c r="B68" s="71" t="s">
         <v>153</v>
       </c>
-      <c r="C67" s="72" t="s">
+      <c r="C68" s="72" t="s">
         <v>152</v>
       </c>
-      <c r="D67" s="70"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B68" s="71" t="s">
+      <c r="D68" s="70"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B69" s="71" t="s">
         <v>154</v>
       </c>
-      <c r="C68" s="72" t="s">
+      <c r="C69" s="72" t="s">
         <v>155</v>
       </c>
-      <c r="D68" s="70"/>
-    </row>
-    <row r="69" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B69" s="66" t="s">
-        <v>247</v>
-      </c>
-      <c r="C69" s="67"/>
-      <c r="D69" s="67"/>
-      <c r="E69" s="67"/>
-      <c r="F69" s="67"/>
+      <c r="D69" s="70"/>
     </row>
     <row r="70" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B70" s="54"/>
-      <c r="C70" s="55"/>
-      <c r="D70" s="55"/>
-      <c r="E70" s="55"/>
-      <c r="F70" s="55"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A71" s="51"/>
-      <c r="B71" s="122" t="s">
-        <v>322</v>
-      </c>
-      <c r="C71" s="67"/>
-      <c r="D71" s="67"/>
-      <c r="E71" s="113"/>
-      <c r="F71" s="113"/>
+      <c r="B70" s="66" t="s">
+        <v>245</v>
+      </c>
+      <c r="C70" s="67"/>
+      <c r="D70" s="67"/>
+      <c r="E70" s="67"/>
+      <c r="F70" s="67"/>
+    </row>
+    <row r="71" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B71" s="54"/>
+      <c r="C71" s="55"/>
+      <c r="D71" s="55"/>
+      <c r="E71" s="55"/>
+      <c r="F71" s="55"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B72" s="71" t="s">
-        <v>323</v>
-      </c>
-      <c r="C72" s="72" t="s">
-        <v>324</v>
-      </c>
-      <c r="D72" s="70"/>
+      <c r="A72" s="51"/>
+      <c r="B72" s="122" t="s">
+        <v>318</v>
+      </c>
+      <c r="C72" s="67"/>
+      <c r="D72" s="67"/>
+      <c r="E72" s="113"/>
+      <c r="F72" s="113"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73" s="51"/>
-      <c r="B73" s="122" t="s">
-        <v>265</v>
-      </c>
-      <c r="C73" s="67"/>
-      <c r="D73" s="67"/>
-      <c r="E73" s="113"/>
-      <c r="F73" s="113"/>
+      <c r="B73" s="71" t="s">
+        <v>319</v>
+      </c>
+      <c r="C73" s="72" t="s">
+        <v>320</v>
+      </c>
+      <c r="D73" s="70"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="51"/>
-      <c r="B74" s="123" t="s">
-        <v>261</v>
-      </c>
-      <c r="C74" s="105" t="s">
-        <v>268</v>
-      </c>
-      <c r="D74" s="55"/>
-      <c r="E74" s="64"/>
-      <c r="F74" s="64"/>
+      <c r="B74" s="122" t="s">
+        <v>263</v>
+      </c>
+      <c r="C74" s="67"/>
+      <c r="D74" s="67"/>
+      <c r="E74" s="113"/>
+      <c r="F74" s="113"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="51"/>
       <c r="B75" s="123" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="C75" s="105" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D75" s="55"/>
       <c r="E75" s="64"/>
@@ -6233,10 +6236,10 @@
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="51"/>
       <c r="B76" s="123" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C76" s="105" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D76" s="55"/>
       <c r="E76" s="64"/>
@@ -6245,10 +6248,10 @@
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="51"/>
       <c r="B77" s="123" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C77" s="105" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D77" s="55"/>
       <c r="E77" s="64"/>
@@ -6257,10 +6260,10 @@
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="51"/>
       <c r="B78" s="123" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C78" s="105" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D78" s="55"/>
       <c r="E78" s="64"/>
@@ -6268,391 +6271,403 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="51"/>
-      <c r="B79" s="122" t="s">
-        <v>266</v>
-      </c>
-      <c r="C79" s="67"/>
-      <c r="D79" s="67"/>
-      <c r="E79" s="113"/>
-      <c r="F79" s="113"/>
+      <c r="B79" s="123" t="s">
+        <v>261</v>
+      </c>
+      <c r="C79" s="105" t="s">
+        <v>270</v>
+      </c>
+      <c r="D79" s="55"/>
+      <c r="E79" s="64"/>
+      <c r="F79" s="64"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="51"/>
-      <c r="B80" s="123" t="s">
-        <v>339</v>
-      </c>
-      <c r="C80" t="s">
-        <v>340</v>
-      </c>
-      <c r="D80"/>
-      <c r="E80"/>
-      <c r="F80"/>
-    </row>
-    <row r="81" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B80" s="122" t="s">
+        <v>264</v>
+      </c>
+      <c r="C80" s="67"/>
+      <c r="D80" s="67"/>
+      <c r="E80" s="113"/>
+      <c r="F80" s="113"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" s="51"/>
       <c r="B81" s="123" t="s">
-        <v>267</v>
+        <v>335</v>
       </c>
       <c r="C81" t="s">
-        <v>273</v>
-      </c>
+        <v>336</v>
+      </c>
+      <c r="D81"/>
+      <c r="E81"/>
+      <c r="F81"/>
     </row>
     <row r="82" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B82" s="122" t="s">
-        <v>280</v>
-      </c>
-      <c r="C82" s="130"/>
-      <c r="D82" s="130"/>
-      <c r="E82" s="130"/>
-      <c r="F82" s="130"/>
+      <c r="B82" s="123" t="s">
+        <v>265</v>
+      </c>
+      <c r="C82" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="83" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B83" s="132" t="s">
-        <v>310</v>
-      </c>
-      <c r="C83" s="131" t="s">
-        <v>281</v>
-      </c>
-      <c r="D83" s="131"/>
-      <c r="E83" s="131"/>
-      <c r="F83" s="131"/>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A84" s="51"/>
-      <c r="B84" s="127" t="s">
-        <v>248</v>
-      </c>
-      <c r="C84" s="129"/>
-      <c r="D84" s="129"/>
-      <c r="E84" s="129"/>
-      <c r="F84" s="129"/>
+      <c r="B83" s="122" t="s">
+        <v>278</v>
+      </c>
+      <c r="C83" s="130"/>
+      <c r="D83" s="130"/>
+      <c r="E83" s="130"/>
+      <c r="F83" s="130"/>
+    </row>
+    <row r="84" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B84" s="132" t="s">
+        <v>308</v>
+      </c>
+      <c r="C84" s="131" t="s">
+        <v>279</v>
+      </c>
+      <c r="D84" s="131"/>
+      <c r="E84" s="131"/>
+      <c r="F84" s="131"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="51"/>
-      <c r="B85" s="88" t="s">
-        <v>117</v>
-      </c>
-      <c r="C85" s="89" t="s">
-        <v>116</v>
-      </c>
-      <c r="D85" s="88"/>
+      <c r="B85" s="127" t="s">
+        <v>246</v>
+      </c>
+      <c r="C85" s="129"/>
+      <c r="D85" s="129"/>
+      <c r="E85" s="129"/>
+      <c r="F85" s="129"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="51"/>
       <c r="B86" s="88" t="s">
-        <v>311</v>
+        <v>117</v>
       </c>
       <c r="C86" s="89" t="s">
-        <v>312</v>
+        <v>116</v>
       </c>
       <c r="D86" s="88"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A87" s="52"/>
+      <c r="A87" s="51"/>
       <c r="B87" s="88" t="s">
-        <v>140</v>
+        <v>309</v>
       </c>
       <c r="C87" s="89" t="s">
-        <v>141</v>
+        <v>310</v>
       </c>
       <c r="D87" s="88"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="52"/>
       <c r="B88" s="88" t="s">
-        <v>323</v>
+        <v>140</v>
       </c>
       <c r="C88" s="89" t="s">
-        <v>325</v>
+        <v>141</v>
       </c>
       <c r="D88" s="88"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A89" s="87"/>
-      <c r="B89" s="69" t="s">
-        <v>111</v>
-      </c>
-      <c r="C89" s="64" t="s">
-        <v>115</v>
-      </c>
-      <c r="D89" s="64"/>
+      <c r="A89" s="52"/>
+      <c r="B89" s="88" t="s">
+        <v>319</v>
+      </c>
+      <c r="C89" s="89" t="s">
+        <v>321</v>
+      </c>
+      <c r="D89" s="88"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" s="87"/>
-      <c r="B90" s="142" t="s">
-        <v>313</v>
-      </c>
-      <c r="C90" s="119"/>
-      <c r="D90" s="119"/>
-      <c r="E90" s="119"/>
-      <c r="F90" s="119"/>
+      <c r="B90" s="69" t="s">
+        <v>111</v>
+      </c>
+      <c r="C90" s="64" t="s">
+        <v>115</v>
+      </c>
+      <c r="D90" s="64"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="87"/>
-      <c r="B91" s="71" t="s">
-        <v>119</v>
-      </c>
-      <c r="C91" s="72" t="s">
-        <v>361</v>
-      </c>
-      <c r="D91" s="72"/>
+      <c r="B91" s="142" t="s">
+        <v>311</v>
+      </c>
+      <c r="C91" s="119"/>
+      <c r="D91" s="119"/>
+      <c r="E91" s="119"/>
+      <c r="F91" s="119"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" s="87"/>
       <c r="B92" s="71" t="s">
-        <v>315</v>
+        <v>119</v>
       </c>
       <c r="C92" s="72" t="s">
-        <v>314</v>
+        <v>351</v>
       </c>
       <c r="D92" s="72"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="87"/>
       <c r="B93" s="71" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="C93" s="72" t="s">
-        <v>317</v>
+        <v>365</v>
       </c>
       <c r="D93" s="72"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A94" s="119" t="s">
-        <v>249</v>
-      </c>
-      <c r="B94" s="142" t="s">
-        <v>318</v>
-      </c>
-      <c r="C94" s="119"/>
-      <c r="D94" s="119"/>
-      <c r="E94" s="119"/>
-      <c r="F94" s="119"/>
-    </row>
-    <row r="95" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="90"/>
-      <c r="B95" s="71" t="s">
+      <c r="A94" s="87"/>
+      <c r="B94" s="71" t="s">
+        <v>313</v>
+      </c>
+      <c r="C94" s="72" t="s">
+        <v>364</v>
+      </c>
+      <c r="D94" s="72"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A95" s="119" t="s">
+        <v>247</v>
+      </c>
+      <c r="B95" s="142" t="s">
+        <v>314</v>
+      </c>
+      <c r="C95" s="119"/>
+      <c r="D95" s="119"/>
+      <c r="E95" s="119"/>
+      <c r="F95" s="119"/>
+    </row>
+    <row r="96" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="90"/>
+      <c r="B96" s="71" t="s">
         <v>38</v>
       </c>
-      <c r="C95" s="72" t="s">
+      <c r="C96" s="72" t="s">
         <v>162</v>
       </c>
-      <c r="D95" s="72"/>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A96" s="119" t="s">
-        <v>256</v>
-      </c>
-      <c r="B96" s="71" t="s">
+      <c r="D96" s="72"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A97" s="119" t="s">
+        <v>254</v>
+      </c>
+      <c r="B97" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="C96" s="72" t="s">
+      <c r="C97" s="72" t="s">
         <v>157</v>
       </c>
-      <c r="D96" s="72"/>
-    </row>
-    <row r="97" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="90"/>
-      <c r="B97" s="71" t="s">
+      <c r="D97" s="72"/>
+    </row>
+    <row r="98" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="90"/>
+      <c r="B98" s="71" t="s">
         <v>199</v>
       </c>
-      <c r="C97" s="110" t="s">
+      <c r="C98" s="110" t="s">
         <v>200</v>
-      </c>
-      <c r="D97" s="72"/>
-    </row>
-    <row r="98" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="91"/>
-      <c r="B98" s="71" t="s">
-        <v>202</v>
-      </c>
-      <c r="C98" s="110" t="s">
-        <v>203</v>
       </c>
       <c r="D98" s="72"/>
     </row>
     <row r="99" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A99" s="91"/>
       <c r="B99" s="71" t="s">
-        <v>320</v>
+        <v>202</v>
       </c>
       <c r="C99" s="110" t="s">
-        <v>319</v>
+        <v>203</v>
       </c>
       <c r="D99" s="72"/>
     </row>
     <row r="100" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A100" s="91"/>
-      <c r="B100" s="142" t="s">
-        <v>321</v>
-      </c>
-      <c r="C100" s="119"/>
-      <c r="D100" s="119"/>
-      <c r="E100" s="119"/>
-      <c r="F100" s="119"/>
+      <c r="B100" s="71" t="s">
+        <v>316</v>
+      </c>
+      <c r="C100" s="110" t="s">
+        <v>315</v>
+      </c>
+      <c r="D100" s="72"/>
     </row>
     <row r="101" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A101" s="91"/>
-      <c r="B101" s="75" t="s">
-        <v>258</v>
-      </c>
-      <c r="C101" s="93"/>
-      <c r="D101" s="93"/>
-      <c r="E101" s="93"/>
-      <c r="F101" s="93"/>
-    </row>
-    <row r="102" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="119" t="s">
-        <v>257</v>
-      </c>
-      <c r="B102" s="84" t="s">
+      <c r="B101" s="142" t="s">
+        <v>317</v>
+      </c>
+      <c r="C101" s="119"/>
+      <c r="D101" s="119"/>
+      <c r="E101" s="119"/>
+      <c r="F101" s="119"/>
+    </row>
+    <row r="102" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A102" s="91"/>
+      <c r="B102" s="75" t="s">
+        <v>256</v>
+      </c>
+      <c r="C102" s="93"/>
+      <c r="D102" s="93"/>
+      <c r="E102" s="93"/>
+      <c r="F102" s="93"/>
+    </row>
+    <row r="103" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A103" s="119" t="s">
+        <v>255</v>
+      </c>
+      <c r="B103" s="84" t="s">
         <v>90</v>
       </c>
-      <c r="C102" s="72" t="s">
+      <c r="C103" s="72" t="s">
         <v>159</v>
       </c>
-      <c r="D102" s="72"/>
-    </row>
-    <row r="103" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="92"/>
-      <c r="B103" s="84" t="s">
+      <c r="D103" s="72"/>
+    </row>
+    <row r="104" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="92"/>
+      <c r="B104" s="84" t="s">
         <v>89</v>
       </c>
-      <c r="C103" s="72" t="s">
+      <c r="C104" s="72" t="s">
         <v>160</v>
       </c>
-      <c r="D103" s="72"/>
-    </row>
-    <row r="104" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="94"/>
-      <c r="B104" s="75" t="s">
-        <v>259</v>
-      </c>
-      <c r="C104" s="93"/>
-      <c r="D104" s="93"/>
-      <c r="E104" s="93"/>
-      <c r="F104" s="93"/>
+      <c r="D104" s="72"/>
     </row>
     <row r="105" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A105" s="94"/>
-      <c r="B105" s="118" t="s">
-        <v>137</v>
-      </c>
-      <c r="C105" s="72" t="s">
-        <v>138</v>
-      </c>
-      <c r="D105" s="72"/>
+      <c r="B105" s="75" t="s">
+        <v>257</v>
+      </c>
+      <c r="C105" s="93"/>
+      <c r="D105" s="93"/>
+      <c r="E105" s="93"/>
+      <c r="F105" s="93"/>
     </row>
     <row r="106" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="92"/>
+      <c r="A106" s="94"/>
       <c r="B106" s="118" t="s">
         <v>137</v>
       </c>
       <c r="C106" s="72" t="s">
-        <v>233</v>
+        <v>138</v>
       </c>
       <c r="D106" s="72"/>
     </row>
     <row r="107" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="94"/>
+      <c r="A107" s="92"/>
       <c r="B107" s="118" t="s">
+        <v>137</v>
+      </c>
+      <c r="C107" s="72" t="s">
+        <v>363</v>
+      </c>
+      <c r="D107" s="72"/>
+    </row>
+    <row r="108" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="94"/>
+      <c r="B108" s="118" t="s">
         <v>191</v>
       </c>
-      <c r="C107" s="72" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B110" s="106" t="s">
+      <c r="C108" s="72" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2"/>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B111" s="106" t="s">
         <v>192</v>
       </c>
-      <c r="C110" s="106" t="s">
+      <c r="C111" s="106" t="s">
         <v>196</v>
       </c>
-      <c r="D110" s="149" t="s">
+      <c r="D111" s="149" t="s">
         <v>197</v>
       </c>
-      <c r="E110" s="149"/>
-      <c r="F110" s="149"/>
-    </row>
-    <row r="111" spans="1:6" ht="127.5" x14ac:dyDescent="0.2">
-      <c r="B111" s="109" t="s">
+      <c r="E111" s="149"/>
+      <c r="F111" s="149"/>
+    </row>
+    <row r="112" spans="1:6" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="B112" s="109" t="s">
         <v>193</v>
       </c>
-      <c r="C111" s="108" t="s">
+      <c r="C112" s="108" t="s">
         <v>205</v>
       </c>
-      <c r="D111" s="150" t="s">
+      <c r="D112" s="150" t="s">
         <v>198</v>
-      </c>
-      <c r="E111" s="150"/>
-      <c r="F111" s="150"/>
-    </row>
-    <row r="112" spans="1:6" ht="102" x14ac:dyDescent="0.2">
-      <c r="B112" s="109" t="s">
-        <v>194</v>
-      </c>
-      <c r="C112" s="115" t="s">
-        <v>204</v>
-      </c>
-      <c r="D112" s="150" t="s">
-        <v>201</v>
       </c>
       <c r="E112" s="150"/>
       <c r="F112" s="150"/>
     </row>
-    <row r="113" spans="2:6" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:6" ht="102" x14ac:dyDescent="0.2">
       <c r="B113" s="109" t="s">
-        <v>195</v>
-      </c>
-      <c r="C113" s="108" t="s">
-        <v>209</v>
+        <v>194</v>
+      </c>
+      <c r="C113" s="115" t="s">
+        <v>204</v>
       </c>
       <c r="D113" s="150" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="E113" s="150"/>
       <c r="F113" s="150"/>
     </row>
-    <row r="114" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B114" s="117"/>
+    <row r="114" spans="2:6" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="B114" s="109" t="s">
+        <v>195</v>
+      </c>
+      <c r="C114" s="108" t="s">
+        <v>209</v>
+      </c>
+      <c r="D114" s="150" t="s">
+        <v>210</v>
+      </c>
+      <c r="E114" s="150"/>
+      <c r="F114" s="150"/>
     </row>
     <row r="115" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B115" s="116" t="s">
+      <c r="B115" s="117"/>
+    </row>
+    <row r="116" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B116" s="116" t="s">
         <v>218</v>
       </c>
-      <c r="C115" s="116" t="s">
+      <c r="C116" s="116" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="116" spans="2:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="B116" s="117" t="s">
+    <row r="117" spans="2:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="B117" s="117" t="s">
         <v>219</v>
       </c>
-      <c r="C116" s="108" t="s">
+      <c r="C117" s="108" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="117" spans="2:6" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="B117" s="117" t="s">
+    <row r="118" spans="2:6" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="B118" s="117" t="s">
         <v>220</v>
       </c>
-      <c r="C117" s="108" t="s">
+      <c r="C118" s="108" t="s">
         <v>222</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
+    <mergeCell ref="D114:F114"/>
     <mergeCell ref="D113:F113"/>
     <mergeCell ref="D112:F112"/>
     <mergeCell ref="D111:F111"/>
-    <mergeCell ref="D110:F110"/>
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D111" r:id="rId1"/>
-    <hyperlink ref="D112" r:id="rId2"/>
-    <hyperlink ref="D113" r:id="rId3"/>
+    <hyperlink ref="D112" r:id="rId1"/>
+    <hyperlink ref="D113" r:id="rId2"/>
+    <hyperlink ref="D114" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -6677,142 +6692,142 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="136" t="s">
+        <v>280</v>
+      </c>
+      <c r="B1" s="136" t="s">
+        <v>281</v>
+      </c>
+      <c r="C1" s="136" t="s">
         <v>282</v>
       </c>
-      <c r="B1" s="136" t="s">
+      <c r="D1" s="136" t="s">
         <v>283</v>
-      </c>
-      <c r="C1" s="136" t="s">
-        <v>284</v>
-      </c>
-      <c r="D1" s="136" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="133" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B2" s="134" t="s">
+        <v>299</v>
+      </c>
+      <c r="C2" s="135" t="s">
         <v>301</v>
       </c>
-      <c r="C2" s="135" t="s">
-        <v>303</v>
-      </c>
       <c r="D2" s="135" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="133" t="s">
+        <v>285</v>
+      </c>
+      <c r="B3" s="135" t="s">
+        <v>297</v>
+      </c>
+      <c r="C3" s="135" t="s">
+        <v>301</v>
+      </c>
+      <c r="D3" s="135" t="s">
         <v>287</v>
-      </c>
-      <c r="B3" s="135" t="s">
-        <v>299</v>
-      </c>
-      <c r="C3" s="135" t="s">
-        <v>303</v>
-      </c>
-      <c r="D3" s="135" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="133" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B4" s="135" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C4" s="135" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D4" s="135" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="133" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B5" s="135" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C5" s="135" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D5" s="135" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="133" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B6" s="135" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C6" s="135" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D6" s="135" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="133" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B7" s="135" t="s">
+        <v>300</v>
+      </c>
+      <c r="C7" s="135" t="s">
         <v>302</v>
       </c>
-      <c r="C7" s="135" t="s">
-        <v>304</v>
-      </c>
       <c r="D7" s="135" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="177.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="133" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B8" s="137" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C8" s="137" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D8" s="137" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="133" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B9" s="135" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C9" s="135" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D9" s="135" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="133" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B10" s="135" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C10" s="135" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D10" s="135" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Se contemplaron documentos firmados
</commit_message>
<xml_diff>
--- a/Organización/Procesos/Soporte Organizacional/2. Administración de Configuración/IWM_Administración de la Configuración.xlsx
+++ b/Organización/Procesos/Soporte Organizacional/2. Administración de Configuración/IWM_Administración de la Configuración.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="369">
   <si>
     <t>Adapiaciones al Estándar de Administración de Datos</t>
   </si>
@@ -1801,6 +1801,15 @@
   </si>
   <si>
     <t>IWM_Auditoria_Organizacional_mmddaa</t>
+  </si>
+  <si>
+    <t>Minuta firmada</t>
+  </si>
+  <si>
+    <t>Reporte de Actividades Firmado</t>
+  </si>
+  <si>
+    <t>Informe Firmado</t>
   </si>
 </sst>
 </file>
@@ -5418,10 +5427,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I118"/>
+  <dimension ref="A1:I121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C97" sqref="C97"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -5527,7 +5536,7 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="49"/>
       <c r="B10" s="88" t="s">
-        <v>333</v>
+        <v>367</v>
       </c>
       <c r="C10" s="89" t="s">
         <v>355</v>
@@ -5536,129 +5545,128 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="49"/>
-      <c r="B11" s="127" t="s">
-        <v>330</v>
-      </c>
-      <c r="C11" s="128"/>
-      <c r="D11" s="128"/>
-      <c r="E11" s="126"/>
-      <c r="F11" s="126"/>
+      <c r="B11" s="88" t="s">
+        <v>333</v>
+      </c>
+      <c r="C11" s="89" t="s">
+        <v>355</v>
+      </c>
+      <c r="D11" s="88"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="49"/>
-      <c r="B12" s="88" t="s">
+      <c r="B12" s="127" t="s">
+        <v>330</v>
+      </c>
+      <c r="C12" s="128"/>
+      <c r="D12" s="128"/>
+      <c r="E12" s="126"/>
+      <c r="F12" s="126"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="49"/>
+      <c r="B13" s="88" t="s">
         <v>331</v>
       </c>
-      <c r="C12" s="89" t="s">
+      <c r="C13" s="89" t="s">
         <v>356</v>
       </c>
-      <c r="D12" s="88"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="62"/>
-      <c r="B13" s="127" t="s">
+      <c r="D13" s="88"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="62"/>
+      <c r="B14" s="127" t="s">
         <v>322</v>
       </c>
-      <c r="C13" s="128"/>
-      <c r="D13" s="128"/>
-      <c r="E13" s="126"/>
-      <c r="F13" s="126"/>
-      <c r="I13" s="48" t="s">
+      <c r="C14" s="128"/>
+      <c r="D14" s="128"/>
+      <c r="E14" s="126"/>
+      <c r="F14" s="126"/>
+      <c r="I14" s="48" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="63"/>
-      <c r="B14" s="88" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="63"/>
+      <c r="B15" s="88" t="s">
         <v>323</v>
       </c>
-      <c r="C14" s="89" t="s">
+      <c r="C15" s="89" t="s">
         <v>357</v>
       </c>
-      <c r="D14" s="88"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="49"/>
-      <c r="B15" s="59" t="s">
-        <v>343</v>
-      </c>
-      <c r="C15" s="53"/>
-      <c r="D15" s="53"/>
-      <c r="E15" s="53"/>
-      <c r="F15" s="53"/>
+      <c r="D15" s="88"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="49"/>
-      <c r="B16" s="48" t="s">
-        <v>344</v>
-      </c>
-      <c r="C16" s="48" t="s">
-        <v>345</v>
-      </c>
+      <c r="B16" s="59" t="s">
+        <v>343</v>
+      </c>
+      <c r="C16" s="53"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="53"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="49"/>
       <c r="B17" s="48" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
       <c r="C17" s="48" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="49"/>
-      <c r="B18" s="127" t="s">
-        <v>346</v>
-      </c>
-      <c r="C18" s="128"/>
-      <c r="D18" s="128"/>
-      <c r="E18" s="126"/>
-      <c r="F18" s="126"/>
+      <c r="B18" s="48" t="s">
+        <v>353</v>
+      </c>
+      <c r="C18" s="48" t="s">
+        <v>354</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="49"/>
-      <c r="B19" s="88" t="s">
-        <v>259</v>
-      </c>
-      <c r="C19" s="89" t="s">
-        <v>358</v>
-      </c>
-      <c r="D19" s="88"/>
+      <c r="B19" s="48" t="s">
+        <v>368</v>
+      </c>
+      <c r="C19" s="48" t="s">
+        <v>354</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="49"/>
-      <c r="B20" s="88" t="s">
-        <v>352</v>
-      </c>
-      <c r="C20" s="89" t="s">
-        <v>359</v>
-      </c>
-      <c r="D20" s="88"/>
+      <c r="B20" s="127" t="s">
+        <v>346</v>
+      </c>
+      <c r="C20" s="128"/>
+      <c r="D20" s="128"/>
+      <c r="E20" s="126"/>
+      <c r="F20" s="126"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="49"/>
-      <c r="B21" s="127" t="s">
-        <v>347</v>
-      </c>
-      <c r="C21" s="128"/>
-      <c r="D21" s="128"/>
-      <c r="E21" s="126"/>
-      <c r="F21" s="126"/>
+      <c r="B21" s="88" t="s">
+        <v>259</v>
+      </c>
+      <c r="C21" s="89" t="s">
+        <v>358</v>
+      </c>
+      <c r="D21" s="88"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="49"/>
       <c r="B22" s="88" t="s">
-        <v>261</v>
+        <v>352</v>
       </c>
       <c r="C22" s="89" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D22" s="88"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="49"/>
       <c r="B23" s="127" t="s">
-        <v>330</v>
+        <v>347</v>
       </c>
       <c r="C23" s="128"/>
       <c r="D23" s="128"/>
@@ -5668,227 +5676,221 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="49"/>
       <c r="B24" s="88" t="s">
-        <v>348</v>
+        <v>261</v>
       </c>
       <c r="C24" s="89" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D24" s="88"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="62"/>
+      <c r="A25" s="49"/>
       <c r="B25" s="127" t="s">
-        <v>322</v>
+        <v>330</v>
       </c>
       <c r="C25" s="128"/>
       <c r="D25" s="128"/>
       <c r="E25" s="126"/>
       <c r="F25" s="126"/>
-      <c r="I25" s="48" t="s">
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="49"/>
+      <c r="B26" s="88" t="s">
+        <v>348</v>
+      </c>
+      <c r="C26" s="89" t="s">
+        <v>361</v>
+      </c>
+      <c r="D26" s="88"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="62"/>
+      <c r="B27" s="127" t="s">
+        <v>322</v>
+      </c>
+      <c r="C27" s="128"/>
+      <c r="D27" s="128"/>
+      <c r="E27" s="126"/>
+      <c r="F27" s="126"/>
+      <c r="I27" s="48" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="63"/>
-      <c r="B26" s="88" t="s">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="63"/>
+      <c r="B28" s="88" t="s">
         <v>323</v>
       </c>
-      <c r="C26" s="89" t="s">
+      <c r="C28" s="89" t="s">
         <v>357</v>
       </c>
-      <c r="D26" s="88"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="51"/>
-      <c r="B27" s="51"/>
-      <c r="C27" s="51"/>
-      <c r="D27" s="51"/>
-      <c r="E27" s="51"/>
-      <c r="F27" s="51"/>
-      <c r="I27" s="125" t="s">
+      <c r="D28" s="88"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="63"/>
+      <c r="B29" s="88" t="s">
+        <v>366</v>
+      </c>
+      <c r="C29" s="89" t="s">
+        <v>357</v>
+      </c>
+      <c r="D29" s="88"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="51"/>
+      <c r="B30" s="51"/>
+      <c r="C30" s="51"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="51"/>
+      <c r="F30" s="51"/>
+      <c r="I30" s="125" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="52"/>
-      <c r="B28" s="59" t="s">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="52"/>
+      <c r="B31" s="59" t="s">
         <v>232</v>
       </c>
-      <c r="C28" s="53"/>
-      <c r="D28" s="53"/>
-      <c r="E28" s="53"/>
-      <c r="F28" s="53"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B29" s="48" t="s">
+      <c r="C31" s="53"/>
+      <c r="D31" s="53"/>
+      <c r="E31" s="53"/>
+      <c r="F31" s="53"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B32" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="C29" s="48" t="s">
+      <c r="C32" s="48" t="s">
         <v>87</v>
       </c>
-      <c r="H29" s="124"/>
-      <c r="I29" s="48" t="s">
+      <c r="H32" s="124"/>
+      <c r="I32" s="48" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H30" s="126"/>
-      <c r="I30" s="48" t="s">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H33" s="126"/>
+      <c r="I33" s="48" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="51"/>
-      <c r="B31" s="51"/>
-      <c r="C31" s="51"/>
-      <c r="D31" s="51"/>
-      <c r="E31" s="51"/>
-      <c r="F31" s="51"/>
-      <c r="H31" s="113"/>
-      <c r="I31" s="48" t="s">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="51"/>
+      <c r="B34" s="51"/>
+      <c r="C34" s="51"/>
+      <c r="D34" s="51"/>
+      <c r="E34" s="51"/>
+      <c r="F34" s="51"/>
+      <c r="H34" s="113"/>
+      <c r="I34" s="48" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="52"/>
-      <c r="B32" s="60" t="s">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="52"/>
+      <c r="B35" s="60" t="s">
         <v>233</v>
       </c>
-      <c r="C32" s="61"/>
-      <c r="D32" s="61"/>
-      <c r="E32" s="52"/>
-      <c r="F32" s="52"/>
-      <c r="H32" s="114"/>
-      <c r="I32" s="48" t="s">
+      <c r="C35" s="61"/>
+      <c r="D35" s="61"/>
+      <c r="E35" s="52"/>
+      <c r="F35" s="52"/>
+      <c r="H35" s="114"/>
+      <c r="I35" s="48" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="62"/>
-      <c r="B33" s="127" t="s">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="62"/>
+      <c r="B36" s="127" t="s">
         <v>253</v>
       </c>
-      <c r="C33" s="128"/>
-      <c r="D33" s="128"/>
-      <c r="E33" s="126"/>
-      <c r="F33" s="126"/>
-      <c r="I33" s="48" t="s">
+      <c r="C36" s="128"/>
+      <c r="D36" s="128"/>
+      <c r="E36" s="126"/>
+      <c r="F36" s="126"/>
+      <c r="I36" s="48" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="63"/>
-      <c r="B34" s="121" t="s">
-        <v>64</v>
-      </c>
-      <c r="C34" s="121" t="s">
-        <v>14</v>
-      </c>
-      <c r="D34" s="121" t="s">
-        <v>58</v>
-      </c>
-      <c r="E34" s="120"/>
-      <c r="F34" s="120"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="63"/>
-      <c r="B35" s="88" t="s">
-        <v>42</v>
-      </c>
-      <c r="C35" s="89" t="s">
-        <v>144</v>
-      </c>
-      <c r="D35" s="88"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="63"/>
-      <c r="B36" s="66" t="s">
-        <v>234</v>
-      </c>
-      <c r="C36" s="67"/>
-      <c r="D36" s="67"/>
-      <c r="E36" s="113"/>
-      <c r="F36" s="113"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="63"/>
-      <c r="B37" s="69" t="s">
-        <v>339</v>
-      </c>
-      <c r="C37" s="64" t="s">
-        <v>337</v>
-      </c>
-      <c r="D37" s="64" t="s">
-        <v>77</v>
-      </c>
+      <c r="B37" s="121" t="s">
+        <v>64</v>
+      </c>
+      <c r="C37" s="121" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" s="121" t="s">
+        <v>58</v>
+      </c>
+      <c r="E37" s="120"/>
+      <c r="F37" s="120"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="63"/>
-      <c r="B38" s="69" t="s">
-        <v>338</v>
-      </c>
-      <c r="C38" s="64" t="s">
-        <v>340</v>
-      </c>
-      <c r="D38" s="64"/>
+      <c r="B38" s="88" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38" s="89" t="s">
+        <v>144</v>
+      </c>
+      <c r="D38" s="88"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="63"/>
-      <c r="B39" s="69" t="s">
+      <c r="B39" s="66" t="s">
+        <v>234</v>
+      </c>
+      <c r="C39" s="67"/>
+      <c r="D39" s="67"/>
+      <c r="E39" s="113"/>
+      <c r="F39" s="113"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" s="63"/>
+      <c r="B40" s="69" t="s">
+        <v>339</v>
+      </c>
+      <c r="C40" s="64" t="s">
+        <v>337</v>
+      </c>
+      <c r="D40" s="64" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" s="63"/>
+      <c r="B41" s="69" t="s">
+        <v>338</v>
+      </c>
+      <c r="C41" s="64" t="s">
+        <v>340</v>
+      </c>
+      <c r="D41" s="64"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" s="63"/>
+      <c r="B42" s="69" t="s">
         <v>76</v>
       </c>
-      <c r="C39" s="64" t="s">
+      <c r="C42" s="64" t="s">
         <v>131</v>
-      </c>
-      <c r="D39" s="64" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" s="65" t="s">
-        <v>80</v>
-      </c>
-      <c r="B40" s="69" t="s">
-        <v>102</v>
-      </c>
-      <c r="C40" s="64" t="s">
-        <v>130</v>
-      </c>
-      <c r="D40" s="70" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="68"/>
-      <c r="B41" s="69" t="s">
-        <v>99</v>
-      </c>
-      <c r="C41" s="64" t="s">
-        <v>113</v>
-      </c>
-      <c r="D41" s="70" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="68"/>
-      <c r="B42" s="69" t="s">
-        <v>100</v>
-      </c>
-      <c r="C42" s="64" t="s">
-        <v>132</v>
       </c>
       <c r="D42" s="64" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="43" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="68"/>
-      <c r="B43" s="71" t="s">
-        <v>91</v>
-      </c>
-      <c r="C43" s="72" t="s">
-        <v>118</v>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" s="65" t="s">
+        <v>80</v>
+      </c>
+      <c r="B43" s="69" t="s">
+        <v>102</v>
+      </c>
+      <c r="C43" s="64" t="s">
+        <v>130</v>
       </c>
       <c r="D43" s="70" t="s">
         <v>158</v>
@@ -5896,216 +5898,220 @@
     </row>
     <row r="44" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A44" s="68"/>
-      <c r="B44" s="66" t="s">
-        <v>235</v>
-      </c>
-      <c r="C44" s="67" t="s">
-        <v>14</v>
-      </c>
-      <c r="D44" s="67"/>
-      <c r="E44" s="113"/>
-      <c r="F44" s="113"/>
+      <c r="B44" s="69" t="s">
+        <v>99</v>
+      </c>
+      <c r="C44" s="64" t="s">
+        <v>113</v>
+      </c>
+      <c r="D44" s="70" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="45" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A45" s="68"/>
-      <c r="B45" s="75" t="s">
+      <c r="B45" s="69" t="s">
+        <v>100</v>
+      </c>
+      <c r="C45" s="64" t="s">
+        <v>132</v>
+      </c>
+      <c r="D45" s="64" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="68"/>
+      <c r="B46" s="71" t="s">
+        <v>91</v>
+      </c>
+      <c r="C46" s="72" t="s">
+        <v>118</v>
+      </c>
+      <c r="D46" s="70" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="68"/>
+      <c r="B47" s="66" t="s">
+        <v>235</v>
+      </c>
+      <c r="C47" s="67" t="s">
+        <v>14</v>
+      </c>
+      <c r="D47" s="67"/>
+      <c r="E47" s="113"/>
+      <c r="F47" s="113"/>
+    </row>
+    <row r="48" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="68"/>
+      <c r="B48" s="75" t="s">
         <v>237</v>
       </c>
-      <c r="C45" s="76"/>
-      <c r="D45" s="76"/>
-      <c r="E45" s="114"/>
-      <c r="F45" s="114"/>
-    </row>
-    <row r="46" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="73" t="s">
+      <c r="C48" s="76"/>
+      <c r="D48" s="76"/>
+      <c r="E48" s="114"/>
+      <c r="F48" s="114"/>
+    </row>
+    <row r="49" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="73" t="s">
         <v>81</v>
       </c>
-      <c r="B46" s="77" t="s">
+      <c r="B49" s="77" t="s">
         <v>136</v>
       </c>
-      <c r="C46" s="70" t="s">
+      <c r="C49" s="70" t="s">
         <v>249</v>
       </c>
-      <c r="D46" s="70"/>
-    </row>
-    <row r="47" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="74"/>
-      <c r="B47" s="77" t="s">
-        <v>78</v>
-      </c>
-      <c r="C47" s="70" t="s">
-        <v>250</v>
-      </c>
-      <c r="D47" s="70"/>
-    </row>
-    <row r="48" spans="1:9" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="74"/>
-      <c r="B48" s="77" t="s">
-        <v>101</v>
-      </c>
-      <c r="C48" s="70" t="s">
-        <v>114</v>
-      </c>
-      <c r="D48" s="70" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="74"/>
-      <c r="B49" s="75" t="s">
-        <v>236</v>
-      </c>
-      <c r="C49" s="76"/>
-      <c r="D49" s="76"/>
-      <c r="E49" s="114"/>
-      <c r="F49" s="114"/>
+      <c r="D49" s="70"/>
     </row>
     <row r="50" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A50" s="74"/>
       <c r="B50" s="77" t="s">
-        <v>104</v>
-      </c>
-      <c r="C50" s="78" t="s">
-        <v>133</v>
-      </c>
-      <c r="D50" s="70" t="s">
-        <v>158</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="C50" s="70" t="s">
+        <v>250</v>
+      </c>
+      <c r="D50" s="70"/>
     </row>
     <row r="51" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A51" s="74"/>
       <c r="B51" s="77" t="s">
-        <v>142</v>
+        <v>101</v>
       </c>
       <c r="C51" s="70" t="s">
-        <v>251</v>
-      </c>
-      <c r="D51" s="72"/>
-      <c r="E51" s="64"/>
+        <v>114</v>
+      </c>
+      <c r="D51" s="70" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="52" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A52" s="74"/>
-      <c r="B52" s="77" t="s">
-        <v>143</v>
-      </c>
-      <c r="C52" s="70" t="s">
-        <v>144</v>
-      </c>
-      <c r="D52" s="72"/>
+      <c r="B52" s="75" t="s">
+        <v>236</v>
+      </c>
+      <c r="C52" s="76"/>
+      <c r="D52" s="76"/>
+      <c r="E52" s="114"/>
+      <c r="F52" s="114"/>
     </row>
     <row r="53" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A53" s="74"/>
-      <c r="B53" s="66" t="s">
-        <v>238</v>
-      </c>
-      <c r="C53" s="67"/>
-      <c r="D53" s="67"/>
-      <c r="E53" s="113"/>
-      <c r="F53" s="113"/>
+      <c r="B53" s="77" t="s">
+        <v>104</v>
+      </c>
+      <c r="C53" s="78" t="s">
+        <v>133</v>
+      </c>
+      <c r="D53" s="70" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="54" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A54" s="74"/>
-      <c r="B54" s="80" t="s">
-        <v>239</v>
-      </c>
-      <c r="C54" s="81"/>
-      <c r="D54" s="81"/>
-      <c r="E54" s="114"/>
-      <c r="F54" s="114"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B54" s="77" t="s">
+        <v>142</v>
+      </c>
+      <c r="C54" s="70" t="s">
+        <v>251</v>
+      </c>
+      <c r="D54" s="72"/>
+      <c r="E54" s="64"/>
+    </row>
+    <row r="55" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A55" s="74"/>
       <c r="B55" s="77" t="s">
-        <v>103</v>
-      </c>
-      <c r="C55" s="83" t="s">
-        <v>248</v>
-      </c>
-      <c r="D55" s="72" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+      <c r="C55" s="70" t="s">
+        <v>144</v>
+      </c>
+      <c r="D55" s="72"/>
+    </row>
+    <row r="56" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A56" s="74"/>
-      <c r="B56" s="77" t="s">
-        <v>341</v>
-      </c>
-      <c r="C56" s="83" t="s">
-        <v>342</v>
-      </c>
-      <c r="D56" s="72"/>
+      <c r="B56" s="66" t="s">
+        <v>238</v>
+      </c>
+      <c r="C56" s="67"/>
+      <c r="D56" s="67"/>
+      <c r="E56" s="113"/>
+      <c r="F56" s="113"/>
     </row>
     <row r="57" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="79" t="s">
-        <v>82</v>
-      </c>
+      <c r="A57" s="74"/>
       <c r="B57" s="80" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C57" s="81"/>
       <c r="D57" s="81"/>
       <c r="E57" s="114"/>
       <c r="F57" s="114"/>
     </row>
-    <row r="58" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="82"/>
-      <c r="B58" s="80" t="s">
-        <v>241</v>
-      </c>
-      <c r="C58" s="81"/>
-      <c r="D58" s="81"/>
-      <c r="E58" s="114"/>
-      <c r="F58" s="114"/>
-    </row>
-    <row r="59" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="82"/>
-      <c r="B59" s="84" t="s">
-        <v>206</v>
-      </c>
-      <c r="C59" s="86" t="s">
-        <v>216</v>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="74"/>
+      <c r="B58" s="77" t="s">
+        <v>103</v>
+      </c>
+      <c r="C58" s="83" t="s">
+        <v>248</v>
+      </c>
+      <c r="D58" s="72" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="74"/>
+      <c r="B59" s="77" t="s">
+        <v>341</v>
+      </c>
+      <c r="C59" s="83" t="s">
+        <v>342</v>
       </c>
       <c r="D59" s="72"/>
     </row>
     <row r="60" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="82"/>
-      <c r="B60" s="84" t="s">
-        <v>207</v>
-      </c>
-      <c r="C60" s="48" t="s">
-        <v>208</v>
-      </c>
-      <c r="D60" s="72" t="s">
-        <v>77</v>
-      </c>
+      <c r="A60" s="79" t="s">
+        <v>82</v>
+      </c>
+      <c r="B60" s="80" t="s">
+        <v>240</v>
+      </c>
+      <c r="C60" s="81"/>
+      <c r="D60" s="81"/>
+      <c r="E60" s="114"/>
+      <c r="F60" s="114"/>
     </row>
     <row r="61" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A61" s="82"/>
-      <c r="B61" s="84" t="s">
-        <v>169</v>
-      </c>
-      <c r="C61" s="85" t="s">
-        <v>215</v>
-      </c>
-      <c r="D61" s="72"/>
+      <c r="B61" s="80" t="s">
+        <v>241</v>
+      </c>
+      <c r="C61" s="81"/>
+      <c r="D61" s="81"/>
+      <c r="E61" s="114"/>
+      <c r="F61" s="114"/>
     </row>
     <row r="62" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A62" s="82"/>
-      <c r="B62" s="80" t="s">
-        <v>242</v>
-      </c>
-      <c r="C62" s="81"/>
-      <c r="D62" s="81"/>
-      <c r="E62" s="114"/>
-      <c r="F62" s="114"/>
+      <c r="B62" s="84" t="s">
+        <v>206</v>
+      </c>
+      <c r="C62" s="86" t="s">
+        <v>216</v>
+      </c>
+      <c r="D62" s="72"/>
     </row>
     <row r="63" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A63" s="82"/>
       <c r="B63" s="84" t="s">
-        <v>85</v>
-      </c>
-      <c r="C63" s="86" t="s">
-        <v>252</v>
+        <v>207</v>
+      </c>
+      <c r="C63" s="48" t="s">
+        <v>208</v>
       </c>
       <c r="D63" s="72" t="s">
         <v>77</v>
@@ -6114,156 +6120,152 @@
     <row r="64" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A64" s="82"/>
       <c r="B64" s="84" t="s">
-        <v>84</v>
-      </c>
-      <c r="C64" s="86" t="s">
-        <v>134</v>
-      </c>
-      <c r="D64" s="72" t="s">
-        <v>77</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="C64" s="85" t="s">
+        <v>215</v>
+      </c>
+      <c r="D64" s="72"/>
     </row>
     <row r="65" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A65" s="82"/>
-      <c r="B65" s="66" t="s">
-        <v>243</v>
-      </c>
-      <c r="C65" s="67"/>
-      <c r="D65" s="67"/>
-      <c r="E65" s="113"/>
-      <c r="F65" s="113"/>
+      <c r="B65" s="80" t="s">
+        <v>242</v>
+      </c>
+      <c r="C65" s="81"/>
+      <c r="D65" s="81"/>
+      <c r="E65" s="114"/>
+      <c r="F65" s="114"/>
     </row>
     <row r="66" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A66" s="82"/>
-      <c r="B66" s="71" t="s">
+      <c r="B66" s="84" t="s">
+        <v>85</v>
+      </c>
+      <c r="C66" s="86" t="s">
+        <v>252</v>
+      </c>
+      <c r="D66" s="72" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="82"/>
+      <c r="B67" s="84" t="s">
+        <v>84</v>
+      </c>
+      <c r="C67" s="86" t="s">
+        <v>134</v>
+      </c>
+      <c r="D67" s="72" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="82"/>
+      <c r="B68" s="66" t="s">
+        <v>243</v>
+      </c>
+      <c r="C68" s="67"/>
+      <c r="D68" s="67"/>
+      <c r="E68" s="113"/>
+      <c r="F68" s="113"/>
+    </row>
+    <row r="69" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="82"/>
+      <c r="B69" s="71" t="s">
         <v>86</v>
       </c>
-      <c r="C66" s="72" t="s">
+      <c r="C69" s="72" t="s">
         <v>135</v>
       </c>
-      <c r="D66" s="72" t="s">
+      <c r="D69" s="72" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" s="65" t="s">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" s="65" t="s">
         <v>83</v>
       </c>
-      <c r="B67" s="66" t="s">
+      <c r="B70" s="66" t="s">
         <v>244</v>
-      </c>
-      <c r="C67" s="67"/>
-      <c r="D67" s="67"/>
-      <c r="E67" s="113"/>
-      <c r="F67" s="113"/>
-    </row>
-    <row r="68" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="65"/>
-      <c r="B68" s="71" t="s">
-        <v>153</v>
-      </c>
-      <c r="C68" s="72" t="s">
-        <v>152</v>
-      </c>
-      <c r="D68" s="70"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B69" s="71" t="s">
-        <v>154</v>
-      </c>
-      <c r="C69" s="72" t="s">
-        <v>155</v>
-      </c>
-      <c r="D69" s="70"/>
-    </row>
-    <row r="70" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B70" s="66" t="s">
-        <v>245</v>
       </c>
       <c r="C70" s="67"/>
       <c r="D70" s="67"/>
-      <c r="E70" s="67"/>
-      <c r="F70" s="67"/>
+      <c r="E70" s="113"/>
+      <c r="F70" s="113"/>
     </row>
     <row r="71" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B71" s="54"/>
-      <c r="C71" s="55"/>
-      <c r="D71" s="55"/>
-      <c r="E71" s="55"/>
-      <c r="F71" s="55"/>
+      <c r="A71" s="65"/>
+      <c r="B71" s="71" t="s">
+        <v>153</v>
+      </c>
+      <c r="C71" s="72" t="s">
+        <v>152</v>
+      </c>
+      <c r="D71" s="70"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72" s="51"/>
-      <c r="B72" s="122" t="s">
-        <v>318</v>
-      </c>
-      <c r="C72" s="67"/>
-      <c r="D72" s="67"/>
-      <c r="E72" s="113"/>
-      <c r="F72" s="113"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B73" s="71" t="s">
-        <v>319</v>
-      </c>
-      <c r="C73" s="72" t="s">
-        <v>320</v>
-      </c>
-      <c r="D73" s="70"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74" s="51"/>
-      <c r="B74" s="122" t="s">
-        <v>263</v>
-      </c>
-      <c r="C74" s="67"/>
-      <c r="D74" s="67"/>
-      <c r="E74" s="113"/>
-      <c r="F74" s="113"/>
+      <c r="B72" s="71" t="s">
+        <v>154</v>
+      </c>
+      <c r="C72" s="72" t="s">
+        <v>155</v>
+      </c>
+      <c r="D72" s="70"/>
+    </row>
+    <row r="73" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B73" s="66" t="s">
+        <v>245</v>
+      </c>
+      <c r="C73" s="67"/>
+      <c r="D73" s="67"/>
+      <c r="E73" s="67"/>
+      <c r="F73" s="67"/>
+    </row>
+    <row r="74" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B74" s="54"/>
+      <c r="C74" s="55"/>
+      <c r="D74" s="55"/>
+      <c r="E74" s="55"/>
+      <c r="F74" s="55"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="51"/>
-      <c r="B75" s="123" t="s">
-        <v>259</v>
-      </c>
-      <c r="C75" s="105" t="s">
-        <v>266</v>
-      </c>
-      <c r="D75" s="55"/>
-      <c r="E75" s="64"/>
-      <c r="F75" s="64"/>
+      <c r="B75" s="122" t="s">
+        <v>318</v>
+      </c>
+      <c r="C75" s="67"/>
+      <c r="D75" s="67"/>
+      <c r="E75" s="113"/>
+      <c r="F75" s="113"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A76" s="51"/>
-      <c r="B76" s="123" t="s">
-        <v>262</v>
-      </c>
-      <c r="C76" s="105" t="s">
-        <v>267</v>
-      </c>
-      <c r="D76" s="55"/>
-      <c r="E76" s="64"/>
-      <c r="F76" s="64"/>
+      <c r="B76" s="71" t="s">
+        <v>319</v>
+      </c>
+      <c r="C76" s="72" t="s">
+        <v>320</v>
+      </c>
+      <c r="D76" s="70"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="51"/>
-      <c r="B77" s="123" t="s">
-        <v>258</v>
-      </c>
-      <c r="C77" s="105" t="s">
-        <v>268</v>
-      </c>
-      <c r="D77" s="55"/>
-      <c r="E77" s="64"/>
-      <c r="F77" s="64"/>
+      <c r="B77" s="122" t="s">
+        <v>263</v>
+      </c>
+      <c r="C77" s="67"/>
+      <c r="D77" s="67"/>
+      <c r="E77" s="113"/>
+      <c r="F77" s="113"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="51"/>
       <c r="B78" s="123" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C78" s="105" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D78" s="55"/>
       <c r="E78" s="64"/>
@@ -6272,10 +6274,10 @@
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="51"/>
       <c r="B79" s="123" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C79" s="105" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D79" s="55"/>
       <c r="E79" s="64"/>
@@ -6283,391 +6285,427 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="51"/>
-      <c r="B80" s="122" t="s">
-        <v>264</v>
-      </c>
-      <c r="C80" s="67"/>
-      <c r="D80" s="67"/>
-      <c r="E80" s="113"/>
-      <c r="F80" s="113"/>
+      <c r="B80" s="123" t="s">
+        <v>258</v>
+      </c>
+      <c r="C80" s="105" t="s">
+        <v>268</v>
+      </c>
+      <c r="D80" s="55"/>
+      <c r="E80" s="64"/>
+      <c r="F80" s="64"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="51"/>
       <c r="B81" s="123" t="s">
+        <v>260</v>
+      </c>
+      <c r="C81" s="105" t="s">
+        <v>269</v>
+      </c>
+      <c r="D81" s="55"/>
+      <c r="E81" s="64"/>
+      <c r="F81" s="64"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82" s="51"/>
+      <c r="B82" s="123" t="s">
+        <v>261</v>
+      </c>
+      <c r="C82" s="105" t="s">
+        <v>270</v>
+      </c>
+      <c r="D82" s="55"/>
+      <c r="E82" s="64"/>
+      <c r="F82" s="64"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83" s="51"/>
+      <c r="B83" s="122" t="s">
+        <v>264</v>
+      </c>
+      <c r="C83" s="67"/>
+      <c r="D83" s="67"/>
+      <c r="E83" s="113"/>
+      <c r="F83" s="113"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84" s="51"/>
+      <c r="B84" s="123" t="s">
         <v>335</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C84" t="s">
         <v>336</v>
       </c>
-      <c r="D81"/>
-      <c r="E81"/>
-      <c r="F81"/>
-    </row>
-    <row r="82" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B82" s="123" t="s">
+      <c r="D84"/>
+      <c r="E84"/>
+      <c r="F84"/>
+    </row>
+    <row r="85" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B85" s="123" t="s">
         <v>265</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C85" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="83" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B83" s="122" t="s">
+    <row r="86" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B86" s="122" t="s">
         <v>278</v>
       </c>
-      <c r="C83" s="130"/>
-      <c r="D83" s="130"/>
-      <c r="E83" s="130"/>
-      <c r="F83" s="130"/>
-    </row>
-    <row r="84" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B84" s="132" t="s">
+      <c r="C86" s="130"/>
+      <c r="D86" s="130"/>
+      <c r="E86" s="130"/>
+      <c r="F86" s="130"/>
+    </row>
+    <row r="87" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B87" s="132" t="s">
         <v>308</v>
       </c>
-      <c r="C84" s="131" t="s">
+      <c r="C87" s="131" t="s">
         <v>279</v>
       </c>
-      <c r="D84" s="131"/>
-      <c r="E84" s="131"/>
-      <c r="F84" s="131"/>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A85" s="51"/>
-      <c r="B85" s="127" t="s">
+      <c r="D87" s="131"/>
+      <c r="E87" s="131"/>
+      <c r="F87" s="131"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A88" s="51"/>
+      <c r="B88" s="127" t="s">
         <v>246</v>
       </c>
-      <c r="C85" s="129"/>
-      <c r="D85" s="129"/>
-      <c r="E85" s="129"/>
-      <c r="F85" s="129"/>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A86" s="51"/>
-      <c r="B86" s="88" t="s">
+      <c r="C88" s="129"/>
+      <c r="D88" s="129"/>
+      <c r="E88" s="129"/>
+      <c r="F88" s="129"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A89" s="51"/>
+      <c r="B89" s="88" t="s">
         <v>117</v>
       </c>
-      <c r="C86" s="89" t="s">
+      <c r="C89" s="89" t="s">
         <v>116</v>
       </c>
-      <c r="D86" s="88"/>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A87" s="51"/>
-      <c r="B87" s="88" t="s">
+      <c r="D89" s="88"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90" s="51"/>
+      <c r="B90" s="88" t="s">
         <v>309</v>
       </c>
-      <c r="C87" s="89" t="s">
+      <c r="C90" s="89" t="s">
         <v>310</v>
       </c>
-      <c r="D87" s="88"/>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A88" s="52"/>
-      <c r="B88" s="88" t="s">
+      <c r="D90" s="88"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A91" s="52"/>
+      <c r="B91" s="88" t="s">
         <v>140</v>
       </c>
-      <c r="C88" s="89" t="s">
+      <c r="C91" s="89" t="s">
         <v>141</v>
       </c>
-      <c r="D88" s="88"/>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A89" s="52"/>
-      <c r="B89" s="88" t="s">
+      <c r="D91" s="88"/>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A92" s="52"/>
+      <c r="B92" s="88" t="s">
         <v>319</v>
       </c>
-      <c r="C89" s="89" t="s">
+      <c r="C92" s="89" t="s">
         <v>321</v>
       </c>
-      <c r="D89" s="88"/>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A90" s="87"/>
-      <c r="B90" s="69" t="s">
-        <v>111</v>
-      </c>
-      <c r="C90" s="64" t="s">
-        <v>115</v>
-      </c>
-      <c r="D90" s="64"/>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A91" s="87"/>
-      <c r="B91" s="142" t="s">
-        <v>311</v>
-      </c>
-      <c r="C91" s="119"/>
-      <c r="D91" s="119"/>
-      <c r="E91" s="119"/>
-      <c r="F91" s="119"/>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A92" s="87"/>
-      <c r="B92" s="71" t="s">
-        <v>119</v>
-      </c>
-      <c r="C92" s="72" t="s">
-        <v>351</v>
-      </c>
-      <c r="D92" s="72"/>
+      <c r="D92" s="88"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="87"/>
-      <c r="B93" s="71" t="s">
-        <v>312</v>
-      </c>
-      <c r="C93" s="72" t="s">
-        <v>365</v>
-      </c>
-      <c r="D93" s="72"/>
+      <c r="B93" s="69" t="s">
+        <v>111</v>
+      </c>
+      <c r="C93" s="64" t="s">
+        <v>115</v>
+      </c>
+      <c r="D93" s="64"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" s="87"/>
-      <c r="B94" s="71" t="s">
+      <c r="B94" s="142" t="s">
+        <v>311</v>
+      </c>
+      <c r="C94" s="119"/>
+      <c r="D94" s="119"/>
+      <c r="E94" s="119"/>
+      <c r="F94" s="119"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A95" s="87"/>
+      <c r="B95" s="71" t="s">
+        <v>119</v>
+      </c>
+      <c r="C95" s="72" t="s">
+        <v>351</v>
+      </c>
+      <c r="D95" s="72"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A96" s="87"/>
+      <c r="B96" s="71" t="s">
+        <v>312</v>
+      </c>
+      <c r="C96" s="72" t="s">
+        <v>365</v>
+      </c>
+      <c r="D96" s="72"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A97" s="87"/>
+      <c r="B97" s="71" t="s">
         <v>313</v>
       </c>
-      <c r="C94" s="72" t="s">
+      <c r="C97" s="72" t="s">
         <v>364</v>
       </c>
-      <c r="D94" s="72"/>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A95" s="119" t="s">
+      <c r="D97" s="72"/>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A98" s="119" t="s">
         <v>247</v>
       </c>
-      <c r="B95" s="142" t="s">
+      <c r="B98" s="142" t="s">
         <v>314</v>
       </c>
-      <c r="C95" s="119"/>
-      <c r="D95" s="119"/>
-      <c r="E95" s="119"/>
-      <c r="F95" s="119"/>
-    </row>
-    <row r="96" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="90"/>
-      <c r="B96" s="71" t="s">
+      <c r="C98" s="119"/>
+      <c r="D98" s="119"/>
+      <c r="E98" s="119"/>
+      <c r="F98" s="119"/>
+    </row>
+    <row r="99" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="90"/>
+      <c r="B99" s="71" t="s">
         <v>38</v>
       </c>
-      <c r="C96" s="72" t="s">
+      <c r="C99" s="72" t="s">
         <v>162</v>
       </c>
-      <c r="D96" s="72"/>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A97" s="119" t="s">
+      <c r="D99" s="72"/>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A100" s="119" t="s">
         <v>254</v>
       </c>
-      <c r="B97" s="71" t="s">
+      <c r="B100" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="C97" s="72" t="s">
+      <c r="C100" s="72" t="s">
         <v>157</v>
       </c>
-      <c r="D97" s="72"/>
-    </row>
-    <row r="98" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="90"/>
-      <c r="B98" s="71" t="s">
+      <c r="D100" s="72"/>
+    </row>
+    <row r="101" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="90"/>
+      <c r="B101" s="71" t="s">
         <v>199</v>
       </c>
-      <c r="C98" s="110" t="s">
+      <c r="C101" s="110" t="s">
         <v>200</v>
       </c>
-      <c r="D98" s="72"/>
-    </row>
-    <row r="99" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="91"/>
-      <c r="B99" s="71" t="s">
-        <v>202</v>
-      </c>
-      <c r="C99" s="110" t="s">
-        <v>203</v>
-      </c>
-      <c r="D99" s="72"/>
-    </row>
-    <row r="100" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="91"/>
-      <c r="B100" s="71" t="s">
-        <v>316</v>
-      </c>
-      <c r="C100" s="110" t="s">
-        <v>315</v>
-      </c>
-      <c r="D100" s="72"/>
-    </row>
-    <row r="101" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="91"/>
-      <c r="B101" s="142" t="s">
-        <v>317</v>
-      </c>
-      <c r="C101" s="119"/>
-      <c r="D101" s="119"/>
-      <c r="E101" s="119"/>
-      <c r="F101" s="119"/>
+      <c r="D101" s="72"/>
     </row>
     <row r="102" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A102" s="91"/>
-      <c r="B102" s="75" t="s">
+      <c r="B102" s="71" t="s">
+        <v>202</v>
+      </c>
+      <c r="C102" s="110" t="s">
+        <v>203</v>
+      </c>
+      <c r="D102" s="72"/>
+    </row>
+    <row r="103" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A103" s="91"/>
+      <c r="B103" s="71" t="s">
+        <v>316</v>
+      </c>
+      <c r="C103" s="110" t="s">
+        <v>315</v>
+      </c>
+      <c r="D103" s="72"/>
+    </row>
+    <row r="104" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="91"/>
+      <c r="B104" s="142" t="s">
+        <v>317</v>
+      </c>
+      <c r="C104" s="119"/>
+      <c r="D104" s="119"/>
+      <c r="E104" s="119"/>
+      <c r="F104" s="119"/>
+    </row>
+    <row r="105" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="91"/>
+      <c r="B105" s="75" t="s">
         <v>256</v>
-      </c>
-      <c r="C102" s="93"/>
-      <c r="D102" s="93"/>
-      <c r="E102" s="93"/>
-      <c r="F102" s="93"/>
-    </row>
-    <row r="103" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="119" t="s">
-        <v>255</v>
-      </c>
-      <c r="B103" s="84" t="s">
-        <v>90</v>
-      </c>
-      <c r="C103" s="72" t="s">
-        <v>159</v>
-      </c>
-      <c r="D103" s="72"/>
-    </row>
-    <row r="104" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="92"/>
-      <c r="B104" s="84" t="s">
-        <v>89</v>
-      </c>
-      <c r="C104" s="72" t="s">
-        <v>160</v>
-      </c>
-      <c r="D104" s="72"/>
-    </row>
-    <row r="105" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="94"/>
-      <c r="B105" s="75" t="s">
-        <v>257</v>
       </c>
       <c r="C105" s="93"/>
       <c r="D105" s="93"/>
       <c r="E105" s="93"/>
       <c r="F105" s="93"/>
     </row>
-    <row r="106" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="94"/>
-      <c r="B106" s="118" t="s">
-        <v>137</v>
+    <row r="106" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="119" t="s">
+        <v>255</v>
+      </c>
+      <c r="B106" s="84" t="s">
+        <v>90</v>
       </c>
       <c r="C106" s="72" t="s">
-        <v>138</v>
+        <v>159</v>
       </c>
       <c r="D106" s="72"/>
     </row>
     <row r="107" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A107" s="92"/>
-      <c r="B107" s="118" t="s">
-        <v>137</v>
+      <c r="B107" s="84" t="s">
+        <v>89</v>
       </c>
       <c r="C107" s="72" t="s">
-        <v>363</v>
+        <v>160</v>
       </c>
       <c r="D107" s="72"/>
     </row>
     <row r="108" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A108" s="94"/>
-      <c r="B108" s="118" t="s">
+      <c r="B108" s="75" t="s">
+        <v>257</v>
+      </c>
+      <c r="C108" s="93"/>
+      <c r="D108" s="93"/>
+      <c r="E108" s="93"/>
+      <c r="F108" s="93"/>
+    </row>
+    <row r="109" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="94"/>
+      <c r="B109" s="118" t="s">
+        <v>137</v>
+      </c>
+      <c r="C109" s="72" t="s">
+        <v>138</v>
+      </c>
+      <c r="D109" s="72"/>
+    </row>
+    <row r="110" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="92"/>
+      <c r="B110" s="118" t="s">
+        <v>137</v>
+      </c>
+      <c r="C110" s="72" t="s">
+        <v>363</v>
+      </c>
+      <c r="D110" s="72"/>
+    </row>
+    <row r="111" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="94"/>
+      <c r="B111" s="118" t="s">
         <v>191</v>
       </c>
-      <c r="C108" s="72" t="s">
+      <c r="C111" s="72" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="109" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B111" s="106" t="s">
+    <row r="112" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.2"/>
+    <row r="114" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B114" s="106" t="s">
         <v>192</v>
       </c>
-      <c r="C111" s="106" t="s">
+      <c r="C114" s="106" t="s">
         <v>196</v>
       </c>
-      <c r="D111" s="149" t="s">
+      <c r="D114" s="149" t="s">
         <v>197</v>
       </c>
-      <c r="E111" s="149"/>
-      <c r="F111" s="149"/>
-    </row>
-    <row r="112" spans="1:6" ht="127.5" x14ac:dyDescent="0.2">
-      <c r="B112" s="109" t="s">
+      <c r="E114" s="149"/>
+      <c r="F114" s="149"/>
+    </row>
+    <row r="115" spans="2:6" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="B115" s="109" t="s">
         <v>193</v>
       </c>
-      <c r="C112" s="108" t="s">
+      <c r="C115" s="108" t="s">
         <v>205</v>
       </c>
-      <c r="D112" s="150" t="s">
+      <c r="D115" s="150" t="s">
         <v>198</v>
       </c>
-      <c r="E112" s="150"/>
-      <c r="F112" s="150"/>
-    </row>
-    <row r="113" spans="2:6" ht="102" x14ac:dyDescent="0.2">
-      <c r="B113" s="109" t="s">
+      <c r="E115" s="150"/>
+      <c r="F115" s="150"/>
+    </row>
+    <row r="116" spans="2:6" ht="102" x14ac:dyDescent="0.2">
+      <c r="B116" s="109" t="s">
         <v>194</v>
       </c>
-      <c r="C113" s="115" t="s">
+      <c r="C116" s="115" t="s">
         <v>204</v>
       </c>
-      <c r="D113" s="150" t="s">
+      <c r="D116" s="150" t="s">
         <v>201</v>
       </c>
-      <c r="E113" s="150"/>
-      <c r="F113" s="150"/>
-    </row>
-    <row r="114" spans="2:6" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="B114" s="109" t="s">
+      <c r="E116" s="150"/>
+      <c r="F116" s="150"/>
+    </row>
+    <row r="117" spans="2:6" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="B117" s="109" t="s">
         <v>195</v>
       </c>
-      <c r="C114" s="108" t="s">
+      <c r="C117" s="108" t="s">
         <v>209</v>
       </c>
-      <c r="D114" s="150" t="s">
+      <c r="D117" s="150" t="s">
         <v>210</v>
       </c>
-      <c r="E114" s="150"/>
-      <c r="F114" s="150"/>
-    </row>
-    <row r="115" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B115" s="117"/>
-    </row>
-    <row r="116" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B116" s="116" t="s">
+      <c r="E117" s="150"/>
+      <c r="F117" s="150"/>
+    </row>
+    <row r="118" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B118" s="117"/>
+    </row>
+    <row r="119" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B119" s="116" t="s">
         <v>218</v>
       </c>
-      <c r="C116" s="116" t="s">
+      <c r="C119" s="116" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="117" spans="2:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="B117" s="117" t="s">
+    <row r="120" spans="2:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="B120" s="117" t="s">
         <v>219</v>
       </c>
-      <c r="C117" s="108" t="s">
+      <c r="C120" s="108" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="118" spans="2:6" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="B118" s="117" t="s">
+    <row r="121" spans="2:6" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="B121" s="117" t="s">
         <v>220</v>
       </c>
-      <c r="C118" s="108" t="s">
+      <c r="C121" s="108" t="s">
         <v>222</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
+    <mergeCell ref="D117:F117"/>
+    <mergeCell ref="D116:F116"/>
+    <mergeCell ref="D115:F115"/>
     <mergeCell ref="D114:F114"/>
-    <mergeCell ref="D113:F113"/>
-    <mergeCell ref="D112:F112"/>
-    <mergeCell ref="D111:F111"/>
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D112" r:id="rId1"/>
-    <hyperlink ref="D113" r:id="rId2"/>
-    <hyperlink ref="D114" r:id="rId3"/>
+    <hyperlink ref="D115" r:id="rId1"/>
+    <hyperlink ref="D116" r:id="rId2"/>
+    <hyperlink ref="D117" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>

</xml_diff>